<commit_message>
Day 11 | DA18
</commit_message>
<xml_diff>
--- a/Batch/18/Day_8.xlsx
+++ b/Batch/18/Day_8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\18\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C3500D-CD8E-4C4B-95A9-B17BE8B50CEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B71FD8-059C-4D6E-9A63-3E882E876EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" tabRatio="741" activeTab="9" xr2:uid="{E4FAC7A2-194B-4DBE-ACA1-546198A701A9}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" tabRatio="741" activeTab="1" xr2:uid="{E4FAC7A2-194B-4DBE-ACA1-546198A701A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors" sheetId="7" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4407" uniqueCount="897">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4407" uniqueCount="901">
   <si>
     <t>Intro To excel</t>
   </si>
@@ -15398,9 +15398,6 @@
     <t>Mid</t>
   </si>
   <si>
-    <t>Proper</t>
-  </si>
-  <si>
     <t>Find</t>
   </si>
   <si>
@@ -15589,6 +15586,21 @@
   </si>
   <si>
     <t>EOMONTH</t>
+  </si>
+  <si>
+    <t>What’s the difference between a blank cell and a cell with ""?</t>
+  </si>
+  <si>
+    <t>True Zero</t>
+  </si>
+  <si>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>Excel's Internal Data Type = IEEE 754 Floating Point</t>
+  </si>
+  <si>
+    <t>Why Excel’s Maximum Date is 31-Dec-9999 = Serial 2,958,465</t>
   </si>
 </sst>
 </file>
@@ -15633,7 +15645,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -15643,6 +15655,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -15660,7 +15684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -15684,6 +15708,14 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -15720,7 +15752,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>169528</xdr:colOff>
+      <xdr:colOff>94331</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>161107</xdr:rowOff>
     </xdr:to>
@@ -15768,8 +15800,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>57912</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="50" name="Ink 49">
@@ -15788,7 +15820,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="50" name="Ink 49">
@@ -15833,8 +15865,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>17232</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="57" name="Ink 56">
@@ -15853,7 +15885,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="57" name="Ink 56">
@@ -15898,8 +15930,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>132079</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="71" name="Ink 70">
@@ -15918,7 +15950,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="71" name="Ink 70">
@@ -15963,8 +15995,8 @@
       <xdr:row>29</xdr:row>
       <xdr:rowOff>140752</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="84" name="Ink 83">
@@ -15983,7 +16015,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="84" name="Ink 83">
@@ -16028,8 +16060,8 @@
       <xdr:row>26</xdr:row>
       <xdr:rowOff>143754</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="85" name="Ink 84">
@@ -16048,7 +16080,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="85" name="Ink 84">
@@ -16089,12 +16121,12 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>778429</xdr:colOff>
+      <xdr:colOff>783191</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>17558</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="86" name="Ink 85">
@@ -16113,7 +16145,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="86" name="Ink 85">
@@ -16158,8 +16190,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>27638</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="88" name="Ink 87">
@@ -16178,7 +16210,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="88" name="Ink 87">
@@ -16210,6 +16242,375 @@
     </mc:AlternateContent>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>95327</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>11735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>485152</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>64705</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="70" name="Ink 69">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DDC7D1A-A7D2-0E6F-E2C8-37483EEA2849}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6401880" y="372682"/>
+            <a:ext cx="1036522" cy="413918"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="70" name="Ink 69">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DDC7D1A-A7D2-0E6F-E2C8-37483EEA2849}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6395732" y="366558"/>
+              <a:ext cx="1048818" cy="426166"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>264750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>69859</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>550312</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>160547</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="72" name="Ink 71">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DE0FD8F-09E0-F709-E1A0-56F8C93F7FDE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7218000" y="611280"/>
+            <a:ext cx="280800" cy="266400"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="72" name="Ink 71">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DE0FD8F-09E0-F709-E1A0-56F8C93F7FDE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7211880" y="605160"/>
+              <a:ext cx="293040" cy="278640"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>220693</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>435777</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>75606</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="110" name="Ink 109">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{658163C0-2ACF-AA4F-BF42-268295CFF84E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7820640" y="1189162"/>
+            <a:ext cx="210322" cy="144998"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="110" name="Ink 109">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{658163C0-2ACF-AA4F-BF42-268295CFF84E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7814528" y="1183061"/>
+              <a:ext cx="222546" cy="157201"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>562830</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>27575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>151795</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>68469</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="123" name="Ink 122">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D9F8EC0-89AA-D058-5466-21AF9471E4E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7516080" y="388522"/>
+            <a:ext cx="882360" cy="397080"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="123" name="Ink 122">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D9F8EC0-89AA-D058-5466-21AF9471E4E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7509958" y="382396"/>
+              <a:ext cx="894605" cy="409331"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>78047</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>96107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>382997</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>160566</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="128" name="Ink 127">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E93B8FFE-0454-CEF8-92A3-45960990C869}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6384600" y="818002"/>
+            <a:ext cx="2245042" cy="605880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="128" name="Ink 127">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E93B8FFE-0454-CEF8-92A3-45960990C869}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6378479" y="811882"/>
+              <a:ext cx="2257284" cy="618120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>10027</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>160421</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>429850</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>132896</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="129" name="Picture 128">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9DFEDDE-283D-1285-078B-E3E1349B0DD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2275974" y="3228474"/>
+          <a:ext cx="5182323" cy="333422"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -16228,8 +16629,8 @@
       <xdr:row>3</xdr:row>
       <xdr:rowOff>74201</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="11" name="Ink 10">
@@ -16248,7 +16649,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="11" name="Ink 10">
@@ -16293,8 +16694,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>57076</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="18" name="Ink 17">
@@ -16313,7 +16714,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="18" name="Ink 17">
@@ -16358,8 +16759,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>178839</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="33" name="Ink 32">
@@ -16378,7 +16779,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="33" name="Ink 32">
@@ -16423,8 +16824,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>74716</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="34" name="Ink 33">
@@ -16443,7 +16844,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="34" name="Ink 33">
@@ -16488,8 +16889,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>36516</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="37" name="Ink 36">
@@ -16508,7 +16909,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="37" name="Ink 36">
@@ -16553,8 +16954,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>104040</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="38" name="Ink 37">
@@ -16573,7 +16974,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="38" name="Ink 37">
@@ -16618,8 +17019,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>16716</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="41" name="Ink 40">
@@ -16638,7 +17039,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="41" name="Ink 40">
@@ -16683,8 +17084,8 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>95515</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="49" name="Ink 48">
@@ -16703,7 +17104,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="49" name="Ink 48">
@@ -16748,8 +17149,8 @@
       <xdr:row>12</xdr:row>
       <xdr:rowOff>7511</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="71" name="Ink 70">
@@ -16768,7 +17169,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="71" name="Ink 70">
@@ -16813,8 +17214,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>29749</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="90" name="Ink 89">
@@ -16833,7 +17234,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="90" name="Ink 89">
@@ -16878,8 +17279,8 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>17558</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="91" name="Ink 90">
@@ -16898,7 +17299,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="91" name="Ink 90">
@@ -16943,8 +17344,8 @@
       <xdr:row>37</xdr:row>
       <xdr:rowOff>27638</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="92" name="Ink 91">
@@ -16963,7 +17364,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="92" name="Ink 91">
@@ -17101,8 +17502,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>74495</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="11" name="Ink 10">
@@ -17121,7 +17522,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="11" name="Ink 10">
@@ -17166,8 +17567,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>68166</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="22" name="Ink 21">
@@ -17186,7 +17587,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="22" name="Ink 21">
@@ -17270,6 +17671,199 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-24T12:54:40.776"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">202 55 1617,'0'0'6328,"15"-15"-6269,15-15 5514,-28 21 618,-4 20-4984,0 34-1186,-3-1 0,-1 0 0,-3 0 0,-20 63 0,23-86-19,2 3-11,3-19-61,0 1 1,0-1 0,0 1 0,-1-1-1,0 0 1,0 1 0,-4 7 0,5-12-536,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-3-1 0,0 1-1073,-8-2-3148</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="278.78">0 246 7091,'0'0'9012,"1"0"-8962,-1-1 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0-1 0,-1 1 0,1 1-1,1-1 1,239 0 3142,-160 0-4640,0 0-3425,-68-2 652,0-6-920</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="558.74">555 42 8708,'0'0'10594,"0"-5"-9775,2-15-455,3 35-178,4 44 41,-7-26-94,9 202 110,-11-234-320,0 1-233,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,-1 0 1,1-1-1,0 1 0,-1 0 0,0 0 1,1-1-1,-1 1 0,0 0 0,0-1 0,0 1 1,0-1-1,-2 3 0,-15 4-7958</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-24T12:54:43.004"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">169 143 9636,'0'0'8039,"0"0"-7995,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1-1,-9 39-48,-2-1 0,-1 0-1,-2-1 1,-24 45 0,14-30 22,-18 57 0,40-103-1,2-5-12,0 1 0,0-1 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,-1 1 0,1-1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,0-1 0,1 1 1,-1 0-1,0 0 0,-1 1 0,1-1 122,1-15 138,0 6-253,1 0 1,1 0-1,-1 1 1,1-1 0,1 0-1,-1 0 1,1 1-1,1 0 1,6-12-1,48-65 73,-26 39-67,-21 29-19,-6 6-4,1 0 1,1 1-1,0 0 0,0 0 0,1 0 1,0 1-1,0 0 0,13-8 1,-21 15-6,1 1 0,0 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 0,0 1 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 1 1,0-1-1,0 0 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 1,-1 1-1,1 0 0,-1-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1-1 0,-1 1 1,0 0-1,0 1 0,11 43 84,-8-32-96,7 38 85,-1 0 0,2 65 0,-9-21-8569,-2-89 2051</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="190.35">83 537 10805,'0'0'6467,"115"-45"-6323,-50 33 0,1 5-96,0 0-48,-9 5-96,-12 0-1713,-12-3-2817</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="745.04">584 249 12406,'0'0'4242,"-1"12"-4176,-6 203 972,7-214-643,1-14 341,0 7-699,1 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,6-4 0,13-7-305,0 1 1,33-13 0,-35 17-112,-6 2 149,-6 3 57,-1 0 1,1-1-1,-1 0 0,14-10 0,-21 13 194,1 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0-1,0 0 1,1-5 0,-14 155 2090,13-135-2505,1 41 1245,7-30-2510,-7-22 1388,-1-1 0,1 1 0,-1 0 0,1 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0-1,9 1-6248</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1586.21">1093 276 9604,'0'0'9720,"0"-6"-9307,2-15-351,0 18-127,-2 18 28,1 22 108,0-19-16,-1-1-1,0 0 1,-1 1 0,-7 33-1,8-51-33,0 0-1,0 0 1,-1-1-1,1 1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,-3-15 273,1-22-251,2 23-24,3-60 31,-2 71-46,-1-1-1,1 1 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,1-1 0,-1 1 1,1 0-1,0 1 1,0-1-1,0 0 1,0 0-1,1 1 1,-1-1-1,6-3 1,-4 4-15,0 1-1,1-1 1,-1 1 0,1 0 0,-1 0-1,0 0 1,1 1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 1-1,1-1 1,-1 1 0,1 0-1,-1 1 1,0-1 0,0 1 0,5 2-1,-3-1 11,1 0 0,-1 1 0,1 0 0,-1 0-1,0 0 1,-1 1 0,1 0 0,-1 0 0,0 0 0,8 11-1,-9-8 17,-1 0 0,0 0 0,-1 1-1,0-1 1,0 1 0,-1-1 0,0 1-1,0-1 1,-1 1 0,-1 16 0,0-4 77,1-20 101,5-27 86,-2 13-274,2 1 0,-1 0 0,2 0 0,0 0 0,0 1 0,1 0 0,0 0 0,1 1 0,1-1-1,-1 2 1,13-11 0,-16 14-26,1 1-1,0 0 0,1 0 0,-1 0 0,1 1 1,0 0-1,0 1 0,0-1 0,1 1 1,-1 1-1,1-1 0,-1 1 0,1 1 0,0-1 1,0 1-1,0 1 0,0-1 0,0 1 0,12 2 1,-17-1 14,-1 1 0,1-1 1,0 1-1,-1-1 1,1 1-1,-1 0 0,0 0 1,1 0-1,-1 1 1,0-1-1,0 0 0,-1 1 1,1 0-1,0-1 1,-1 1-1,1 0 0,-1 0 1,0-1-1,0 1 1,0 0-1,-1 0 0,1 0 1,-1 1-1,1 2 1,2 14-6,-1 0 0,-1 26 0,-1-44 15,0 0-2,0 10 2,0 0 0,0 0 0,-1 0-1,-1 0 1,0 0 0,-5 16 0,6-27-135,1 0 0,-1 1 0,1-1-1,-1 0 1,1 1 0,0-1 0,0 0 0,-1 1-1,1-1 1,0 1 0,0-1 0,1 0 0,-1 1-1,0-1 1,0 1 0,1-1 0,-1 0-1,0 1 1,1-1 0,0 0 0,-1 0 0,1 1-1,0-1 1,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,1 0-1,-1-1 1,0 1 0,0 0 0,0-1 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 1 0,0-1-1,1 0 1,-1 0 0,1 0 0,-1 0 0,2 0-1,11 1-1581,0-1 0,-1 0 0,26-5 0,-32 5 909,38-10-3524</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2388.11">1905 370 4178,'0'0'3380,"10"-15"-1342,32-49 177,-40 62-2015,0 0 0,-1 0 0,1 0 0,-1-1 1,1 1-1,-1-1 0,0 1 0,0-1 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 0,-1 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,-1 1 0,1-1 1,-1 0-1,0 0 0,0-2 0,-1 3-145,0 1-1,0-1 1,0 0-1,0 1 1,0-1 0,0 1-1,-1 0 1,1 0-1,0 0 1,-1 0 0,1 0-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1 0 1,1 0 0,-1 0-1,-3 0 1,-5 0-6,1 0 0,-1 1 1,0 1-1,0-1 0,1 2 0,-1-1 1,1 1-1,0 1 0,-14 6 0,18-6-29,0-1 0,1 1-1,-1 0 1,1 1 0,0-1 0,0 1-1,1 0 1,-1 0 0,1 1-1,0-1 1,0 1 0,1 0-1,0 0 1,0 0 0,0 1-1,-2 8 1,4-14-15,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1-1,-1 1 1,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,1-1-1,-1 1 1,1 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,3 0 0,2 0 12,0 1 0,-1-2 0,1 1 0,0-1 1,0 0-1,0 0 0,-1 0 0,1-1 0,0 0 0,0 0 0,5-2 0,-3 0 6,0-1 0,0 0 0,-1-1 0,1 0-1,-1 0 1,0 0 0,-1-1 0,1 0-1,-1 0 1,0-1 0,-1 0 0,10-14 0,-16 25-8,0 0 1,1 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,1 1 0,-1-1-1,1 0 1,0 0 0,0 0-1,0 0 1,1 0 0,0 0-1,-1 0 1,1 0 0,0-1-1,1 1 1,-1-1-1,1 1 1,4 3 0,-1-2-64,1-1 1,-1 0-1,1 0 1,0-1-1,0 0 0,1 0 1,-1-1-1,1 0 1,-1 0-1,15 1 1,82 0-1703,-72-3 1059,-25 0 545,-1 0 0,0-1-1,0 1 1,0-1 0,0-1 0,1 1 0,-2-1 0,1 0 0,0 0 0,11-6 0,-15 6 107,0 1 0,1-1 1,-1 0-1,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,-1 1 1,1-1-1,-1 0 0,0 1 1,1-1-1,-1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,-1-5 0,1 6 77,-1 0 0,0-1-1,1 1 1,-1 0 0,0 0-1,0 0 1,0-1 0,0 1-1,-1 0 1,1 1 0,-1-1-1,1 0 1,-1 0 0,0 1-1,1-1 1,-1 0 0,0 1-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,-1 1 1,1-1 0,0 0 0,-1 1-1,-2-1 1,-10-1 399,1 0 1,-1 1-1,-21 1 0,22 0-267,8 0-132,1 1 1,-1-1-1,0 1 0,1 0 0,-1 1 0,1-1 1,-11 5-1,14-5-34,0 0 0,0 0 1,0 0-1,0 0 0,1 1 0,-1-1 0,0 0 1,1 1-1,-1-1 0,1 1 0,-1-1 0,1 1 1,0 0-1,0 0 0,0-1 0,0 1 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,1 0 1,-1 0-1,1 4 0,0-5-1,1 0 0,-1-1-1,0 1 1,1 0 0,-1-1 0,1 1 0,0 0-1,-1-1 1,1 1 0,-1-1 0,1 1-1,0-1 1,-1 1 0,1-1 0,0 1-1,0-1 1,-1 0 0,1 0 0,0 1 0,0-1-1,0 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0-1,1 0 1,32-2 114,-31 2-112,10-3 17,-1 0 0,1-1 1,-1 0-1,0 0 0,0-2 0,0 1 0,0-2 0,-1 1 0,0-2 0,-1 1 1,15-14-1,-3 1 3,-1-2 0,-1 0 1,-1 0-1,17-27 0,-24 30 338,-1 0-1,-1-1 0,0-1 1,12-39-1,-23 122 38,2-12-419,-3 38-62,-10 127-124,9-191-955,-1 0-1,-1-1 0,-1 1 0,-2-1 0,0-1 0,-19 38 1,-16 9-8365</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3422.59">268 829 4274,'0'0'3498,"-9"0"-2090,0 1-853,-6 0 94,-2-1 3173,11 9-23,6-8-3772,0-1 1,0 0 0,0 0 0,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 1 0,0-1 0,1 0 0,-1 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 1 0,0-1 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,1 0 0,115-7-75,28 0-109,-150 47 1,-25 33 579,21-54-358,1 2 0,1-1 0,-7 29 0,14-44-111,-2 8-1300,5-6-2304</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4199.58">781 940 5090,'0'0'9060,"0"-1"-8980,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,0 0 0,1 1 0,-1-1-1,0 0 1,-1-1 0,-1 2 4,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 1,-1 1-1,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 1,0 0-1,-5 3 0,7-3-68,0-1 1,-1 1-1,1-1 1,0 1-1,0 0 1,0-1-1,0 1 1,1 0-1,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1-1-1,0 1 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,0 0 1,-1 0-1,1 0 1,2 3-1,-2-3-8,1 0-1,-1 1 0,1-1 0,0 0 0,0-1 1,0 1-1,0 0 0,1-1 0,-1 1 0,0-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,0-1 0,0 1 0,3-1 1,64 3 58,-55-3-62,-13 0 1,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 1,-1-1-1,1 1 0,-1-1 0,0 0 0,1 1 0,0-4 0,0 0 11,0-1 1,0 0-1,-1 1 1,0-1 0,0 0-1,0 0 1,-1 0-1,0-7 1,-2 6-20,1 0 1,-1 0-1,0 0 1,0 0-1,-1 0 1,0 1-1,0-1 1,-1 1-1,0 0 1,0 0-1,-8-9 1,6 7 5,0 0-1,0-1 1,1 1 0,1-1 0,-6-13 0,10 21-18,0 1 1,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0 0-1,0-1 1,1 1 0,-1-1-1,0 1 1,0 0 0,0-1-1,0 1 1,1 0 0,-1 0-1,0-1 1,1 1-1,-1 0 1,0-1 0,0 1-1,1 0 1,-1 0 0,0 0-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,24-5-267,40 5 69,-48 1 132,13-2 51,-16 0 17,0 1 0,1 0 0,-1 1 0,0 1 0,0 0 1,22 6-1,-35-7 18,0-1-1,0 0 1,-1 0 0,1 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1-1,0-1 1,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0-1,1 0 1,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,-1 1 0,-41 35 340,40-34-330,-7 5-463,-29 22 1363,24-10-2805,9 1-4451</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4669.54">1355 768 10197,'0'0'6472,"-4"-12"-6018,-16-35-84,19 46-364,0-1 0,0 1 0,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 1-1,-1-1 1,0 0 0,1 1 0,-1 0-1,0-1 1,1 1 0,-1 0-1,0 0 1,0 0 0,1 0 0,-4 0-1,-32 7 32,31-5-38,0 0-1,0 1 0,0 0 1,0 0-1,1 0 1,-1 1-1,1 0 0,0 0 1,0 0-1,1 1 1,-1-1-1,1 1 1,0 0-1,0 0 0,1 1 1,-1-1-1,1 1 1,0 0-1,1 0 0,0 0 1,0 0-1,0 0 1,0 1-1,1-1 1,0 0-1,0 10 0,1-15-18,1-1 0,-1 1 0,1 0 0,-1-1-1,1 1 1,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 1-1,1-1 1,-1 0 0,1 0 0,0 1 0,-1-1-1,1 0 1,0 0 0,-1 1 0,1-1 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1-1 0,0 1 0,-1 0 0,1 0-1,0-1 1,-1 1 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1-1 0,0 0 0,29-14 128,-18 3-110,0-1-1,-1 0 0,12-20 1,-21 32 31,-1 25-192,-3 2 281,-1-1-1,-10 41 1,2-7 2,7-30-3103</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6532.43">1639 790 5090,'0'0'9805,"0"-19"-6756,-8 213-4655,8-194 1414,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0-1,1 0 1,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,2-1 0,23-9-1780,-13 0 1864,-1 0 0,0-1 0,-1 0 0,0 0 1,11-19-1,-16 23 506,0-1 0,-1 1 0,0-1 0,0 0 0,-1 0 0,3-9 0,-15 22 6560,5-1-6915,0 1 0,0-1 0,0 1 0,0 0 0,1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,-2 10 0,5-14-35,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 1,1 1-1,-1-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,3 0 0,0 0 14,1-1 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1-1-1,1 0 1,6-1 0,-6 1-12,-4 0 7,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0-3 0,1-2 98,0-1 1,-1 0-1,0 1 0,-1-1 0,-1-10 1,2 16-126,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,0 0-1,0 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,0 1-1,-1-1 1,1 0-1,-2 0 1,0 1-357,1-1 1,-1 0-1,0 1 1,1-1-1,-1 1 1,0 0-1,1 0 1,-1 0-1,1 0 1,0 1-1,-1-1 1,1 1-1,-3 2 1,-4 8-4467</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6812.88">2197 823 11989,'0'0'6790,"-2"3"-6792,-5 9-29,-42 80 359,45-82-405,0 1 0,0-1-1,1 1 1,0 0 0,1 0 0,0 0 0,0 15-1,2-18-534,0-8 416,-1 1 0,1 0 1,0-1-1,0 1 1,0 0-1,-1-1 0,1 1 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,1-1-1,-1 1 1,0 0-1,0-1 0,0 1 1,1 0-1,-1-1 1,0 1-1,1 0 0,-1-1 1,0 1-1,1-1 1,-1 1-1,1-1 0,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 1-1,1-1 1,0 0-1,-1 1 0,1-1 1,0 0-1,-1 0 1,1 0-1,1 1 0,14-1-5158</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7002.45">2300 872 7684,'0'0'8435,"4"28"-8323,4-2-112,-4 0 80,4 4-80,-3 1-48,-5 4-720,0-7-1761,0-2-3346</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink12.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-24T12:54:19.252"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">21 1028 11861,'0'0'3997,"4"5"-4002,0 4 29,0-1 0,0 1 0,0 0 1,-1 0-1,-1 0 0,0 0 1,0 0-1,-1 1 0,0-1 1,0 0-1,-1 1 0,0-1 0,-3 19 1,0-10 26,0 0 1,-1-1-1,0 0 1,-2 0-1,0 0 1,-1 0-1,-9 15 1,18-64 3558,1-11-3864,3 26 238,0-1 1,2 2-1,16-29 0,-20 38-28,1 0 0,0 0 0,0 0 0,1 0 0,0 1 0,0 0 0,0 0 0,1 1 0,0-1 0,9-4 0,-14 9 39,0 0-1,-1 0 1,1 0 0,0 0-1,0 1 1,-1-1-1,1 1 1,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,0 1-1,0-1 1,0 1-1,0-1 1,0 1 0,2 1-1,-2 0 1,0-1 0,0 1 1,0 0-1,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0 3 0,2 11 4,0 0 0,-2 0 1,0 0-1,-2 18 0,1-20 23,0 28 88,0-43 194,1-12-305,1 1 0,1-1 0,-1 1 0,2 0 0,0 0 0,0 0 0,1 0 0,0 0 1,0 1-1,2 0 0,-1 0 0,1 1 0,0 0 0,1 0 0,0 0 0,13-9 0,-20 17-6,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 0,0 1 1,0-1-1,-1 0 1,1 0-1,0 1 0,0-1 1,0 1-1,0 0 1,0-1-1,0 1 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 1 1,0-1-1,0 1 0,-1 0 1,1 0-1,2 1 1,-2 0-3,0 0 0,0 0 1,-1 1-1,1-1 1,0 0-1,-1 1 0,0 0 1,0-1-1,1 1 1,-1 0-1,-1-1 0,1 1 1,0 0-1,-1 0 1,0 0-1,1 0 0,-1 0 1,-1 3-1,-3 204 327,6-210-305,-1-1 1,1 1-1,-1 0 1,1-1-1,-1 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,1-1 1,13-15-110,-1 0 1,-1 0 0,-1-1-1,-1-1 1,0 0-1,-1 0 1,10-32 0,-12 33-56,-6 26-86,-12 31-80,7-34 317,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,1 0 0,-1 1 0,1-1 0,0 1 0,0 0 0,1-1 0,0 11 0,1-15-3,1 0 0,0 0 0,0 0-1,0 0 1,1-1 0,-1 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0-1 0,2 1-1,4-1-44,-4 2-191,0-1-1,0 0 1,0 0-1,0-1 0,0 1 1,1-1-1,-1 0 1,0 0-1,0 0 1,-1 0-1,1-1 0,0 0 1,0 0-1,-1 0 1,1 0-1,-1 0 1,1-1-1,-1 1 0,4-5 1,11-20-5975</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="189.44">637 974 9925,'0'0'5458,"41"30"-5458,-25-6-400,5-3-1841,-5 2-1169,5-4-608</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="653.76">891 1131 5891,'0'0'10495,"-9"-7"-10071,4 4-408,3 0 11,0 1 0,-1 0 0,0 0 0,1-1 0,-1 2 1,0-1-1,0 0 0,0 1 0,-1-1 0,1 1 1,0 0-1,0 0 0,-1 0 0,1 1 0,0-1 0,-1 1 1,1-1-1,-1 1 0,1 0 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 0,0 0 0,-1 0 1,-4 3-1,2-1-9,1 1-1,0-1 1,0 1 0,0 1 0,0-1 0,1 1-1,0-1 1,0 1 0,0 1 0,0-1 0,1 0 0,0 1-1,0 0 1,0 0 0,1 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,1 1 0,0 11 0,1-17-21,1 0 0,-1 0 1,1-1-1,-1 1 0,0 0 1,1-1-1,-1 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,-1 1 0,1-1 1,0 1-1,-1-1 0,1 0 0,0 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,1 0 1,30-3-74,-24 1 59,0-1 0,-1 0 0,0 0-1,1-1 1,-1 0 0,0 0 0,-1-1 0,1 0-1,-1 0 1,0-1 0,11-11 0,4-9-122,30-45 0,-32 42 119,4-4 124,-2-1 0,-1-1 0,29-71 0,-48 104 208,-2 9-270,-1 0 1,0 0-1,0-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,-1 0 0,-5 7 1,-8 14 112,9-10-108,0 0 1,1 0 0,0 0 0,1 1-1,1 0 1,1 0 0,1 1 0,0-1 0,2 1-1,0 36 1,1-53-103,1 0 1,-1 0-1,0 0 0,1 0 0,0 0 1,-1 0-1,1-1 0,0 1 1,0 0-1,0 0 0,0-1 0,0 1 1,0 0-1,1-1 0,-1 1 0,0-1 1,1 0-1,-1 1 0,1-1 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,2 0 0,2 1-1016,1 0 0,0-1-1,-1 1 1,1-2 0,0 1 0,9-1 0,19 0-5132</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="916.55">1441 842 10709,'0'0'7441,"-17"11"-7359,2-2-53,1-1 7,0 1 0,1 1 0,-1 0 0,2 1 0,0 0 0,-13 15-1,8-5 73,1 0 0,1 2 0,1 0 0,1 0-1,1 1 1,0 1 0,2 0 0,2 0 0,0 1-1,1 0 1,2 0 0,0 1 0,2-1-1,0 30 1,4-53-136,-1 0-1,0 0 1,1 1-1,-1-1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 0 1,0 1-1,4 1 0,0 0-320,0 0 0,0 0 0,0-1 0,0 0-1,0 0 1,1-1 0,-1 0 0,10 2 0,21 2-3197</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2192.92">1605 1090 7860,'0'0'8251,"0"-9"-2966,0 52-5199,0-42 290,0-37-51,0-71-194,0 107-77,-1 15-295,-2 90 280,3-76-24,1-15 79,2-18-68,1-24-232,-5 0-32,1 15-1455,0 0-1,0-1 1,3-16-1,-2 26 1105,0 0-1,1 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,0 0-1,0 1 1,1-1-1,-1 0 0,1 1 1,0 0-1,6-6 1,-9 9 782,1-1 0,-1 1 0,0-1 0,1 1 0,-1 0 0,1-1 1,-1 1-1,1 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 1,0 0-1,-1 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 1,-1 0-1,1 0 0,-1 1 0,1-1 0,-1 1 0,1-1 0,10 29 3059,-6 37-1517,-5-65-1629,0 12-326,0 18 356,0-10-5249</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2679.54">2057 1052 10197,'0'0'10183,"3"-11"-9772,2-1-319,-2 8-40,-2 0 0,1-1 0,0 1-1,-1-1 1,0 1 0,0-1 0,0 1 0,-1-1 0,0-7 0,-41 10 140,34 2-195,0 1 0,0 0 0,0 0 0,0 1 0,0 0 0,0 0 0,1 1 0,-1 0 0,1 0 0,0 0 0,-1 1 0,2 0 0,-1 0 0,0 0 0,1 1 0,0 0 0,0 0 0,0 0 0,1 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,2 1 0,-1-1 0,1 1 0,0 0 0,0 0 0,1 0 0,-2 12 0,3-15 8,0 0-1,1 1 1,-1-1 0,1 1-1,0-1 1,0 0 0,0 1-1,0-1 1,1 0 0,-1 0 0,1 0-1,0 0 1,1 0 0,3 5-1,1-2 8,0-1-1,0 0 0,0 0 0,1 0 1,0-1-1,9 5 0,2 1-5,-9-5-55,1 1 0,0-2 1,18 8-1,-37-7-143,-10 0 216,-14 3-205,-37 8 515,26-13-5151</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2941.15">2164 1162 10661,'0'0'5987,"0"26"-6340,0-7 353,0 4 1777,-9-2-896,9-4-785,-4-1-16,0-2-80,4-4-224,-4-3-1089,4-5-560,-4-2-1776</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3113.32">2216 1059 8308,'0'0'7123,"13"-12"-7171,-5 24-96,-4-3-736,0 6-2130,-4-6-1616</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3995.95">2216 1059 10181,'16'35'727,"-11"-25"-349,0 1 0,0-1 0,1 0 0,11 15 0,-6-10 924,-5-9-1001,0 1 0,0 0 0,-1 1 0,0 0 0,0-1-1,-1 2 1,0-1 0,-1 0 0,1 1 0,-2 0 0,1-1 0,-1 1 0,1 16-1,-5-25-168,0 1-1,-1 0 0,1-1 1,-1 0-1,1 1 0,-1-1 1,0 0-1,1 0 0,-1-1 1,1 1-1,-1 0 0,1-1 1,-1 0-1,1 1 0,0-1 1,-1 0-1,-3-2 0,5 0-172,0 1-1,0 0 1,0 0 0,0 0 0,0-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1-1 0,0 1-1,0-1 1,0 1 0,0 0-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,0 1 0,0-1-1,0 1 1,0-1 0,3 0-1,12-4-685,0 1-1,0 1 0,0 1 0,33-3 0,-28 4-392,0-1-1,24-6 1,-69 8 877,16 0 378,0 0 0,1 1 1,-1 0-1,0 0 1,0 0-1,0 1 1,-10 3-1,10-1 6,1 0 1,0 1-1,0 0 0,0 0 0,-8 8 0,12-10-105,0 0 1,-1 0-1,1 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,0 0 0,-1-1 1,1 1-1,0 0 0,0 0 0,0 4 0,4-5-39,0-1-1,0 0 1,-1-1-1,1 1 1,0 0 0,0-1-1,0 1 1,0-1-1,0 0 1,0 0 0,0-1-1,5 0 1,-2 1-33,0 0-54,0-1 1,0 0-1,0-1 1,0 1-1,-1-1 0,1 0 1,0 0-1,-1-1 1,0 0-1,1 0 1,-1 0-1,4-4 0,-5 5 128,-1-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,-1 0 1,1-1-1,-1 1 1,0-1-1,0 1 0,0-1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,0 1-1,0-7 0,-1 8 1604,0 5-1659,0-1 0,0 1 0,0-1-1,1 1 1,-1-1 0,0 1 0,1-1 0,0 1-1,0-1 1,1 3 0,0-3-88,1 0-1,-1-1 1,1 1-1,0-1 1,-1 0-1,1 1 1,0-2-1,0 1 1,0 0-1,0 0 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0-1 0,0 1-1,3-2 1,-1 1 8,0 0 1,0 0 0,0-1 0,0 1-1,0-1 1,0-1 0,-1 1 0,1-1 0,-1 1-1,5-5 1,32-39 2634,-41 45-2011,1 23-390,-7 165 1201,3-162-1208,-1 1 1,-1-1-1,-1 0 0,-1 0 1,-12 28-1,16-48-101,0 0 1,0-1-1,-1 1 1,0-1-1,0 0 1,0 0-1,0-1 1,-1 1-1,0-1 1,1 0-1,-1 0 0,0 0 1,0-1-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1-1 1,-1 0-1,1 0 1,-1-1-1,-6 0 1,4 1-132,0 0 1,0-1-1,0 0 1,0-1-1,0 0 1,0 0-1,0-1 1,0 0 0,0 0-1,1-1 1,-1 0-1,1 0 1,0-1-1,0 0 1,-8-5 0,-9-21-4490,10-9-6688</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4165.63">2635 996 12358,'0'0'4786,"12"75"-7972,-12-52-3120</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5046.95">2947 1280 6915,'0'0'8500,"3"-11"-7654,-1 6-707,1 0-24,-1 0 0,0 0 0,0-1 0,0 1 1,-1-1-1,1 0 0,-2 1 0,1-1 0,0 0 0,-1 0 0,0 1 0,-2-12 0,1 15-100,-1 1 0,1-1 1,0 1-1,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,0 1 0,-4 1 0,-1 0-18,0-1 0,0 2-1,0-1 1,0 1 0,0 0 0,-11 7-1,15-7 4,-1 0-1,1 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 1,-1 0-1,1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 1 1,0-1-1,0 0 0,0 1 0,1-1 0,0 1 0,0-1 1,0 7-1,2-10-13,-1 0-1,0 0 1,0 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1-1,-1 1 1,0-1 0,1 0 0,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,3 0 0,29-3-328,-27 0 282,0 0 1,0 0 0,-1-1 0,0 1-1,0-2 1,0 1 0,0 0 0,0-1-1,6-9 1,-7 10 729,-5 6-663,1 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,1 1-1,-1 0 1,0-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,2 2 0,-2-3 5,0 1-1,0-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0-1-1,0 1 0,-1 0 1,1 0-1,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 0,0-1 1,0 0-1,-1 1 1,1-1-1,-1 0 1,1 0-1,0 1 0,-1-1 1,1 0-1,-1 0 1,0 0-1,1-1 0,4-9 11,-2 0-1,1 0 0,-1 0 0,-1-1 0,0 1 0,-1-1 0,0 1 0,-1-1 0,0 1 1,-1-1-1,-2-12 0,3 22-30,0 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,1-1 0,-1 1-1,0 0 1,0 1 0,0-1 0,-1 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,-1 1 0,0-1-1,1 1 1,-1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1 0,-1 0-1,1-1 1,0 1 0,-4 0 0,0 0-8,1 0 1,-1 1 0,0-1-1,1 1 1,-1 0 0,0 1-1,1-1 1,-1 1 0,1 0-1,0 1 1,-10 5 0,6-2 18,0 0 1,0 1 0,1 1-1,0-1 1,0 1 0,1 1-1,-1 0 1,2 0 0,0 0-1,0 0 1,0 1 0,1 0-1,1 0 1,0 1 0,0-1-1,1 1 1,0 0 0,1 0-1,0 0 1,0 21 0,2-30 6,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0 0 0,0-1 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 1 1,0-1-1,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 1,0 1-1,-1-1 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,2 0 1,69 2-421,-56-3-175,22 0-2436,-5-7-4230</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5294.49">3115 953 6547,'0'0'6931,"-12"79"-6883,8-65-48,0-2-448,-1-7-2177</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5467.42">3115 953 8996,'62'0'3682,"-58"-3"-1361,0 3-208,0 0-929,8 0-767,-4 5-225,1 14-112,-1 4-80,-8 8-80,0 1-881,0-1-1456,-12-3-5314</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6534.72">3357 1271 10757,'0'0'7665,"0"2"-7575,0 4-60,0-4 1354,1 0-1427,-1 0 40,1 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,0 0 0,-1 3 0,-6-2 27,0-1 0,0 0 1,-1-1-1,1 0 1,-1 0-1,0 0 0,-13-2 1,4 0-15,18 1-11,-1 0-1,1 0 0,0 0 1,-1-1-1,1 1 1,-1 0-1,1-1 0,0 1 1,-1 0-1,1-1 1,0 1-1,-1 0 0,1-1 1,0 1-1,0 0 1,-1-1-1,1 1 0,0-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,0 1-1,0 0 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 1,0-1-1,1 1 0,-1-1 1,0 1-1,0-1 1,0 1-1,1 0 0,-1-1 1,0 1-1,0-1 1,1 1-1,12-22-563,-12 21 551,1-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 1,0 0-1,1 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1-1 0,0 1 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,0 2 0,0 0 20,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,0-1-1,0 1 1,-1-1 0,1 1 0,-1-1-1,-4 6 1,-5 3-383,-1 0-1,0 0 1,-20 13-1,-20 20-5573,40-33 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8184.49">3944 547 5907,'0'0'6315,"-4"-36"960,-11 32-7226,-1 1 0,1 1-1,-20-1 1,29 2-58,-1 1-1,0 0 1,0 1 0,1-1-1,-1 1 1,0 1-1,1-1 1,-1 1 0,-11 5-1,16-6-2,1 0-1,-1 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1-1 1,1 1-1,-1-1 0,1 1 1,0 0-1,-1-1 1,1 1-1,0 0 1,0-1-1,0 1 0,1-1 1,-1 1-1,0 0 1,1-1-1,0 4 0,0-2 5,1 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,1 0 0,0-1 0,-1 0 0,7 4 0,8 3-9,1-2 0,0 0 0,30 8 0,30 10-518,-78-25 528,0 0-1,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 1 1,0-1-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,1 0 0,-1 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 0 1,0 1-1,0-1 0,0 0 0,1 0 0,-1 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 1-1,0-1 0,-1 0 0,1 0 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,0 0 1,-1 0-1,1 0 0,0 1 0,0-1 1,-18 9-57,-26 2 141,5-5-626,-2-1 1,-55 0-1,121-17-7223,-1 1 1988</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8482.66">4244 421 11749,'0'0'3437,"2"6"-3323,4 20 170,-2 0 0,0 0-1,-2 0 1,-1 0 0,-3 42-1,1-12-3433,1-51-1770</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9477.79">4194 612 9540,'0'0'5944,"4"0"-5813,58-4 772,84 5 1,26 0-931,-171-1 33,0 0 1,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,-1 0-1,1 0 1,0 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1-1,-1-1 1,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,0-1-1,1 0 1,-1 1 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 0-1,0 0 1,-1 0 8,1 0 0,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 1-1,0 0 1,0-1-1,0 1 1,0 0 0,-3 0-1,-6-1-9,0 1 0,-1 0-1,1 0 1,-1 1 0,1 1-1,0 0 1,-20 6 0,26-7-6,1 0-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,1 0 0,-1 0 0,0 1 0,1-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1-1,1-1 1,-1 1 0,1-1 0,0 6 0,1-9-11,0 1 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1-1 0,0 1 0,31-2-319,-29-1 286,1 0 0,-1 1 0,0-2 0,1 1 0,-1 0 0,-1-1 0,1 0 0,0 1 0,-1-2 0,0 1 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,3-9 0,-5 13 600,20 50-846,-19-48 314,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0-1 0,1 1-1,2 0 1,-3-1 7,0 0-1,0 0 0,0 0 0,0-1 1,-1 1-1,1 0 0,0 0 1,0-1-1,0 1 0,0 0 0,-1-1 1,1 1-1,0-1 0,0 1 1,-1-1-1,1 1 0,0-1 0,-1 1 1,1-1-1,-1 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,1 1 1,-1-1-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 1 0,1-3 0,-1 1-65,1 0 0,0-1 0,1 1 0,-1 0-1,0 0 1,0 0 0,1 0 0,0 1 0,-1-1-1,1 0 1,0 1 0,0-1 0,-1 1 0,1-1-1,0 1 1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 1 0,0-1 0,1 1 0,-1 0-1,5-1 1,11 0-100,0 0 0,29 3 0,-17 0 217,-7 2-100,-19 9 168,2 9 84,-5-21-186,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,2-2 0,26-11 269,-22 7-308,0 1-1,-1-1 1,1-1-1,-2 1 1,1-1 0,-1 0-1,0 0 1,0 0 0,-1-1-1,0 0 1,0 1-1,-1-2 1,3-8 0,-1-4-99,-2-1 1,0 0 0,-2 0 0,0-27 0,-21 98-20,15-22-177,1 1 0,1 1-1,2 51 1,1-56-1474,0-14-1782,4-5-1841</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9682.39">4810 537 11941,'0'0'5747,"16"-4"-5747,13 8 32,4 6-32,8-1-544,0 1-401,0-1-783,-4 0-2674,-12-2-5699</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10065.32">5110 644 4978,'0'0'12390,"-13"0"-11654,17 0-784,13 0-192,8 0-496,3 0-849,-3 0-2065,-5-7-2817</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10362.66">5266 472 11701,'0'0'3271,"-2"6"-2975,-2 41 730,1 59 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11061.72">5360 524 1024,'0'0'8164,"4"-25"-731,8 39-5896,-9-7-1320,-2 1 0,1 0 1,-1 0-1,0-1 0,-1 13 1,5 27 1279,-4-51-1421,1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,6-5 0,-3 3-13,-6 5-74,0 0-1,1 0 1,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,-1 1 1,1-1 0,0 0-1,0 1 1,0-1 0,-1 0 0,1 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,1 0-1,-1 0 1,0-1 0,0 1 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0-1,0 1 1,2 0 0,-1 2-23,0-1 0,0 1 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0 3 1,0-6 15,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,0-1 1,-1 1-1,1-1 0,0 0 0,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,1 0 0,-1-1 0,2 2 0,37 2-7232,-38-4 6431,11 0-6435</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11833.28">5669 548 560,'0'0'14196,"6"-4"-11888,-11 2-2258,0 0 0,0 1 1,0 0-1,0 0 0,0 0 0,0 1 1,-1-1-1,1 1 0,0 1 0,-10 1 1,-3-2-23,16 1-25,-1-1-1,1 1 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 1,0-1-1,0 1 0,0 0 0,0-1 1,1 1-1,-1 0 0,1 0 1,-2 2-1,2-2 3,0-1-1,0 1 1,0-1 0,0 1 0,0 0 0,0-1-1,0 1 1,1 0 0,-1-1 0,1 1 0,-1 0-1,1 0 1,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,1 0 0,-1-1-1,0 1 1,1 0 0,0 0 0,1 2-1,0-3 3,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0-1 1,0 1-1,1-1 0,-1 1 0,0-1 0,0 0 0,1 0 0,-1 0 1,0 0-1,4-1 0,36-7 176,-37 5-175,1-1 0,-1 1 0,0-1 0,0-1 1,0 1-1,-1-1 0,1 1 0,-1-2 0,0 1 0,0 0 1,-1-1-1,5-9 0,-2 2 2,0-1 0,-1 1 0,0-1 0,4-22 0,-12 132-377,4-94 372,-1 0-1,1-1 1,0 1-1,-1-1 1,1 0-1,0 1 1,0-1 0,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,2 0 0,52 2 58,-43-3-64,-11 1-2,-1 0 0,0 0 0,1 0-1,-1 0 1,1 0 0,-1-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,1-1 0,-1 0 0,0 1-1,0-1 1,1 0 0,-1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0-1 1,0 1 0,-1 0 0,1-1 0,0-1-1,3-44 175,-4 42-110,-2 4-26,0 0 0,0 1-1,-1-1 1,1 1 0,0 0 0,-1-1-1,1 1 1,0 0 0,-1 0 0,1 1-1,0-1 1,-1 0 0,-3 2 0,3 0-36,-1 0 1,1 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,1-1 0,0 1 0,-2 6 0,0 2-158,1 1 0,0-1 0,1 1 0,0 15 0,1-26-27,0 0 1,0 0 0,1 0-1,-1 0 1,0-1-1,1 1 1,0 0-1,-1 0 1,1-1 0,0 1-1,0 0 1,0-1-1,0 1 1,0-1 0,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 0 1,1 0 0,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0 0,0 0-1,-1-1 1,1 1-1,0-1 1,0 1-1,0-1 1,2 0 0,21 2-4095</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12185.76">5997 502 9204,'0'0'7729,"1"6"-7369,-1 1-526,7 73 1048,-7-75-1127,0 0 0,0 0 0,0-1-1,-1 1 1,0 0 0,1-1 0,-2 1 0,1 0 0,0-1 0,-1 1-1,0-1 1,0 0 0,0 0 0,-5 7 0,6-11 38,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1 0,-1-1 0,0 0-1,1 1 1,-1-1 0,0 0 0,1 0 0,-1 1-1,0-1 1,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,1 0 0,-1 0 0,0 0-1,1-1 1,-1 1 0,0 0 0,1 0 0,-1-1-1,0 1 1,1 0 0,-1-1 0,1 1 0,-1 0 0,0-1-1,1 1 1,-1-1 0,1 1 0,0-1 0,-1 0-1,1 1 1,-1-1 0,1 1 0,0-1 0,-1 0 0,1 1-1,0-1 1,0 0 0,-1 0 0,-13-40-2559,12 35 3035,-3-44 8354,5 43-5808,34 5-446,-24 3-2272,1 0 1,-1 1-1,1 0 0,-1 1 1,0 0-1,0 1 1,0 0-1,0 0 1,17 12-1,-6-2-85,0 1 1,37 33-1,-53-44-347,-1 0 0,0 0 1,0 0-1,0 1 0,-1 0 1,1-1-1,-1 1 0,0 0 0,-1 0 1,1 1-1,-1-1 0,2 7 1,-2 17-7414</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14109.5">2458 237 6835,'0'0'7969,"1"0"-7954,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1-1 0,0 1-1,0 0 1,0 0 0,0 0 0,168-20 4563,-68 6-3860,114-1-1,-213 15-626,-13 0-6,-65 5-75,-145 26 0,211-29-11,8-2-4,1 0 0,0 0 0,0 1 1,0-1-1,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0 0 1,-2 3-1,4-4-2,1 1 0,-1-1 1,1 1-1,-1 0 0,1-1 0,-1 0 1,1 1-1,0-1 0,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 0,0 0 1,0 1-1,-1-1 0,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,1 0-1,65 6-82,20-6 1,110 1-1497,-67 2-3345,-82-2-294</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="14854.52">3846 954 6515,'0'0'11933,"0"-1"-11846,0 1 0,0 0 0,0 0 0,0-1-1,0 1 1,1 0 0,-1 0 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0-1-1,0 1 1,-1 0 0,1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0 0 0,-1-1 0,-8 2-81,-1 0 0,1 1 0,0 0 0,-1 1 0,1 0 0,0 0 0,0 1 0,1 0 0,-1 0 0,1 1 0,0 1 0,0-1 0,1 1 1,-1 0-1,1 1 0,1-1 0,-1 2 0,1-1 0,0 1 0,1-1 0,0 2 0,0-1 0,1 0 0,0 1 0,0 0 0,1 0 0,0 0 1,-1 11-1,2-6-9,0 0 1,1 0 0,1 0-1,1 0 1,3 23 0,-3-33-17,0 1 1,1 0 0,0-1 0,0 1-1,0-1 1,1 1 0,-1-1 0,1 0-1,0 0 1,0 0 0,0-1 0,1 1-1,-1-1 1,1 0 0,0 0 0,0 0 0,0 0-1,0-1 1,9 4 0,-1-1-3,1-1 1,-1 0 0,1-1-1,-1 0 1,1-1 0,0-1-1,0 0 1,0-1-1,0 0 1,24-4 0,-35 3 28,-1 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-2-1 0,1-1-4,0 1-1,-1 0 1,1 0 0,-1 0 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 1-1,-1-1 1,1 1 0,-1 0 0,0 0-1,-5-3 1,3 3-14,-1 0-1,0 1 1,0-1 0,0 1-1,0 0 1,0 1 0,0 0-1,0-1 1,0 2-1,-11 1 1,13-1-294,1 0-1,-1 0 1,1 0 0,0 0 0,0 1-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0 0,1 1-1,-1-1 1,1 1 0,-1-1 0,1 1-1,0 0 1,0 0 0,0 0-1,-2 5 1,-2 9-4834</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="16642.19">2848 1682 5491,'0'0'10836,"78"0"-7847,-59 0-2735,-4 1-166,0-1 0,-1-1 0,1 0 0,-1-1 0,0 0-1,15-5 1,-115 2 1297,78 5-1393,-3 0 1,-1 0-1,1 0 0,-1 2 1,1-1-1,-1 1 0,-12 4 1,111-5-463,-19 1-4788,-43-2 346</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="33959.26">3025 434 6627,'0'0'6035,"0"-6"-5288,1-9 153,-1 6-452,1 1 0,-1 0-1,-1-1 1,0 1 0,0 0 0,-4-15-1,4 21-434,0 0 0,0 1 0,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-3 2 0,2-1-15,1 0-1,0-1 1,-1 1 0,1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,-1 3 0,1-1-10,-1 1 0,1-1 0,0 0-1,1 0 1,-1 1 0,1-1 0,0 0 0,0 1 0,2 7-1,-1-11 2,0 0-1,0-1 1,0 1-1,0-1 0,0 1 1,1-1-1,-1 0 0,0 0 1,1 1-1,-1-1 0,1 0 1,-1 0-1,1 0 0,-1-1 1,1 1-1,0 0 1,-1 0-1,1-1 0,0 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,0 0 0,0 0 1,0 0-1,-1 0 0,4-1 1,-2 1-4,0 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 0 0,0 1 1,1-1-1,-1-1 0,0 1 0,-1 0 0,1-1 0,0 0 0,0 1 0,3-4 0,1-5-21,0 0-1,-1-1 0,0 0 1,0 0-1,-2 0 1,5-13-1,-3 13-541,1 16 358,0 11 202,6 31 7,-13-47 12,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,0 0-1,1 1 1,-1-1-1,0 0 1,0 1-1,1-1 0,-1 0 1,0 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,0 0 1,1 1-1,-1-1 0,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,0-1-1,1 1 1,-1 0-1,1 0 0,-1 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,1-1-1,-1 1 1,1-1-1,10-10 112,-8 6-98,-1 0-1,0 0 1,0 1-1,0-1 1,-1 0-1,0 0 1,0-1-1,0 1 1,-1 0-1,1 0 0,-1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,-2 0-1,-1-7 1,2 9-16,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,-1 0 1,1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,-7 2 0,-1-2-7,1 2 0,0 0 0,-1 0 0,1 1 0,0 0 0,0 0 0,0 1 1,0 1-1,1 0 0,-1 0 0,-14 10 0,19-11 7,0 1 0,0 0 0,1 0-1,0 1 1,-1 0 0,2-1 0,-1 1 0,0 0 0,1 1-1,0-1 1,0 1 0,1-1 0,0 1 0,0 0 0,0 0-1,0 0 1,1 0 0,0 0 0,1 0 0,-1 0 0,1 7-1,0-12 6,0 0-1,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,0 0 0,0 0 1,-1-1-1,1 1 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 1,0 0-1,1 0 0,-1 1 0,2-1 1,45 0 259,-31-1-39,13 1 58,1-1 0,39-7-1,-57 5-1448,0 0 0,0-1-1,0 0 1,19-10 0,-11 2-4737</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34459.98">3423 191 10213,'0'0'4604,"1"6"-4508,2 6 29,-1 0-1,0 1 0,0 20 0,-2-29-102,0-1 0,0 0 1,0 1-1,0-1 0,0 1 0,-1-1 0,0 0 1,0 1-1,1-1 0,-2 0 0,1 0 1,0 0-1,-1 1 0,1-1 0,-1-1 0,0 1 1,0 0-1,0 0 0,-1-1 0,-3 4 1,2-61 1817,4 43-1839,1 1 0,0 0 1,1-1-1,0 1 0,0 0 0,1 0 0,1 1 0,0-1 0,0 1 0,1-1 0,0 1 0,12-15 0,-17 24-2,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 1 1,1-1-1,-1 0 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1 1,-1 1-1,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 0 0,1-1 0,-1 2 0,20 44 204,-19-44-193,2 11 97,0 0-1,-1 0 0,-1 1 0,0-1 1,-1 24-1,-1-30-306,0 1 0,0 0 0,0-1 0,-6 15 0,6-19-208,0 0 0,-1-1 0,1 1-1,0 0 1,-1-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0-1,0 0 1,-4 2 0,-3 1-5392</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="36473.49">3407 326 8948,'0'0'5088,"15"-5"-4861,296-77 1168,-305 80-1368,0-1 0,0 1 0,0-1-1,-1 0 1,0 0 0,1-1 0,-1 1 0,-1-1 0,1 0 0,0-1 0,5-6 0,-8 8-13,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,0-1 1,0 0-1,0 1 0,0-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,-1 1 0,1-1 0,-1 0 1,1 0-1,-2-3 0,1 6-18,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 1,-1 1-1,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-2 0 0,-32 6-65,31-3 69,-1 0 0,1 0 1,0 0-1,1 1 0,-1-1 1,0 1-1,1 0 0,0 0 0,0 0 1,0 0-1,1 1 0,-1-1 1,1 1-1,0-1 0,-2 9 1,-3 10 28,1 0 1,-3 26 0,3-10 41,5-39-49,1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0 0,1 0-1,-1 1 1,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,1 1 1,-1-1-1,0 0 1,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 1 0,0-1-1,1 0 1,14-6 352,26-22-472,-30 20 202,-6 4-102,1 1 1,-1 0 0,1 0-1,-1 1 1,1-1 0,0 1-1,11-2 1,-15 4 1,0 0 0,0-1-1,1 1 1,-1 1 0,0-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 1 0,-1 0 0,1 0-1,0-1 1,0 1 0,0 0 0,-1 1 0,1-1-1,0 0 1,-1 0 0,1 1 0,-1-1 0,1 1-1,-1-1 1,0 1 0,2 3 0,8 14 258,-8-14-350,-1-1 0,1 1 1,0-1-1,0 0 1,0 0-1,0 0 0,5 4 1,-6-7-221,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 1,1-1-1,-1 0 0,0 1 0,0-1 0,0 0 0,0-1 1,0 1-1,0 0 0,1-1 0,-1 1 0,0-1 0,3-1 1,-1 1-65,-1-1 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0-1 0,4-5 0,23-37 526,-10 14 2007,-20 31-2068,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,4 18 1407,-2 28-1030,-2-45-128,3-3-199,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,-1-1 0,3-4 0,7-6-115,-9 10-38,-2 2 3,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,3-1 0,-1 4 24,-1 1-1,1-1 1,-1 0-1,0 1 1,0-1-1,0 1 1,-1 0 0,1 0-1,-1 0 1,0 0-1,0 0 1,0 0 0,0 7-1,21-17 1366,75-60-1334,-96 65-45,16 44-307,-14-40 286,0 0 1,0 0 0,0-1 0,0 1 0,1-1 0,0 0 0,-1 1-1,1-2 1,0 1 0,0 0 0,0-1 0,0 0 0,0 0 0,0 0-1,1 0 1,-1-1 0,0 1 0,9-2 0,9 2-499,0-2 0,28-4 1,-44 4 511,-1 0 0,1 0 0,-1 0 1,0-1-1,1 1 0,-1-1 0,0-1 0,0 1 1,0-1-1,0 0 0,-1 0 0,1 0 1,-1-1-1,0 0 0,0 1 0,0-1 0,0-1 1,-1 1-1,1-1 0,-1 1 0,0-1 0,-1 0 1,1 0-1,-1 0 0,0 0 0,0-1 1,-1 1-1,1 0 0,-1-1 0,0-10 0,-4 15 55,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 1 0,0-1 0,0 0-1,-4 2 1,2 0-48,0 0-1,0 0 1,0 0 0,1 1-1,-1 0 1,1 0-1,0 0 1,-1 1-1,2-1 1,-1 1-1,0 0 1,1 0 0,0 0-1,-1 0 1,2 1-1,-1-1 1,0 1-1,1 0 1,0 0-1,0 0 1,1 0 0,-1 0-1,0 6 1,2-11-5,1 1 1,-1-1-1,0 1 1,1-1 0,-1 1-1,0-1 1,1 1-1,-1-1 1,1 0 0,-1 1-1,0-1 1,1 0-1,-1 1 1,1-1 0,-1 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,2 0-1,19-1 24,-19 1-23,5-1 5,0 0 0,-1-1 0,1 0-1,0-1 1,-1 1 0,1-1 0,-1 0-1,0-1 1,0 1 0,0-1 0,9-8-1,21-13 2332,-36 28-2334,0-1-1,0 1 1,1 0-1,-1 0 1,1-1-1,-1 1 1,1 0-1,0-1 1,0 1-1,0-1 1,1 1-1,-1-1 1,0 1 0,1-1-1,0 0 1,-1 0-1,1 0 1,2 3-1,1-2-96,-1 0-1,0-1 0,0 1 1,1-1-1,-1 1 1,1-1-1,0-1 1,0 1-1,7 1 0,11 0-922,0 0-1,0-2 1,37-2-1,-32 1-536,-26 0 1492,-1 0-1,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1-1 1,0 1-1,1 0 0,-1-1 1,0 1-1,0-1 0,0 1 1,1-1-1,-1 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-2 1,-1 1-1,1 0 0,1-1 0,2-32 1314,-4 30-1001,0 3-155,-1 1 1,1-1-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,1 1 1,-1-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-2 0-1,-41 0 1233,33 1-1243,9-2-76,-1 1 0,1 1 1,0-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 1 0,0 0 1,0 0-1,0-1 1,0 1-1,1 0 0,-1 1 1,0-1-1,0 0 1,1 0-1,-1 1 1,1-1-1,-1 1 0,1-1 1,0 1-1,0 0 1,-1 0-1,1-1 0,0 1 1,1 0-1,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,1 3 1,4-4 2,1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0-1 0,6 0 0,-6-1 7,1 1 0,-1-1 1,0 0-1,0-1 0,0 1 0,-1-1 1,1 0-1,-1-1 0,1 1 1,-1-1-1,0 0 0,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 0 1,-1 0-1,6-9 0,-5 3 23,1 0-1,-2 0 1,1-1-1,-2 1 0,1-1 1,-2 0-1,1 1 1,-2-1-1,0-12 1,1 4-156,-2-37 877,-1 52-434,-4 34-451,1 2 163,2 0 1,1 1-1,3 37 0,0-56-21,0 1-1,1-1 1,1-1-1,0 1 1,1 0-1,0-1 1,1 0-1,0 0 1,1 0-1,11 16 1,22 20-154,-30-38-456,1 1 0,-2-1-1,0 1 1,0 0 0,-1 1-1,0 0 1,-1 0 0,8 24-1,-12-9-3854</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink13.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:02:36.928"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">218 50 3282,'0'2'22389,"0"16"-22552,-17 182 405,1-54-41,10-73 12,6-73-239,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,-8-8-4329,-2-8-4249</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="334.14">96 171 15319,'0'0'6707,"3"-12"-6195,-3 12-511,1-5 42,0 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,1 0 0,-1 1 1,1-1-1,0 1 0,0-1 1,0 1-1,0 0 0,1 0 0,0 1 1,0-1-1,0 1 0,0 0 1,0 0-1,6-3 0,17-8 199,1 1 0,54-17 0,-69 27-287,0-1-1,0 2 0,0 0 1,0 0-1,0 1 0,0 1 1,1 0-1,-1 1 1,16 3-1,-28-4-75,1 1 0,-1 0-1,0-1 1,1 1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0-1,1 1 1,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1-1,0 1 1,0 1 0,0 2-564,0 0 1,0 1-1,-1-1 0,1 0 0,-1 0 1,-1 0-1,-1 7 0,-15 20-6604</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="629.47">22 585 13190,'0'0'9476,"-22"6"-8867,33-6-177,10 0-128,22 0 288,7-4-272,6-11-256,8 3 32,-11-4-96,-10 4-608,-11 2-2193,-8 2-1937,-6 0-3794</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1337.58">575 303 6627,'0'0'14252,"0"0"-14231,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1-1 0,-1 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,1 0-1,-1-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0-1,3 12 319,-1 0 0,-1 1 0,0-1 0,0 1 0,-1-1 0,-3 16 0,2 11 194,-10 20 219,11-58-426,0-13 15,1 1-331,0 1 1,0-1-1,1 1 1,1-1-1,0 1 1,6-14-1,-8 19-16,1 1 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 0 0,1 1 1,0-1-1,1 1 0,-1 0 0,0 0 0,1 0 0,0 0 1,-1 1-1,1 0 0,7-4 0,-8 6-3,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,3 2 0,4 6 10,1 1 1,-2 0-1,11 16 0,-14-19 1,1 0 0,-1 0 0,1-1 0,0 0 1,12 10-1,-17-16 9,0-1 1,0 1 0,0-1-1,-1 0 1,1 1 0,0-1-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 0 0,0 0-1,-1 1 1,1-1 0,-1 0-1,1 0 1,0 0 0,-1 1-1,1-3 1,21-43 230,-18 34-243,4-5-111,-1 0-1,-1-1 1,-1 0-1,-1 0 1,0 0-1,2-29 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1616.5">1047 215 15431,'0'0'9119,"-4"74"-7772,-15-6-639,13-50-1080,0 0-1,1 1 0,2 0 1,-3 32-1,17-53-8170,2-10 284</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1911.52">1067 270 10213,'0'0'13408,"-1"-5"-12986,0 4-425,1 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,1 0 0,3 0-15,1 0 0,0 0 0,0 1 0,-1 0 0,1 0 0,8 3 1,-4-2 24,0 1 0,-1 1 1,1 0-1,-1 1 0,0-1 1,0 2-1,0-1 0,0 1 1,14 14-1,-19-16-4,0 0-1,0 1 1,-1 0 0,1 0 0,-1 0-1,0 0 1,-1 0 0,1 0 0,-1 1-1,0 0 1,0-1 0,-1 1 0,1 0-1,-1 0 1,-1 0 0,1-1-1,-1 1 1,-1 10 0,1-14 36,-1 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1-1,0 0 1,-1 0 0,1 1 0,-1-1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,-4 2 0,-54 22 825,48-21-797,-18 7 15,-46 20-788</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2220.61">1373 303 17336,'0'0'7230,"-7"-10"-5248,5 40-1972,-1 0 0,-1 0 0,-15 51 0,7-30-1290,10-31-2221,2-7-3595</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2701.33">1600 296 13542,'0'0'7689,"-1"15"-6955,-2 14-369,-1 0 0,-1 0 0,-2 0 0,-1-1 0,-1 0 0,-13 28 1,22-56-355,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-2-15 179,4-22-235,5 8-11,3 2-1,0-1 1,1 1-1,2 1 1,1 0 0,20-29-1,-8 25-27,-14 29-35,-2 19 37,-5 5 163,-1 1 0,-1 0 0,-1-1-1,-2 41 1,-1-33-224,2-1 1,5 35-1,-5-55-3446</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2906.14">1593 470 8052,'0'0'13878,"60"-28"-13798,-17 16-16,-1 0-64,-6 2-176,-8 1-320,-14 3-1089,-14 4-896,-10 2-256</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink14.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:02:45.016"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">107 103 4786,'0'-3'16502,"0"-1"-13003,-1 12-3493,-1-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,-7 13 0,-4 12 37,-47 117 133,57-143-156,-2 14 75,6-19 51,9-11-9494,4 0-51</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="979.13">584 95 2353,'0'0'14866,"-3"-40"-10809,4 38-3986,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 1,0 0-1,4-2 0,36-14 176,-36 15-239,0 0 1,0 0-1,0 1 1,0 0-1,12-1 1,-17 4-17,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 1 1,-1 1 0,1 0 3,0 1 10,-1 1 0,0 0 0,0 0 0,0 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,-1 0 0,1 0 0,-7 6 0,-1 1 8,-1-1 1,0 0-1,-1-1 0,-14 9 1,26-18-14,0-1-1,0 0 1,0 1 0,0-1 0,0 1-1,1 0 1,-1-1 0,0 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0 0,1 0-1,-1 0 1,1 2 0,0-3 5,1 1 0,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 1,1 0-1,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,1 0-1,59 0 316,-49 0-254,17-2 1476,-15 0-3426,-7 2-2545,0 0-3388</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1738.4">1031 114 11445,'0'0'7876,"1"-34"-4461,7 30-3414,-1 0 1,0 1-1,1-1 0,-1 1 1,1 1-1,0 0 1,0 0-1,0 0 1,0 1-1,0 0 1,1 0-1,9 2 0,-23 26-169,2-21 188,-2 1-1,1-1 1,-1 0-1,0 0 0,0 0 1,0-1-1,-1 0 0,-12 9 1,11-10-24,1 1-1,0 0 1,0 1-1,0-1 1,1 1 0,0 0-1,0 0 1,1 1-1,-5 7 1,11-12-86,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 1,0 1-1,0 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,4 1 0,18 10-291,-23-12 374,0 1 1,0-1-1,0 1 1,-1 0-1,1-1 1,0 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 2-1,-2-2 17,1 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,-3 0 0,-61 11 862,61-11-1108,-30-2 1289,24-6-2403,14-9-3685,6 6-274</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2656.47">1279 106 7267,'0'0'8964,"10"-26"-3249,-9 26-5695,-1-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 1,0 0-1,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,1 23 97,-2-21-114,0 66 280,1-67-279,-1-1-1,1 1 1,0-1 0,-1 0-1,1 1 1,0-1-1,-1 0 1,1 1 0,0-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1-1-1,1 1 1,0 0 0,-1 0-1,1-1 1,1 0 0,23-8-33,-21 7 10,-1 0-1,1 0 1,-1-1-1,1 1 1,-1-1 0,0 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,-1 0 1,0-1-1,1 0 1,-2 0-1,1 1 1,2-7 0,-4 9 35,-1 36-347,-5-12 489,-1 0 0,0-1 0,-21 39 0,28-55 560,1-3-2629</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3084.09">1688 95 10261,'0'0'7790,"-5"0"-7515,3 0-224,-1 0 1,1 0-1,-1 1 1,1-1-1,0 0 0,0 1 1,-1 0-1,1-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,1 1 0,-1 0 1,0-1-1,1 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1 0 1,0 1-1,0-1 1,0 3-1,0-2-37,1 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1-1 0,-1 1-1,1 0 1,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,5 4 0,-4-3 0,1 1 0,-1-1 0,1 1 0,-1 0 0,0 0 0,-1 1 0,3 4 0,-5-8 25,0 1-1,0-1 1,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1-1,0 0 1,0 1 0,0-1 0,-3 0 0,-23 5-1301,10-7-5692</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3341.47">1695 104 10773,'0'0'10183,"6"-3"-9759,26-9-307,0 1 0,53-9 0,-50 13-5772,-59 14-3026</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
       <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:02:59.520"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
@@ -17282,7 +17876,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="192.1">479 1 16023,'0'0'897,"46"24"-6788</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="476.8">1127 24 10853,'0'0'6462,"-16"9"-4950,5-3-1214,-1 0-91,2-1 0,-1 2 0,1 0 1,0 0-1,0 1 0,1 0 0,0 0 0,0 1 0,-8 12 0,-12 19 578,3 2 0,-37 78 0,53-97-690,1 0-1,1 1 1,1 0-1,1 0 1,2 1-1,0 0 1,0 34-1,3-56-105,1 0-1,0 0 0,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,0-1-1,0 1 0,0 0 1,0 0-1,1-1 1,-1 1-1,1-1 0,0 1 1,0-1-1,-1 1 1,2-1-1,2 2 0,-1-1-235,1-1 0,-1 1 1,1-1-1,0-1 0,-1 1 0,1-1 0,0 1 0,0-2 0,0 1 0,1 0 0,6-1 0,34-1-4987,6-5-4229</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1110.92">1241 163 7203,'0'0'12030,"-18"48"-10323,15-34-1999,-3 24 813,12-24-2856,11-9-4069,-3-5-135</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1294.18">1254 163 9220,'60'-11'5971,"-60"20"-5571,-4 7 112,-3 0-336,0 6-128,0-1-48,4 1 0,-1-4-544,4-4-2257,0-4-4242</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1294.17">1254 163 9220,'60'-11'5971,"-60"20"-5571,-4 7 112,-3 0-336,0 6-128,0-1-48,4 1 0,-1-4-544,4-4-2257,0-4-4242</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1583.22">1417 215 10517,'0'0'9676,"0"8"-8350,-2 18-966,-2 0 0,0 0 0,-2-1-1,-15 46 1,1-6-254,19-63-151,-13 45-653,1-20-4543,6-18 575</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1844.16">1321 231 11925,'0'0'6003,"85"-63"-5843,-60 61-48,-4 0-96,-3 2 0,0 0 0,-4 0-16,-7 12-48,-3 2-496,-4 2-400,0 5-561,-4 1-2241,-10 0-1904</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2036.08">1261 531 10309,'0'0'7411,"-11"4"-7283,29-4 96,3 0 0,11 0-224,4-8-608,3-2-2001,-8-4-5075</inkml:trace>
@@ -17295,7 +17889,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink16.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -17323,7 +17917,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink17.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -17352,7 +17946,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink18.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -17380,7 +17974,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink19.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -17406,185 +18000,6 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">79 318 11253,'0'0'5312,"1"-13"-4594,6-44 378,-5 51-942,1 0 0,0 0 0,0 0 0,0 0 0,1 0 1,0 1-1,0 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,0 1 0,9-4 0,-10 5-10,2-1 46,-1 0 0,1 1 0,0 0 0,0 0 0,1 1 0,-1-1 0,11-1 0,-16 3-183,0 1 0,1 0-1,-1 0 1,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 2 0,-1 6 3,-1 0-1,1 0 0,-2 0 0,1 0 1,-1-1-1,-1 1 0,1-1 0,-2 0 0,1 0 1,-1 0-1,0 0 0,0-1 0,-12 12 1,-12 11 49,-51 42 0,79-71-59,-14 13 10,11-10 0,-1 1 0,1 0 0,-1-1 0,-1 0 0,1 0 0,0 0 0,-1-1 0,0 0 1,0 0-1,-12 4 0,18-7 70,0-2-72,1 0 1,-1 1 0,1-1-1,-1 1 1,1-1 0,0 0-1,0 1 1,0-1 0,0 1-1,0 0 1,0-1 0,0 1-1,1 0 1,-1 0 0,0-1 0,1 1-1,-1 0 1,1 0 0,-1 1-1,1-1 1,-1 0 0,1 0-1,0 1 1,-1-1 0,1 1-1,0 0 1,-1-1 0,3 1-1,3-2-42,1 1 0,-1 0 1,0 1-1,0-1 0,12 2 0,-14 1 34,0 0 1,0 0-1,0 0 1,0 1 0,0 0-1,0 0 1,-1 0-1,1 1 1,-1-1-1,0 1 1,4 5 0,32 23-366,-31-28-798,0 0 0,0 0 0,0-1-1,1 0 1,-1 0 0,1-1 0,17 1 0,8-2-6838</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="279.95">420 67 4178,'0'0'18696,"0"-11"-17884,2-34-294,2 34-423,-2 20-140,13 18 74,-2 1 0,0 1 1,-2 0-1,-2 1 0,0 0 1,5 36-1,-10-47-4,-1-1 1,-1 1-1,0 0 0,-1-1 1,-2 1-1,1 0 0,-7 32 1,4-41-199,0 0 0,0 0 0,-1 0 1,0 0-1,-1-1 0,-7 12 1,5-12-485,0 0 0,-1 0 0,0 0 0,0-1 0,-1 0 0,-12 8 0,-79 44-12386</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:03:15.421"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">19 140 13654,'0'0'3538,"54"0"-3122,-37-2-272,5 0-64,-5 2-64,-3 0-16,1 0-256,-8 0-640,0 2-721,-7 4-1489,0 4-1135</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="205.23">0 259 10885,'0'0'7507,"50"-6"-6994,-22-2-257,4 0-176,-3 2-64,-4 0-16,-4 0-448,-3-2-913,-4 2-304,-7-3-1760,3-1-1442</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="650.2">213 54 6931,'0'0'12155,"-8"-10"-10458,-26-26-337,22 29 788,8 16-1870,7 17-476,0-19 189,1 0-1,0-1 1,0 1-1,0-1 1,0 0-1,1 0 1,0 0-1,1-1 1,-1 1-1,1-1 1,0 0 0,0-1-1,1 0 1,-1 0-1,1 0 1,9 3-1,-2-1-165,-1 0-1,1-1 0,0-1 1,0 0-1,1-1 0,-1-1 1,24 2-1,-17-4 107,-29 15 95,-80 63 286,56-52-119,-50 53-1,29-16-1305</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1630.17">803 101 6227,'0'0'10471,"0"-6"-9267,1-10-1063,0-7 4563,-12 43-2872,-47 144-1600,57-193 522,0 20-757,0 0 0,1 0-1,0 0 1,1 1-1,1-12 1,-1 15-7,0 1 1,0-1-1,1 1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,3-3-1,-5 6-1,-1 0 0,1 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,2 1 1,-1 0-2,1-1 1,-1 2-1,1-1 0,-1 0 1,1 0-1,-1 1 0,0-1 0,0 1 1,4 4-1,6 4 32,0 1 0,-1 1 0,-1 0 0,0 1 0,-1-1 0,12 23 0,-14-27-1255,-6-8 830,-1 0 0,1 1 0,-1-1-1,1 0 1,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,6-9-6987</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1878.71">993 51 6243,'0'0'9938,"1"-4"-9357,1-11 65,-3 39 895,-8 44 258,-7-20-1522,-2 9-303,13-18-3103,8-37-1016,12-4 128,-1-8-297</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2132.15">1032 153 3570,'0'0'5941,"2"-12"-3836,2-1-1214,4-14-89,-8 0 4770,2 44-4907,-1 0 0,-1 0 0,0 1-1,-4 21 1,2-23-827,-2-1-1,0-1 0,0 1 0,-1-1 0,-9 18 0,9-18-2823</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2388.58">1033 133 2881,'0'0'15189,"3"-9"-14253,11-25-352,-13 33-564,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,1 1-1,-1-1 1,0 0 0,1 1-1,-1 0 1,0-1 0,1 1-1,-1 0 1,1-1 0,-1 1-1,0 0 1,1 0 0,-1 0-1,3 1 1,27 4 305,-25-2-271,0 0-1,-1 0 1,1 1-1,-1-1 1,1 1-1,-1 1 1,-1-1-1,1 1 1,-1-1-1,6 8 1,-7-9 53,-1 1-1,1 0 1,-1-1 0,1 1 0,-1 0-1,0 0 1,0 0 0,-1 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,-1 1 0,1-1-1,-1 7 1,-2-8-62,1-1 1,-1 0-1,0 1 0,0-1 0,0 0 1,-1 0-1,1 0 0,0-1 0,-1 1 0,0 0 1,1-1-1,-1 0 0,0 1 0,1-1 1,-1 0-1,0 0 0,0-1 0,-3 1 1,-6 4 20,-73 27-324,27-13-2779,11-8-2976</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink16.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:03:31.197"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">186 202 11909,'0'0'10282,"0"-5"-9510,1-29 1321,-1 30-409,-1 27-1571,1-19-228,-4 27 263,-2 1 0,-1-1 0,-16 48 0,-10 38-2413,25-37-5128,8-59 1823</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="242.69">66 235 13078,'-3'-15'694,"1"-2"-282,-3-11 1271,1-1 0,1 1 0,3-54 0,0 80-1652,1 0 0,0 0 1,0 0-1,-1 1 0,1-1 0,1 0 0,-1 1 0,0-1 0,0 1 1,1-1-1,-1 1 0,0 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 1 0,0 0 1,4-1-1,57-3-106,-56 5 102,-2-1-92,1 0 0,-1 0 0,-1 1 0,1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 1 0,5 5 0,-4-3-346,-1 0 1,0-1-1,0 1 0,-1 1 0,0-1 0,0 1 1,0-1-1,-1 1 0,0 0 0,0 0 1,0 0-1,0 9 0,-1 20-4287</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="421.48">1 523 9941,'0'0'5938,"67"4"-5890,-24-4-48,3 0-832,0-6-3730</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="870">398 366 12054,'0'0'5052,"0"9"-4323,0 169 2782,25-201-3127,-2-3-322,-11 13-32,0-2 0,14-21 0,-21 36-277,0 12 166,3 19 114,-7-27-42,0 2 20,1-1 1,-1 1-1,1-1 1,0 0-1,0 0 1,1 0-1,0 0 1,0-1-1,0 1 0,0-1 1,0 1-1,9 7 1,-8-10-77,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 0 0,1 1 1,-1-2-1,1 1 0,-1 0 0,7-3 0,-3 2-579,-1-1 0,1 0-1,-1 0 1,0-1 0,0 0 0,8-5 0,8-8-4233</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1794.6">828 434 3986,'0'0'12910,"-3"-8"-11939,2 6-961,1 0 52,-1 0 1,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1-1,0 1 1,0 0 0,0 0 0,0-1 0,0 1 0,0 1 0,0-1 0,0 0 0,-1 0-1,1 1 1,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,-2 0-1,2 1-36,-1-1-1,1 1 0,-1 0 0,1 0 0,0 0 1,0 1-1,0-1 0,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,1 1 1,-1-1-1,1 1 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 7 1,-1-1-5,1-1 0,-1 1 0,2 0 0,0 0 0,0 0 0,0 0 0,1 0 0,0 0 0,3 12 1,-3-20-18,1 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,-1 0 1,1 0-1,0-1 0,0 1 0,-1 0 1,1-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 1,1 0-1,34-17 47,-19 2-262,-2-1 0,0 0 0,-1-1 0,-1-1 0,-1 0 0,-1 0 0,0-1 0,-1-1 0,-2 1 0,0-2-1,-1 1 1,-1-1 0,-1 0 0,-1 0 0,0-1 0,-1-30 0,-3 53 242,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,-1 1 0,-9 6 376,-7 13-357,9-3 29,0 1-1,2 0 0,0 0 1,1 1-1,0-1 1,2 1-1,0 0 0,2 0 1,0 1-1,0-1 1,2 0-1,4 23 0,-5-39-70,0-1-1,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,0-1 0,1 1 0,0 0 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1-1 0,2 2 0,-1-2 10,-1-1-1,1 1 0,0 0 0,-1-1 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0-1 1,0 1-1,0 0 0,3-6 0,3-4-42,-1 0-1,-1-1 1,0-1 0,-1 1-1,0-1 1,-1 0-1,0-1 1,-2 1-1,1-1 1,1-22 0,-12 99 201,5-49-110,0 0-1,1 0 1,0 0-1,1 0 1,3 26-1,-2-37-86,-1 0-1,1-1 0,0 1 1,0 0-1,-1-1 0,1 1 1,0 0-1,0-1 0,1 1 1,-1-1-1,0 0 0,0 1 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 0,0-1 1,-1 1-1,1 0 0,0-1 1,2 1-1,0 0-729,1-1 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 0-1,-1-1 1,1 0-1,5-1 0,16-11-11555</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1926.27">1277 156 14663,'0'0'1793,"14"48"-12006</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2359.55">1397 279 10229,'0'0'10575,"-14"-4"-10137,-49-7-324,61 11-113,-1 0 0,1 1-1,0-1 1,-1 0-1,1 1 1,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1-1,1 1 1,-1 0-1,1-1 1,-1 1 0,1 0-1,-2 3 1,-18 46 25,17-40 1,2-3-36,0 0-1,0 0 0,1 0 1,0 1-1,1-1 1,0 9-1,0-10-6,1-7 15,-1 1 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,0-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,2 1 0,33-10 3,-25 0-2,1 0 0,-1 0 0,-1 0 0,0-2 0,0 1 1,-1-1-1,-1 0 0,9-19 0,1 1 7,-17 30-11,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1-1,0-1 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0-1,5 16-65,1 24 162,-5-36-67,-1 2 12,1 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,0 0 1,1-1-1,-1 1 0,1-1 1,1 1-1,-1-1 1,5 6-1,-5-8-41,1 0 0,-1 0 1,1 0-1,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,9-1 1,62-1-3504,-34-8-523</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3835.11">753 754 6307,'1'-1'14188,"1"-2"-11556,7-5-2418,75-6-165,-46 8 16,-30 4 51,-9 2 84,-8 0-199,-18-1 18,0 1 0,0 2 0,1 1 0,-38 8 0,61-10-16,3 0 15,0 0 25,32-1-267,153-12 219,-161 10-794,-14 2-6822</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5839.69">185 906 8772,'0'0'11104,"0"-6"-9848,-2-14 493,-5 45 217,-5 22-1927,2-21-374,-13 44-221,17-21-8099,6-38-330</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6534.7">511 880 9236,'0'0'8564,"-1"-8"-7694,-5-35 637,7 41-1448,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0 0 0,0-1-1,0 1 1,3-1 0,0 0-45,0 0 0,0 1 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 1 0,9 1 0,-13 0-13,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,0 0 0,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 1-1,-3 37 54,3-40-55,-1 7 10,-1-1 0,-1 0-1,1 1 1,-1-1 0,0-1 0,0 1 0,-1 0-1,0-1 1,0 0 0,0 1 0,-1-2 0,1 1-1,-1 0 1,0-1 0,-8 5 0,5-3 17,1 1 1,-1 0 0,1 1 0,0-1-1,-7 12 1,14-18-16,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1-1,0-1 1,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1-1,0 1 1,1-1 0,-1 0 0,0 1 0,1-1 0,0 1 0,25 5 160,35-12-205,12-12-1741,-28 3-2793,-18 3-2293</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7339.86">834 772 8052,'0'0'7422,"-3"-2"-6686,1 1-377,-7-6-319,5-1 4038,44 2-3601,-33 5-462,21 2-31,-27 0 17,-1-1 0,1 1-1,0-1 1,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1-1,-1 1 1,1 0 0,-1 0-1,0 0 1,0-1-1,1 1 1,-1 0 0,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1 0-1,0 1 1,-1 3 21,-1 1-1,0-1 1,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0-1-1,-1 0 1,1 0 0,-9 6-1,7-5-28,0-1 1,1 1-1,-1 0 0,1 0 0,1 1 0,-1 0 0,1 0 0,-5 8 0,9-14-54,0 1 0,1 0-1,-1 0 1,0-1 0,0 1-1,0 0 1,1 0-1,-1-1 1,0 1 0,1 0-1,-1-1 1,1 1 0,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1 0,0 0-1,-1 1 1,1-1 0,0 1-1,-1-1 1,1 0-1,0 0 1,0 1 0,32 13-93,-17-8-98,-15-5 244,1 0-1,-1-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 1,0 0-1,-1 0 0,1 1 0,-1-1 0,1 3 0,-1-3 38,0 0 1,0 0 0,0 0-1,-1 0 1,1 1-1,0-1 1,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1 0-1,0 0 1,0-1-1,0 1 1,1 0-1,-1 0 1,-2 0 0,-1 2 66,-1-1 1,0 1-1,1-1 0,-1 0 1,0-1-1,0 1 1,-1-1-1,1 0 1,-10 1-1,12-2-697,-18 0 1376,15-1-3367</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7861.28">1062 715 8964,'0'0'9154,"2"-4"-7626,8-15-276,-8 14 826,-2 90-1862,0-84-231,1 0-1,-1 0 1,0-1 0,1 1 0,-1 0-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1 0,0 1 0,-1-1-1,1 1 1,0-1 0,0 1-1,-1-1 1,1 1 0,0-1 0,0 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,-1-1-1,1 1 1,0 0 0,1-1 0,35-14-679,-11-16 541,-10 13 324,-15 19-168,0 1 0,0-1-1,-1 0 1,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,-1 0 0,1 1 0,0-1 0,-1 2-1,-2 14 33,-1 1-1,-1-1 0,0 0 1,-1 0-1,-15 29 0,-4 12-7291,20-41-3481</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8221.38">1606 688 15879,'0'0'5902,"-7"5"-5820,6-4-80,-2 1 9,0-1-1,0 1 1,0 0-1,1 0 0,-1 1 1,1-1-1,-1 0 1,1 1-1,0 0 1,0-1-1,0 1 1,0 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 6 0,0 2 41,0 1-1,0-1 0,2 1 0,-1-1 1,1 1-1,1-1 0,0 0 0,0 0 1,1 1-1,1-2 0,5 13 0,-7-20 5,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 1-1,-1-1 1,1 0 0,-1 1-1,0-1 1,1 1 0,-2-1 0,1 0-1,-1 4 1,1-5-186,-1 0 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,0-1 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,-1-1 1,0 1-1,1 0 0,-1-1 0,0 1 1,1-1-1,-1 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,0 0 0,-2-1 0,-6-1-5607</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8390.38">1593 730 7555,'0'0'8644,"93"-51"-7699,-51 37-113,8 4-239,-8 0 255,-6 6-528,-15 1-272,-14 3-48,-18 7-9396</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink17.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:03:40.999"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">41 314 13142,'0'0'5034,"-1"16"-4327,0-4-548,0 1 43,0 0 0,0 1 1,-1-1-1,-1 0 1,0-1-1,-1 1 0,0 0 1,-10 18-1,14-31-175,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-1 1 1,1-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1-13 325,4-16-447,-1 23 92,1-1 0,-1 1 0,2 1 0,-1-1 1,1 0-1,0 1 0,0-1 0,0 1 1,1 0-1,0 1 0,0-1 0,0 1 0,0 0 1,1 0-1,-1 1 0,1 0 0,0-1 0,0 2 1,1-1-1,-1 1 0,0 0 0,1 0 1,9 0-1,-15 2-2,0 1 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1 0-1,0-1 1,-1 1-1,1 0 1,-1 0 0,1 0-1,-1-1 1,1 1 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,1 0 0,-1-1-1,0 1 1,0 0 0,-1 0-1,1 1 1,1 35 28,-1-30-26,-18 84 245,18-90-219,25-30 149,102-92-832,-120 122 414,-4 11 200,-2 15 129,-1-24-97,-1 12 62,1 25 21,0-39-68,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1-1 0,0 1 1,0 0-1,-1-1 0,1 1 0,0-1 1,0 1-1,-1-1 0,1 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 1,-1 0-1,3 0 0,3-1 5,1 0 0,-1 0 0,1-1 0,-1 0 0,0-1 0,1 1 0,-1-1 0,-1 0 0,1-1 1,0 1-1,-1-1 0,0 0 0,6-6 0,0 0 6,0 0 1,-1-1 0,0 0 0,-1-1 0,9-14-1,-20 34 51,1 0 0,1 0 0,0 0-1,0 0 1,2 13 0,-1 4 132,-1-13-126,0-9-29,-1-1 0,1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 1,0-1-1,1 4 0,-1-5-88,0 0 1,0 0 0,0 0-1,1 0 1,-1-1-1,0 1 1,0 0 0,1-1-1,-1 1 1,0-1 0,1 0-1,-1 1 1,1-1-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,4-1-1,-3 1-356,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,4-2 0,10-12-5097</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="158.62">587 241 9316,'0'0'6515,"-3"23"-6659,3-5-1200,0 2-2818,0-2-6019</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="610.64">749 336 8084,'0'0'12848,"-12"-2"-12071,4 0-641,5 1-99,0 0 0,-1 1 0,1-1 0,0 1-1,0-1 1,0 1 0,0 0 0,-1 0 0,1 0 0,0 1-1,0-1 1,0 1 0,-1-1 0,1 1 0,0 0 0,0 1 0,0-1-1,0 0 1,1 1 0,-1 0 0,-4 3 0,1-1 50,1 1 1,-1 0-1,1 0 1,0 0-1,1 1 1,-1 0-1,1 0 1,0 0-1,0 0 0,1 1 1,0-1-1,0 1 1,1 0-1,0 0 1,0 0-1,0 0 1,1 0-1,0 10 1,1-17-85,0 1 0,0-1 1,1 1-1,-1-1 0,0 0 0,1 1 1,-1-1-1,0 0 0,1 1 0,-1-1 1,0 0-1,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1-1 0,-1 1 1,2 0-1,19-7 161,-8-4-145,1-2 1,-1 0 0,-1 0-1,0-2 1,-1 1-1,-1-1 1,0-1 0,-1 0-1,-1 0 1,11-30 0,-18 93-140,-22 28 588,16-60-446,0 0 0,1-1 0,1 1 0,0 0 0,0 23 0,3-37-108,0 1 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,2 0 0,59-5-4435,-49 1 2883,0 0 0,0-1 0,-1 0-1,21-12 1,7-8-7510</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="824.12">1076 237 7603,'0'0'13660,"-7"5"-13078,-7 5-199,1 1 0,0 1 1,1 0-1,0 1 1,1 0-1,1 1 0,-14 22 1,-61 118 940,77-139-1276,0 1 0,2 0 0,-1 0 0,2 0 0,1 1 0,0 0 0,0 0 0,0 32 0,4-47-78,-1-1-1,2 1 1,-1 0-1,0-1 1,0 1-1,0 0 0,1 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,1-1 0,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,0 0-1,-1-1 1,4 2-1,2-1-365,0-1 1,0 1-1,0-1 0,0 0 0,0-1 1,0 1-1,9-3 0,36-13-5321</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1905.47">1300 341 8820,'0'0'7948,"0"-4"-7145,0-7-988,0-2 4344,-4 25-2171,-4 16-1942,5-20-317,0 1 0,1 0-1,0-1 1,1 1 0,-1 10-1,3-18-154,0-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,1-1 0,2 1-1369,12 0-3231</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2066.63">1300 341 4882,'67'-4'2177,"-67"-8"576,4 5 561,-4-1 4209,0 18-7443,0 7-15,0 1-65,-4 2-65,0 0-1855,1 1-2018,3-7-8340</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2294.7">1500 338 6739,'0'0'13094,"8"18"-12149,-8 12-385,-4 1-272,-3 1-160,-4 3-112,4-5-16,0-2-1169,4-3-2112,-1-5-2578</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2527.3">1486 330 13558,'0'0'8100,"82"-65"-7924,-54 65-144,1 0 0,6 2-16,-3 8-32,-4 6-112,-3 5-1489,-7 1-1200,-8-2-1361,-10 0-8516</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2742.85">1417 617 12005,'0'0'8692,"28"0"-8627,11-8-65,7 0-881,0-4-1824,4 0-2914</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3146.65">1806 427 12230,'0'0'5613,"-2"12"-5050,-2 1-436,-1 3 210,1 1 0,0-1 0,-1 31 0,5-47-238,32-19 923,-5-7-868,-20 17 49,1 2 0,0-1 0,0 1-1,12-7 1,-19 16-109,-1-1 1,1 1-1,0-1 0,0 1 0,0 0 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 0,0 0 1,0 3-1,4 14-173,-3-18-144,0 1-1,1-1 1,-1 0 0,1 1 0,0-1 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,3 0 0,40-1-7155,-41 0 6334,18-2-3750</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3685.09">2068 470 5042,'0'0'11827,"-6"-7"-10784,-17-20-432,22 27-588,1-1-1,-1 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,1-1 1,-1 0-1,0 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0 0 0,1-1 1,-1 1-1,1-1 0,-1 1 1,1 0-1,-1 0 1,1-1-1,-1 1 0,1 0 1,0 0-1,-1 0 0,1 0 1,-16 32 525,15-31-541,1 0 0,-1 0 0,0 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 1,0 0-1,0 2 0,0-3-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 0 0,0 0-1,2-1 1,3 0 8,0 0 1,0 0-1,0-1 0,-1 0 0,1 0 0,-1-1 0,1 0 1,-1 0-1,0 0 0,0 0 0,6-6 0,0-3-68,-1-2 1,0 1-1,-1-1 0,-1-1 0,0 1 0,-1-1 0,0-1 0,-1 0 0,-1 1 1,5-30-1,-17 106 195,-3 48 487,11-107-628,-1-1 1,1 0-1,-1 0 1,1 1-1,0-1 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 0,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,1-1-1,47-5-13,-44 3-58,0 1-1,-1-1 1,1 0-1,-1 0 1,10-8-1,-13 10 28,0-1-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 0,0 0 1,1 0-1,-1-1 1,0 1-1,0 0 1,0-1-1,0 1 0,0-5 1,-1 7 168,-4 27 49,2-21-389,-10 40 760,9-14-4288,3-28-1107</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3854.8">2416 262 12854,'0'0'3586,"0"40"-8389,0-24-1183</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4245.87">2508 391 5635,'0'0'13379,"-5"-6"-12248,3 4-1104,2 1 2,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 2 0,-2 2 3,-1 0-1,1 0 1,0 1-1,0 0 1,0 0-1,1 0 1,0 0 0,0 0-1,1 1 1,-1-1-1,2 1 1,-1 0-1,1-1 1,0 1-1,0 0 1,0 14-1,2-21-26,-1 1 0,1-1 0,-1 1-1,1-1 1,0 1 0,-1-1-1,1 1 1,0-1 0,-1 1 0,1-1-1,0 0 1,-1 1 0,1-1-1,0 0 1,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1-1,0 0 1,-1 0 0,1 0-1,0-1 1,-1 1 0,1-1 0,0 1-1,0-1 1,30-13 68,-18 1-55,-11 11-12,-1 0 0,1 0 0,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 0,0 1 0,0-1 1,0 1-1,0 0 0,1 0 0,3-2 0,-6 62 51,0-34-5396</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4433.91">2615 341 12710,'0'0'6595,"0"30"-6579,-4-18-32,1-2-208,3-2-1249,0-1-1696</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4581.58">2628 341 10501,'7'14'8804,"-7"-12"-8468,0 10-272,0 6-64,-7 3 16,7-3-16,0 0-1056,0-4-1666,0-2-6082</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4871.67">2752 241 11125,'0'0'8092,"8"7"-7033,0 0-851,-1 1 1,0 0-1,0 1 0,-1-1 1,0 1-1,0 0 0,-1 1 1,0-1-1,5 15 1,-4-6-43,0 0 0,-1 1 0,4 33 0,-8-47-156,-1 0 0,1 1 0,-1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1-1,0-1 1,-1 1 0,1 0 0,-1-1 0,0 1 0,0-1 0,-6 7 0,-8 5-294,-2 0-1,-30 20 0,-13 2-4941,26-21-1694</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5997.47">2862 458 9508,'0'0'10474,"0"0"-10444,0 0-1,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,-1-1 1,1 1-1,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 0,0 0 0,-1 0 0,0 0 0,-21 1 278,19 0-256,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,-2-2 0,4 1-39,-1 0 1,1 0 0,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0-1 0,0 1-1,1-1 1,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1-1,-1 0 1,1 1 0,0-4 0,0-47 86,0 51-98,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 1-1,0-1 1,0 0 0,0 0 0,-1 1-1,1-1 1,0 1 0,0-1-1,0 1 1,1-1 0,-1 1 0,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,2 0 0,-2 1 1,0-1 1,0 1-1,1 0 1,-1 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,-1 1 1,2-1 14,-1 0 1,0-1 0,-1 1 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1-1-1,1 1 1,-1 0 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1-1,-1 1 1,1-1 0,0 1 0,-3 1-1,3-2-6,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1-1 0,1 1-12,-1-1-1,0 0 1,0 0 0,1 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,-1 1 0,1-1-1,0 1 1,0-1 0,0 1-1,1-1 1,-1 1-1,0-1 1,0 1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,2 0 0,-2 1-21,1-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 1-1,0-1 1,0 1-1,-1 0 1,1 0-1,4 2 1,-6-2 15,1 0 0,-1 0-1,0 0 1,0 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1 0,-1 0-1,1-1 1,0 1 0,-1-1 0,1 1 0,-1 0-1,0-1 1,0 1 0,1 0 0,-1 0 0,0-1-1,-1 3 1,-2-3 43,1 0 1,-1 0-1,0 0 0,0-1 0,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0-1 1,0 0-1,0 1 0,0-1 0,-4-2 0,6 2-38,0 0-1,0-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,1 0-1,0 0 1,-1 0-1,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,1-1-1,-1 0 1,0 0-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1 0-1,0-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,0 1 1,-1-1-1,1 0 1,0 1-1,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0-1,2 0 1,-3 1-14,1-1 1,-1 1-1,1 0 1,-1-1-1,1 1 1,-1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 1 0,0-1-1,-1 0 1,1 1-1,0-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1 0,0 3-1,4 44-14,-4-45 28,0 9 20,-1 0-1,0 0 0,-1 0 1,0 0-1,-1-1 0,0 1 1,-1-1-1,-1 0 0,1 0 1,-2 0-1,0-1 0,-1 1 1,0-1-1,0-1 0,-10 11 1,-38 42-302,15-25-2783,11-14-2173</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8872.62">3199 353 5587,'0'0'10967,"-1"-6"-9905,-1 2-711,1 0-1,0 0 1,0-1 0,0 1-1,0-1 1,1 1-1,0-7 1,0 9-259,1 1 1,-1-1-1,1 0 1,-1 0-1,1 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,1 0 0,4-1 1,1 0 0,-1 1-1,0-1 1,0 1 0,1 1-1,14 0 1,-18 0-67,-3 0-21,0 1-1,0 0 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 1,0 1-1,1-1 0,-1 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,-1 0-1,1 3 0,-7 40 128,0-33-105,-1 1 0,0-1 0,-1-1 0,0 1 0,-1-1 0,0-1 0,0 0 0,-1-1 0,-21 14 0,35-23-92,0 1 0,0-1 1,-1 1-1,1 0 0,0 0 1,0 0-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 1 0,4 2 1,-5-3 49,1 0-1,-1 1 1,1-1 0,-1 1 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 1 0,-1-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0-1,-1 0 1,1 4 0,0-5 27,-1 1 1,0-1-1,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,0 1 0,1-1 1,-1 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-4 2 1,1-2 76,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,-7 1 0,-6 0-181,-9 1 185,10-1-6222</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9597.66">3482 514 8052,'0'0'9657,"-45"20"-7725,45-19-1912,-1-1 0,1 0 0,0 0 0,0 0 0,-1 0 1,1 1-1,0-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 1,0 0-1,0-1 0,-1 1 0,7-12 16,-6 12-41,0 1 0,0-1 0,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 2 34,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,-1 1 0,-7 0 59,9-1-88,0 1 0,-1-1 1,1 1-1,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 1,0 1-1,0-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 1,0 1-1,1-1 0,-1 0 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-2 1,0 1-8,-1-1 0,1 1 0,-1-1 1,1 1-1,-1 0 0,1-1 1,0 1-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,2 0-1,-2 0-9,0 1 1,-1 0-1,1 0 0,0 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 1,-1 1-1,1-1 0,-1 1 1,1-1-1,0 1 0,-1-1 1,1 1-1,-1-1 0,1 1 1,-1-1-1,1 1 0,-1 0 1,1 2 5,0-1 0,0 1 1,0-1-1,-1 1 0,1-1 1,-1 1-1,0-1 0,1 1 1,-1 0-1,-1 2 0,1 1 18,-1 0 0,1 0 0,-1-1 0,-1 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,-4 4 0,-7 6-150,-1-1 1,-20 18 0,5-10-3989,17-15-1793</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10531.14">3627 366 11461,'0'0'9986,"21"-18"-7934,-17 16-2041,-1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1-1 0,-1 1 1,0-1-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,2-6 0,-1-4 34,0 0 0,0 0 1,-1-25-1,-1 35-28,0 2 1,1 7-53,0 1 0,-1-1-1,0 0 1,0 0 0,0 1-1,0-1 1,-3 10 0,2-10 24,-5 42 102,-2 16 82,-1 66 0,4-129-116,-1-1-1,1 1 0,0-1 1,-1 0-1,1 0 0,0-1 1,0 1-1,-6-3 0,-3 3-51,12 0-5,-1 0 0,1 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,0-1 1,-1 0-1,1 1 1,-3-3-1,4 3-52,41 0-163,2-3-1743,-14-2-3390,-7-1-1993</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11105.36">3823 17 10789,'0'0'10167,"-8"-17"-8627,11 18-1514,0 0 1,0 0 0,0-1 0,0 2 0,0-1 0,-1 0-1,1 0 1,0 1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 1 0,2 3 0,31 55 113,-31-54-91,7 14-57,-2 1 0,-1 1 0,0-1 0,-2 1 0,0 0 0,-2 0 0,0 1 0,-2 0 0,-1-1 0,0 1 0,-2 0 0,-1 0 0,-1-1 0,0 1 0,-2-1 0,-1 0 0,-1 0 0,-1-1 0,-1 0 0,-17 32 0,-64 94-2401,21-57-3066,26-43-1152</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink18.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:41:25.521"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 47 6563,'0'0'12198,"14"-17"-6158,-21 177-5934,7-159 180,0-37-14,1 26-273,0 0-1,1-1 1,0 1-1,0 0 1,6-12 0,-5 11 5,1 0 0,-1 1 0,-1-1 0,0-1 0,0-14 0,-2 25-23,0 28-605,-10 61 648,10-87 230,0-35 116,0-31-2344</inkml:trace>
-</inkml:ink>
-</file>
-
-<file path=xl/ink/ink19.xml><?xml version="1.0" encoding="utf-8"?>
-<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
-  <inkml:definitions>
-    <inkml:context xml:id="ctx0">
-      <inkml:inkSource xml:id="inkSrc0">
-        <inkml:traceFormat>
-          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
-          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
-        </inkml:traceFormat>
-        <inkml:channelProperties>
-          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
-          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
-        </inkml:channelProperties>
-      </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:41:25.522"/>
-    </inkml:context>
-    <inkml:brush xml:id="br0">
-      <inkml:brushProperty name="width" value="0.035" units="cm"/>
-      <inkml:brushProperty name="height" value="0.035" units="cm"/>
-      <inkml:brushProperty name="color" value="#004F8B"/>
-    </inkml:brush>
-  </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">3 82 21582,'-3'43'0,"31"-125"0,-24 39 0,-33 125 0</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -17637,6 +18052,185 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:03:15.421"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">19 140 13654,'0'0'3538,"54"0"-3122,-37-2-272,5 0-64,-5 2-64,-3 0-16,1 0-256,-8 0-640,0 2-721,-7 4-1489,0 4-1135</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="205.23">0 259 10885,'0'0'7507,"50"-6"-6994,-22-2-257,4 0-176,-3 2-64,-4 0-16,-4 0-448,-3-2-913,-4 2-304,-7-3-1760,3-1-1442</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="650.2">213 54 6931,'0'0'12155,"-8"-10"-10458,-26-26-337,22 29 788,8 16-1870,7 17-476,0-19 189,1 0-1,0-1 1,0 1-1,0-1 1,0 0-1,1 0 1,0 0-1,1-1 1,-1 1-1,1-1 1,0 0 0,0-1-1,1 0 1,-1 0-1,1 0 1,9 3-1,-2-1-165,-1 0-1,1-1 0,0-1 1,0 0-1,1-1 0,-1-1 1,24 2-1,-17-4 107,-29 15 95,-80 63 286,56-52-119,-50 53-1,29-16-1305</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1630.16">803 101 6227,'0'0'10471,"0"-6"-9267,1-10-1063,0-7 4563,-12 43-2872,-47 144-1600,57-193 522,0 20-757,0 0 0,1 0-1,0 0 1,1 1-1,1-12 1,-1 15-7,0 1 1,0-1-1,1 1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,1 0 1,3-3-1,-5 6-1,-1 0 0,1 1 0,0-1 0,0 1-1,0-1 1,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,2 1 1,-1 0-2,1-1 1,-1 2-1,1-1 0,-1 0 1,1 0-1,-1 1 0,0-1 0,0 1 1,4 4-1,6 4 32,0 1 0,-1 1 0,-1 0 0,0 1 0,-1-1 0,12 23 0,-14-27-1255,-6-8 830,-1 0 0,1 1 0,-1-1-1,1 0 1,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,6-9-6987</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1878.71">993 51 6243,'0'0'9938,"1"-4"-9357,1-11 65,-3 39 895,-8 44 258,-7-20-1522,-2 9-303,13-18-3103,8-37-1016,12-4 128,-1-8-297</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2132.15">1032 153 3570,'0'0'5941,"2"-12"-3836,2-1-1214,4-14-89,-8 0 4770,2 44-4907,-1 0 0,-1 0 0,0 1-1,-4 21 1,2-23-827,-2-1-1,0-1 0,0 1 0,-1-1 0,-9 18 0,9-18-2823</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2388.58">1033 133 2881,'0'0'15189,"3"-9"-14253,11-25-352,-13 33-564,0 0 0,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,1 1-1,-1-1 1,0 0 0,1 1-1,-1 0 1,0-1 0,1 1-1,-1 0 1,1-1 0,-1 1-1,0 0 1,1 0 0,-1 0-1,3 1 1,27 4 305,-25-2-271,0 0-1,-1 0 1,1 1-1,-1-1 1,1 1-1,-1 1 1,-1-1-1,1 1 1,-1-1-1,6 8 1,-7-9 53,-1 1-1,1 0 1,-1-1 0,1 1 0,-1 0-1,0 0 1,0 0 0,-1 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,-1 1 0,1-1-1,-1 7 1,-2-8-62,1-1 1,-1 0-1,0 1 0,0-1 0,0 0 1,-1 0-1,1 0 0,0-1 0,-1 1 0,0 0 1,1-1-1,-1 0 0,0 1 0,1-1 1,-1 0-1,0 0 0,0-1 0,-3 1 1,-6 4 20,-73 27-324,27-13-2779,11-8-2976</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink21.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:03:31.197"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">186 202 11909,'0'0'10282,"0"-5"-9510,1-29 1321,-1 30-409,-1 27-1571,1-19-228,-4 27 263,-2 1 0,-1-1 0,-16 48 0,-10 38-2413,25-37-5128,8-59 1823</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="242.69">66 235 13078,'-3'-15'694,"1"-2"-282,-3-11 1271,1-1 0,1 1 0,3-54 0,0 80-1652,1 0 0,0 0 1,0 0-1,-1 1 0,1-1 0,1 0 0,-1 1 0,0-1 0,0 1 1,1-1-1,-1 1 0,0 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 1 0,0 0 1,4-1-1,57-3-106,-56 5 102,-2-1-92,1 0 0,-1 0 0,-1 1 0,1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 1 0,5 5 0,-4-3-346,-1 0 1,0-1-1,0 1 0,-1 1 0,0-1 0,0 1 1,0-1-1,-1 1 0,0 0 0,0 0 1,0 0-1,0 9 0,-1 20-4287</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="421.47">1 523 9941,'0'0'5938,"67"4"-5890,-24-4-48,3 0-832,0-6-3730</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="870">398 366 12054,'0'0'5052,"0"9"-4323,0 169 2782,25-201-3127,-2-3-322,-11 13-32,0-2 0,14-21 0,-21 36-277,0 12 166,3 19 114,-7-27-42,0 2 20,1-1 1,-1 1-1,1-1 1,0 0-1,0 0 1,1 0-1,0 0 1,0-1-1,0 1 0,0-1 1,0 1-1,9 7 1,-8-10-77,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,1-1 0,-1 0 0,1 1 1,-1-2-1,1 1 0,-1 0 0,7-3 0,-3 2-579,-1-1 0,1 0-1,-1 0 1,0-1 0,0 0 0,8-5 0,8-8-4233</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1794.6">828 434 3986,'0'0'12910,"-3"-8"-11939,2 6-961,1 0 52,-1 0 1,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1-1,0 1 1,0 0 0,0 0 0,0-1 0,0 1 0,0 1 0,0-1 0,0 0 0,-1 0-1,1 1 1,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,-2 0-1,2 1-36,-1-1-1,1 1 0,-1 0 0,1 0 0,0 0 1,0 1-1,0-1 0,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,1 0 0,-1 0 0,1 1 1,-1-1-1,1 1 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,-1 7 1,-1-1-5,1-1 0,-1 1 0,2 0 0,0 0 0,0 0 0,0 0 0,1 0 0,0 0 0,3 12 1,-3-20-18,1 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,-1 0 1,1 0-1,0-1 0,0 1 0,-1 0 1,1-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 1,1 0-1,34-17 47,-19 2-262,-2-1 0,0 0 0,-1-1 0,-1-1 0,-1 0 0,-1 0 0,0-1 0,-1-1 0,-2 1 0,0-2-1,-1 1 1,-1-1 0,-1 0 0,-1 0 0,0-1 0,-1-30 0,-3 53 242,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1-1-1,0 1 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,-1 1 0,-9 6 376,-7 13-357,9-3 29,0 1-1,2 0 0,0 0 1,1 1-1,0-1 1,2 1-1,0 0 0,2 0 1,0 1-1,0-1 1,2 0-1,4 23 0,-5-39-70,0-1-1,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,0-1 0,1 1 0,0 0 0,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,1-1 0,2 2 0,-1-2 10,-1-1-1,1 1 0,0 0 0,-1-1 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0-1 1,0 1-1,0 0 0,3-6 0,3-4-42,-1 0-1,-1-1 1,0-1 0,-1 1-1,0-1 1,-1 0-1,0-1 1,-2 1-1,1-1 1,1-22 0,-12 99 201,5-49-110,0 0-1,1 0 1,0 0-1,1 0 1,3 26-1,-2-37-86,-1 0-1,1-1 0,0 1 1,0 0-1,-1-1 0,1 1 1,0 0-1,0-1 0,1 1 1,-1-1-1,0 0 0,0 1 1,1-1-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,0 0 0,0-1 1,-1 1-1,1 0 0,0-1 1,2 1-1,0 0-729,1-1 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 0-1,-1-1 1,1 0-1,5-1 0,16-11-11555</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1926.27">1277 156 14663,'0'0'1793,"14"48"-12006</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2359.55">1397 279 10229,'0'0'10575,"-14"-4"-10137,-49-7-324,61 11-113,-1 0 0,1 1-1,0-1 1,-1 0-1,1 1 1,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1-1,1 1 1,-1 0-1,1-1 1,-1 1 0,1 0-1,-2 3 1,-18 46 25,17-40 1,2-3-36,0 0-1,0 0 0,1 0 1,0 1-1,1-1 1,0 9-1,0-10-6,1-7 15,-1 1 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,0-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,2 1 0,33-10 3,-25 0-2,1 0 0,-1 0 0,-1 0 0,0-2 0,0 1 1,-1-1-1,-1 0 0,9-19 0,1 1 7,-17 30-11,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1-1 0,-1 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1-1,0-1 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0-1,5 16-65,1 24 162,-5-36-67,-1 2 12,1 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,0 0 1,1-1-1,-1 1 0,1-1 1,1 1-1,-1-1 1,5 6-1,-5-8-41,1 0 0,-1 0 1,1 0-1,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,0-1 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,9-1 1,62-1-3504,-34-8-523</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3835.11">753 754 6307,'1'-1'14188,"1"-2"-11556,7-5-2418,75-6-165,-46 8 16,-30 4 51,-9 2 84,-8 0-199,-18-1 18,0 1 0,0 2 0,1 1 0,-38 8 0,61-10-16,3 0 15,0 0 25,32-1-267,153-12 219,-161 10-794,-14 2-6822</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5839.69">185 906 8772,'0'0'11104,"0"-6"-9848,-2-14 493,-5 45 217,-5 22-1927,2-21-374,-13 44-221,17-21-8099,6-38-330</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6534.7">511 880 9236,'0'0'8564,"-1"-8"-7694,-5-35 637,7 41-1448,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 0,0 1 0,0 0 0,0-1-1,0 1 1,3-1 0,0 0-45,0 0 0,0 1 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0 1 0,9 1 0,-13 0-13,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,-1-1-1,1 1 1,0 0 0,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 1-1,-3 37 54,3-40-55,-1 7 10,-1-1 0,-1 0-1,1 1 1,-1-1 0,0-1 0,0 1 0,-1 0-1,0-1 1,0 0 0,0 1 0,-1-2 0,1 1-1,-1 0 1,0-1 0,-8 5 0,5-3 17,1 1 1,-1 0 0,1 1 0,0-1-1,-7 12 1,14-18-16,-1-1 0,1 0 0,0 1 0,-1-1 0,1 1-1,0-1 1,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1-1,1-1 1,-1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1-1,0 1 1,1-1 0,-1 0 0,0 1 0,1-1 0,0 1 0,25 5 160,35-12-205,12-12-1741,-28 3-2793,-18 3-2293</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7339.86">834 772 8052,'0'0'7422,"-3"-2"-6686,1 1-377,-7-6-319,5-1 4038,44 2-3601,-33 5-462,21 2-31,-27 0 17,-1-1 0,1 1-1,0-1 1,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1-1,-1 1 1,1 0 0,-1 0-1,0 0 1,0-1-1,1 1 1,-1 0 0,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1 0-1,0 1 1,-1 3 21,-1 1-1,0-1 1,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0-1-1,-1 0 1,1 0 0,-9 6-1,7-5-28,0-1 1,1 1-1,-1 0 0,1 0 0,1 1 0,-1 0 0,1 0 0,-5 8 0,9-14-54,0 1 0,1 0-1,-1 0 1,0-1 0,0 1-1,0 0 1,1 0-1,-1-1 1,0 1 0,1 0-1,-1-1 1,1 1 0,-1-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1-1-1,-1 1 1,1-1 0,0 0-1,-1 1 1,1-1 0,0 1-1,-1-1 1,1 0-1,0 0 1,0 1 0,32 13-93,-17-8-98,-15-5 244,1 0-1,-1-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 1,0 0-1,-1 0 0,1 1 0,-1-1 0,1 3 0,-1-3 38,0 0 1,0 0 0,0 0-1,-1 0 1,1 1-1,0-1 1,-1 0-1,1 0 1,-1 0-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1 0-1,0 0 1,0-1-1,0 1 1,1 0-1,-1 0 1,-2 0 0,-1 2 66,-1-1 1,0 1-1,1-1 0,-1 0 1,0-1-1,0 1 1,-1-1-1,1 0 1,-10 1-1,12-2-697,-18 0 1376,15-1-3367</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7861.28">1062 715 8964,'0'0'9154,"2"-4"-7626,8-15-276,-8 14 826,-2 90-1862,0-84-231,1 0-1,-1 0 1,0-1 0,1 1 0,-1 0-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1 0,0 1 0,-1-1-1,1 1 1,0-1 0,0 1-1,-1-1 1,1 1 0,0-1 0,0 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,-1-1-1,1 1 1,0 0 0,1-1 0,35-14-679,-11-16 541,-10 13 324,-15 19-168,0 1 0,0-1-1,-1 0 1,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 1 0,0-1 0,0 0-1,0 1 1,0-1 0,-1 0 0,1 1 0,0-1 0,-1 2-1,-2 14 33,-1 1-1,-1-1 0,0 0 1,-1 0-1,-15 29 0,-4 12-7291,20-41-3481</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8221.37">1606 688 15879,'0'0'5902,"-7"5"-5820,6-4-80,-2 1 9,0-1-1,0 1 1,0 0-1,1 0 0,-1 1 1,1-1-1,-1 0 1,1 1-1,0 0 1,0-1-1,0 1 1,0 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 6 0,0 2 41,0 1-1,0-1 0,2 1 0,-1-1 1,1 1-1,1-1 0,0 0 0,0 0 1,1 1-1,1-2 0,5 13 0,-7-20 5,-1 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 1-1,-1-1 1,1 0 0,-1 1-1,0-1 1,1 1 0,-2-1 0,1 0-1,-1 4 1,1-5-186,-1 0 0,0-1 1,0 0-1,0 1 0,0-1 0,0 1 0,0-1 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,-1-1 1,0 1-1,1 0 0,-1-1 0,0 1 1,1-1-1,-1 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,0 0 0,-2-1 0,-6-1-5607</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8390.37">1593 730 7555,'0'0'8644,"93"-51"-7699,-51 37-113,8 4-239,-8 0 255,-6 6-528,-15 1-272,-14 3-48,-18 7-9396</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink22.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:03:40.999"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">41 314 13142,'0'0'5034,"-1"16"-4327,0-4-548,0 1 43,0 0 0,0 1 1,-1-1-1,-1 0 1,0-1-1,-1 1 0,0 0 1,-10 18-1,14-31-175,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-1 1 1,1-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1-13 325,4-16-447,-1 23 92,1-1 0,-1 1 0,2 1 0,-1-1 1,1 0-1,0 1 0,0-1 0,0 1 1,1 0-1,0 1 0,0-1 0,0 1 0,0 0 1,1 0-1,-1 1 0,1 0 0,0-1 0,0 2 1,1-1-1,-1 1 0,0 0 0,1 0 1,9 0-1,-15 2-2,0 1 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1 0-1,0-1 1,-1 1-1,1 0 1,-1 0 0,1 0-1,-1-1 1,1 1 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,1 0 0,-1-1-1,0 1 1,0 0 0,-1 0-1,1 1 1,1 35 28,-1-30-26,-18 84 245,18-90-219,25-30 149,102-92-832,-120 122 414,-4 11 200,-2 15 129,-1-24-97,-1 12 62,1 25 21,0-39-68,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,0 0 0,1 0 1,-1-1-1,1 1 0,-1 0 0,1 0 0,-1-1 1,1 1-1,-1 0 0,1-1 0,0 1 1,0 0-1,-1-1 0,1 1 0,0-1 1,0 1-1,-1-1 0,1 0 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 1,-1 0-1,3 0 0,3-1 5,1 0 0,-1 0 0,1-1 0,-1 0 0,0-1 0,1 1 0,-1-1 0,-1 0 0,1-1 1,0 1-1,-1-1 0,0 0 0,6-6 0,0 0 6,0 0 1,-1-1 0,0 0 0,-1-1 0,9-14-1,-20 34 51,1 0 0,1 0 0,0 0-1,0 0 1,2 13 0,-1 4 132,-1-13-126,0-9-29,-1-1 0,1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 1 1,0-1-1,1 4 0,-1-5-88,0 0 1,0 0 0,0 0-1,1 0 1,-1-1-1,0 1 1,0 0 0,1-1-1,-1 1 1,0-1 0,1 0-1,-1 1 1,1-1-1,-1 0 1,0 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,0 0 1,4-1-1,-3 1-356,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,4-2 0,10-12-5097</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="158.62">587 241 9316,'0'0'6515,"-3"23"-6659,3-5-1200,0 2-2818,0-2-6019</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="610.64">749 336 8084,'0'0'12848,"-12"-2"-12071,4 0-641,5 1-99,0 0 0,-1 1 0,1-1 0,0 1-1,0-1 1,0 1 0,0 0 0,-1 0 0,1 0 0,0 1-1,0-1 1,0 1 0,-1-1 0,1 1 0,0 0 0,0 1 0,0-1-1,0 0 1,1 1 0,-1 0 0,-4 3 0,1-1 50,1 1 1,-1 0-1,1 0 1,0 0-1,1 1 1,-1 0-1,1 0 1,0 0-1,0 0 0,1 1 1,0-1-1,0 1 1,1 0-1,0 0 1,0 0-1,0 0 1,1 0-1,0 10 1,1-17-85,0 1 0,0-1 1,1 1-1,-1-1 0,0 0 0,1 1 1,-1-1-1,0 0 0,1 1 0,-1-1 1,0 0-1,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1-1 0,-1 1 1,2 0-1,19-7 161,-8-4-145,1-2 1,-1 0 0,-1 0-1,0-2 1,-1 1-1,-1-1 1,0-1 0,-1 0-1,-1 0 1,11-30 0,-18 93-140,-22 28 588,16-60-446,0 0 0,1-1 0,1 1 0,0 0 0,0 23 0,3-37-108,0 1 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0-1,-1 1 1,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,2 0 0,59-5-4435,-49 1 2883,0 0 0,0-1 0,-1 0-1,21-12 1,7-8-7510</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="824.12">1076 237 7603,'0'0'13660,"-7"5"-13078,-7 5-199,1 1 0,0 1 1,1 0-1,0 1 1,1 0-1,1 1 0,-14 22 1,-61 118 940,77-139-1276,0 1 0,2 0 0,-1 0 0,2 0 0,1 1 0,0 0 0,0 0 0,0 32 0,4-47-78,-1-1-1,2 1 1,-1 0-1,0-1 1,0 1-1,0 0 0,1 0 1,-1-1-1,1 1 1,-1 0-1,1-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 1-1,1-1 0,-1 0 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1-1-1,1 1 1,0 0-1,-1-1 1,4 2-1,2-1-365,0-1 1,0 1-1,0-1 0,0 0 0,0-1 1,0 1-1,9-3 0,36-13-5321</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1905.47">1300 341 8820,'0'0'7948,"0"-4"-7145,0-7-988,0-2 4344,-4 25-2171,-4 16-1942,5-20-317,0 1 0,1 0-1,0-1 1,1 1 0,-1 10-1,3-18-154,0-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,1-1 0,2 1-1369,12 0-3231</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2066.63">1300 341 4882,'67'-4'2177,"-67"-8"576,4 5 561,-4-1 4209,0 18-7443,0 7-15,0 1-65,-4 2-65,0 0-1855,1 1-2018,3-7-8340</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2294.69">1500 338 6739,'0'0'13094,"8"18"-12149,-8 12-385,-4 1-272,-3 1-160,-4 3-112,4-5-16,0-2-1169,4-3-2112,-1-5-2578</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2527.3">1486 330 13558,'0'0'8100,"82"-65"-7924,-54 65-144,1 0 0,6 2-16,-3 8-32,-4 6-112,-3 5-1489,-7 1-1200,-8-2-1361,-10 0-8516</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2742.85">1417 617 12005,'0'0'8692,"28"0"-8627,11-8-65,7 0-881,0-4-1824,4 0-2914</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3146.65">1806 427 12230,'0'0'5613,"-2"12"-5050,-2 1-436,-1 3 210,1 1 0,0-1 0,-1 31 0,5-47-238,32-19 923,-5-7-868,-20 17 49,1 2 0,0-1 0,0 1-1,12-7 1,-19 16-109,-1-1 1,1 1-1,0-1 0,0 1 0,0 0 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 0,0 0 1,0 3-1,4 14-173,-3-18-144,0 1-1,1-1 1,-1 0 0,1 1 0,0-1 0,-1 0-1,1 0 1,0 0 0,0 0 0,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,3 0 0,40-1-7155,-41 0 6334,18-2-3750</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3685.09">2068 470 5042,'0'0'11827,"-6"-7"-10784,-17-20-432,22 27-588,1-1-1,-1 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,1-1 1,-1 0-1,0 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 1 0,1-1 1,-1 1-1,0 0 0,1-1 1,-1 1-1,1-1 0,-1 1 1,1 0-1,-1 0 1,1-1-1,-1 1 0,1 0 1,0 0-1,-1 0 0,1 0 1,-16 32 525,15-31-541,1 0 0,-1 0 0,0 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 1,0 0-1,0 2 0,0-3-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 0 0,1 1-1,-1-1 1,0 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,0 0 0,0 0-1,2-1 1,3 0 8,0 0 1,0 0-1,0-1 0,-1 0 0,1 0 0,-1-1 0,1 0 1,-1 0-1,0 0 0,0 0 0,6-6 0,0-3-68,-1-2 1,0 1-1,-1-1 0,-1-1 0,0 1 0,-1-1 0,0-1 0,-1 0 0,-1 1 1,5-30-1,-17 106 195,-3 48 487,11-107-628,-1-1 1,1 0-1,-1 0 1,1 1-1,0-1 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 1,0-1-1,1 1 1,-1-1-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 0,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,1 0 1,1-1-1,47-5-13,-44 3-58,0 1-1,-1-1 1,1 0-1,-1 0 1,10-8-1,-13 10 28,0-1-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,0 0-1,-1 0 0,0 0 1,1 0-1,-1-1 1,0 1-1,0 0 1,0-1-1,0 1 0,0-5 1,-1 7 168,-4 27 49,2-21-389,-10 40 760,9-14-4288,3-28-1107</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3854.8">2416 262 12854,'0'0'3586,"0"40"-8389,0-24-1183</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4245.87">2508 391 5635,'0'0'13379,"-5"-6"-12248,3 4-1104,2 1 2,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 2 0,-2 2 3,-1 0-1,1 0 1,0 1-1,0 0 1,0 0-1,1 0 1,0 0 0,0 0-1,1 1 1,-1-1-1,2 1 1,-1 0-1,1-1 1,0 1-1,0 0 1,0 14-1,2-21-26,-1 1 0,1-1 0,-1 1-1,1-1 1,0 1 0,-1-1-1,1 1 1,0-1 0,-1 1 0,1-1-1,0 0 1,-1 1 0,1-1-1,0 0 1,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1-1,0 0 1,-1 0 0,1 0-1,0-1 1,-1 1 0,1-1 0,0 1-1,0-1 1,30-13 68,-18 1-55,-11 11-12,-1 0 0,1 0 0,-1 0 0,1 0 1,0 1-1,-1-1 0,1 0 0,0 1 0,0-1 1,0 1-1,0 0 0,1 0 0,3-2 0,-6 62 51,0-34-5396</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4433.91">2615 341 12710,'0'0'6595,"0"30"-6579,-4-18-32,1-2-208,3-2-1249,0-1-1696</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4581.58">2628 341 10501,'7'14'8804,"-7"-12"-8468,0 10-272,0 6-64,-7 3 16,7-3-16,0 0-1056,0-4-1666,0-2-6082</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4871.67">2752 241 11125,'0'0'8092,"8"7"-7033,0 0-851,-1 1 1,0 0-1,0 1 0,-1-1 1,0 1-1,0 0 0,-1 1 1,0-1-1,5 15 1,-4-6-43,0 0 0,-1 1 0,4 33 0,-8-47-156,-1 0 0,1 1 0,-1-1 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1-1,0-1 1,-1 1 0,1 0 0,-1-1 0,0 1 0,0-1 0,-6 7 0,-8 5-294,-2 0-1,-30 20 0,-13 2-4941,26-21-1694</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5997.46">2862 458 9508,'0'0'10474,"0"0"-10444,0 0-1,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,-1-1 1,1 1-1,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 0,0 0 0,-1 0 0,0 0 0,-21 1 278,19 0-256,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,-2-2 0,4 1-39,-1 0 1,1 0 0,0 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0-1 0,0 1 0,0-1 0,0 1-1,1-1 1,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1-1,-1 0 1,1 1 0,0-4 0,0-47 86,0 51-98,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,0 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0 0,0 1-1,0-1 1,0 0 0,0 0 0,-1 1-1,1-1 1,0 1 0,0-1-1,0 1 1,1-1 0,-1 1 0,0-1-1,0 1 1,0 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,2 0 0,-2 1 1,0-1 1,0 1-1,1 0 1,-1 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 1 1,0-1-1,-1 0 1,1 0-1,0 0 1,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,-1 1 1,2-1 14,-1 0 1,0-1 0,-1 1 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1-1-1,1 1 1,-1 0 0,0 0 0,1-1-1,-1 1 1,0 0 0,0-1-1,-1 1 1,1-1 0,0 1 0,-3 1-1,3-2-6,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1-1 0,1 1-12,-1-1-1,0 0 1,0 0 0,1 0-1,-1 1 1,1-1 0,0 0-1,0 0 1,-1 1 0,1-1-1,0 1 1,0-1 0,0 1-1,1-1 1,-1 1-1,0-1 1,0 1 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,2 0 0,-2 1-21,1-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 1-1,0-1 1,0 1-1,-1 0 1,1 0-1,4 2 1,-6-2 15,1 0 0,-1 0-1,0 0 1,0 0 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1 0,-1 0-1,1-1 1,0 1 0,-1-1 0,1 1 0,-1 0-1,0-1 1,0 1 0,1 0 0,-1 0 0,0-1-1,-1 3 1,-2-3 43,1 0 1,-1 0-1,0 0 0,0-1 0,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0-1 1,0 0-1,0 1 0,0-1 0,-4-2 0,6 2-38,0 0-1,0-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,1 0 1,-1 1-1,0-1 1,1 0-1,0 0 1,-1 0-1,1 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,1-1-1,-1 0 1,0 0-1,1 0 1,0 1-1,-1-1 1,1 0-1,0 1 1,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1 0-1,0-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,1 0-1,-1 0 1,1 0-1,0 1 1,-1-1-1,1 0 1,0 1-1,0 0 1,0-1-1,-1 1 1,1 0-1,0 0 1,0 0-1,2 0 1,-3 1-14,1-1 1,-1 1-1,1 0 1,-1-1-1,1 1 1,-1 0 0,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 1 0,0-1-1,-1 0 1,1 1-1,0-1 1,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1 0,0 3-1,4 44-14,-4-45 28,0 9 20,-1 0-1,0 0 0,-1 0 1,0 0-1,-1-1 0,0 1 1,-1-1-1,-1 0 0,1 0 1,-2 0-1,0-1 0,-1 1 1,0-1-1,0-1 0,-10 11 1,-38 42-302,15-25-2783,11-14-2173</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8872.62">3199 353 5587,'0'0'10967,"-1"-6"-9905,-1 2-711,1 0-1,0 0 1,0-1 0,0 1-1,0-1 1,1 1-1,0-7 1,0 9-259,1 1 1,-1-1-1,1 0 1,-1 0-1,1 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 0,1 1 1,-1 0-1,0 0 0,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,1 0 0,4-1 1,1 0 0,-1 1-1,0-1 1,0 1 0,1 1-1,14 0 1,-18 0-67,-3 0-21,0 1-1,0 0 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,-1 0-1,1 0 0,-1 0 1,0 1-1,1-1 0,-1 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,-1 0-1,1 3 0,-7 40 128,0-33-105,-1 1 0,0-1 0,-1-1 0,0 1 0,-1-1 0,0-1 0,0 0 0,-1-1 0,-21 14 0,35-23-92,0 1 0,0-1 1,-1 1-1,1 0 0,0 0 1,0 0-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 1 0,4 2 1,-5-3 49,1 0-1,-1 1 1,1-1 0,-1 1 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,-1 0-1,1 0 1,0 1 0,-1-1 0,1 1 0,-1-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0-1,-1 0 1,1 4 0,0-5 27,-1 1 1,0-1-1,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,0 1 0,1-1 1,-1 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-4 2 1,1-2 76,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,-7 1 0,-6 0-181,-9 1 185,10-1-6222</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9597.66">3482 514 8052,'0'0'9657,"-45"20"-7725,45-19-1912,-1-1 0,1 0 0,0 0 0,0 0 0,-1 0 1,1 1-1,0-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0 1 1,-1 0-1,1 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 1,0 0-1,0-1 0,-1 1 0,7-12 16,-6 12-41,0 1 0,0-1 0,0 1 0,0-1 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 2 34,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,-1 1 0,-7 0 59,9-1-88,0 1 0,-1-1 1,1 1-1,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 1,0 1-1,0-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 1,0 1-1,1-1 0,-1 0 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-2 1,0 1-8,-1-1 0,1 1 0,-1-1 1,1 1-1,-1 0 0,1-1 1,0 1-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,2 0-1,-2 0-9,0 1 1,-1 0-1,1 0 0,0 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0 0-1,0 1 0,-1-1 1,1 0-1,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 1,-1 1-1,1-1 0,-1 1 1,1-1-1,0 1 0,-1-1 1,1 1-1,-1-1 0,1 1 1,-1-1-1,1 1 0,-1 0 1,1 2 5,0-1 0,0 1 1,0-1-1,-1 1 0,1-1 1,-1 1-1,0-1 0,1 1 1,-1 0-1,-1 2 0,1 1 18,-1 0 0,1 0 0,-1-1 0,-1 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,-4 4 0,-7 6-150,-1-1 1,-20 18 0,5-10-3989,17-15-1793</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10531.14">3627 366 11461,'0'0'9986,"21"-18"-7934,-17 16-2041,-1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1-1 0,-1 1 1,0-1-1,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,2-6 0,-1-4 34,0 0 0,0 0 1,-1-25-1,-1 35-28,0 2 1,1 7-53,0 1 0,-1-1-1,0 0 1,0 0 0,0 1-1,0-1 1,-3 10 0,2-10 24,-5 42 102,-2 16 82,-1 66 0,4-129-116,-1-1-1,1 1 0,0-1 1,-1 0-1,1 0 0,0-1 1,0 1-1,-6-3 0,-3 3-51,12 0-5,-1 0 0,1 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,0-1 1,-1 0-1,1 1 1,-3-3-1,4 3-52,41 0-163,2-3-1743,-14-2-3390,-7-1-1993</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11105.35">3823 17 10789,'0'0'10167,"-8"-17"-8627,11 18-1514,0 0 1,0 0 0,0-1 0,0 2 0,0-1 0,-1 0-1,1 0 1,0 1 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 1 0,2 3 0,31 55 113,-31-54-91,7 14-57,-2 1 0,-1 1 0,0-1 0,-2 1 0,0 0 0,-2 0 0,0 1 0,-2 0 0,-1-1 0,0 1 0,-2 0 0,-1 0 0,-1-1 0,0 1 0,-2-1 0,-1 0 0,-1 0 0,-1-1 0,-1 0 0,-17 32 0,-64 94-2401,21-57-3066,26-43-1152</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink23.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:41:25.521"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 47 6563,'0'0'12198,"14"-17"-6158,-21 177-5934,7-159 180,0-37-14,1 26-273,0 0-1,1-1 1,0 1-1,0 0 1,6-12 0,-5 11 5,1 0 0,-1 1 0,-1-1 0,0-1 0,0-14 0,-2 25-23,0 28-605,-10 61 648,10-87 230,0-35 116,0-31-2344</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink24.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:41:25.522"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.035" units="cm"/>
+      <inkml:brushProperty name="height" value="0.035" units="cm"/>
+      <inkml:brushProperty name="color" value="#004F8B"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3 82 21582,'-3'43'0,"31"-125"0,-24 39 0,-33 125 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink25.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
       <inkml:timestamp xml:id="ts0" timeString="2025-05-18T16:22:53.355"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
@@ -17646,7 +18240,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">134 325 5250,'0'0'13860,"-13"-2"-8567,-40-3-5266,49 6-28,1-1-1,0 1 1,0 0 0,-1 0 0,1 0-1,0 0 1,0 1 0,0-1 0,0 1-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,1 1 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1-1,0 0 1,1 0 0,0 0 0,-1 0-1,1 0 1,0 1 0,0-1 0,1 0-1,-1 0 1,1 1 0,0-1 0,-1 0-1,1 1 1,1-1 0,0 6-1,0-8 3,0 0-1,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 1,1 0-1,0 0 0,0 0 0,0 0 0,3-1 0,-1 1-13,1-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 1,1-1-1,4-1 0,-2-3-57,0 0 0,-1 0 1,0 0-1,0-1 0,0 0 0,-1 0 1,0-1-1,0 1 0,-1-1 0,0 0 1,0 0-1,-1 0 0,0-1 0,3-12 0,-1-4 43,-1 0-1,-2-1 0,0-42 0,-3 54 249,-2 21 52,-2 24-143,2 28-52,2-36 25,0 0-1,1 0 0,1 0 0,6 30 1,-6-50-93,0 0 1,0 0 0,0 0 0,0 1-1,1-1 1,-1-1 0,1 1-1,0 0 1,0 0 0,0-1-1,0 1 1,1-1 0,-1 1-1,1-1 1,-1 0 0,1 0-1,0 0 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0-1,1-1 1,-1 1 0,0-1-1,1 0 1,-1 0 0,0 0-1,1 0 1,-1 0 0,0-1-1,1 1 1,-1-1 0,5-2 0,-2 1-25,0 1 1,0-1 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0-1 0,0 1 0,0-1-1,-1 0 1,0 0 0,1 0 0,-1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-2 0 0,4-8 0,-5 10-9,0 0 1,0 0-1,0 0 1,-1-1-1,0 1 1,1 0-1,-1-1 1,0 1-1,-1 0 1,1 0-1,-1-1 1,-1-5-1,1 8 17,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,0-1 1,-1 0-1,1 1 0,-2 0 0,-1 1 12,1 0 0,0 0-1,-1 0 1,1 1 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,1 1 0,-1-1 0,1 1 0,-1 0-1,1 0 1,1 0 0,-1-1 0,0 1 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,0 5 0,0-9-7,-1 1 0,1 0 0,-1 0 0,1-1-1,0 1 1,-1 0 0,1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 0 0,30-13 12,-25 8-27,-1-1-1,1 0 0,-1-1 0,-1 1 0,0-1 0,0 0 0,0 0 1,-1 0-1,0-1 0,0 1 0,-1-1 0,-1 1 0,2-13 1,0-15-80,-4-71 1,-1 47 134,2 60-8,-3 25-104,-2 20 157,1-1 0,2 1 1,7 72-1,-5-113-72,1-1 0,-1 0 0,1 0 0,0 0 0,-1 1 0,2-1 0,-1 0-1,0 0 1,0 0 0,1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 1-1,1-2 1,0 1 0,-1 0 0,1 0 0,0-1 0,0 0 0,7 2 0,-6-1-318,0-2 0,0 1 0,0 0-1,1-1 1,-1 0 0,0 0 0,0 0 0,8-2 0,-7 1-688,-1 0 0,0 0 0,1-1 0,-1 1 0,0-1 1,0 0-1,-1-1 0,8-4 0,9-11-9948</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="326.48">681 49 12374,'0'0'6717,"-6"14"-4913,-12 72 494,-27 168-1789,45-252-1004,-1 13-993,2-5-7948</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="326.47">681 49 12374,'0'0'6717,"-6"14"-4913,-12 72 494,-27 168-1789,45-252-1004,-1 13-993,2-5-7948</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1021.01">794 238 10837,'0'0'7305,"0"32"-5641,-3 98 2143,3-129-3468,2-3-292,0-1-1,0 1 0,0-1 1,-1 1-1,1-1 0,-1 0 0,0 0 1,1 0-1,0-3 0,1-2-10,6-6 1,-6 10-21,0 0 0,0 0-1,-1-1 1,1 0 0,-1 1-1,3-9 1,4 24-294,-7 4 273,-3-10 14,2 1 0,-1-1-1,0 1 1,1-1 0,0 0 0,1 0 0,-1 1 0,1-1 0,0 0 0,0 0 0,5 7 0,-6-11-9,0-1 0,0 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 0 0,0 0 1,0-1-1,1 1 0,-1 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,-1 0 0,2-1 1,24-32 9,-20 25-10,0 1-45,11-10 193,-16 18-134,0 0 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1-1,-1-1 1,1 1 0,0-1 0,0 1-1,-1 0 1,1-1 0,0 1-1,-1 0 1,1-1 0,-1 1 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0-1-1,1 1 1,-1 0 0,0 0 0,0 0-1,1 0 1,-1 2 0,6 18-178,9 19 931,-2-26-3465,6-9-4371,-12-5 60</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1560.14">1093 293 9364,'0'0'10349,"3"3"-9100,0 0-1051,0 1 1,0 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 0-1,0 1 1,-1-1 0,1 1 0,-1-1 0,0 1 0,0 0-1,0 5 1,-1-10-188,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,13-7 223,7-10-107,-19 16-129,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 1 0,-1-1 0,1 0-1,0 0 1,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,1 1 0,-1 0 0,0 0-1,0 0 1,0 0 0,1 0 0,-1 0 0,2 1 0,-1 0 7,1 1 0,-1 1 0,0-1 1,0 0-1,0 0 0,0 1 0,0-1 1,-1 1-1,4 5 0,-5-7-5,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0-1 0,0 1 0,-1 0 1,1 0-1,0-1 0,0 1 0,0-1 0,0 1 1,0 0-1,0-1 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 1,0 0-1,2-1 0,-1 0-5,0-1-1,0 1 0,0-1 1,0 0-1,0 0 0,0 1 1,-1-1-1,1 0 1,0-1-1,-1 1 0,0 0 1,0 0-1,1-1 1,-1 1-1,0-3 0,0 6-84,1 2 32,0 0-1,0 0 1,0-1 0,1 1 0,-1-1 0,1 0-1,-1 0 1,1 0 0,0 0 0,0 0 0,-1 0-1,1-1 1,1 1 0,-1-1 0,4 2 0,-4-3-525,0-1 0,-1 1 0,1 0 0,0-1 1,-1 1-1,1-1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0-1 1,1 1-1,-1-1 0,3-3 0,12-8-7183</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1872.78">1514 28 10965,'0'0'11000,"1"-7"-10173,5-13-342,-4 43 202,-6 53 395,-25 74-69,3-18-751,26-122-657,6-4-4736,15-17-2570,-5-1 754</inkml:trace>
@@ -17657,7 +18251,7 @@
 </inkml:ink>
 </file>
 
-<file path=xl/ink/ink21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ink/ink26.xml><?xml version="1.0" encoding="utf-8"?>
 <inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
   <inkml:definitions>
     <inkml:context xml:id="ctx0">
@@ -17718,18 +18312,18 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">151 994 14150,'0'0'9925,"-12"-30"-7532,11 29-2365,-1 1-1,1 0 0,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,1 1-1,-1-1 1,1 1-1,0-1 0,-1 1 1,1 0-1,0 0 1,-1-1-1,1 1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,0 1-1,1-1 0,-2 2 1,-27 52-179,25-47 216,-2 6-64,0 1 0,1 0 0,-4 17 1,8-26-14,0 0 0,0 0 1,0 0-1,1 0 1,0 1-1,0-1 0,0 0 1,1 0-1,0 0 1,3 12-1,-3-16 6,0-1-1,0 1 1,1-1 0,-1 1 0,0-1-1,1 1 1,-1-1 0,0 0-1,1 0 1,0 1 0,-1-1-1,1 0 1,0-1 0,0 1-1,-1 0 1,1 0 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,3-1 0,0 1 9,0-1 1,1 0-1,-1 0 1,0 0-1,-1 0 0,1-1 1,0 0-1,0 0 1,5-3-1,-3-1 9,0 1-1,0-1 0,0-1 1,-1 1-1,0-1 1,0 0-1,-1 0 1,0-1-1,0 1 1,-1-1-1,0 0 0,0-1 1,-1 1-1,0-1 1,0 1-1,-1-1 1,0 0-1,-1 0 1,0 0-1,0 0 0,-1 0 1,0 0-1,-2-15 1,1 20-5,-1 0 1,1 0 0,-1-1-1,0 1 1,0 0 0,0 1-1,0-1 1,0 0-1,-1 0 1,0 1 0,0 0-1,0-1 1,0 1 0,-1 0-1,1 1 1,-1-1-1,1 1 1,-1-1 0,0 1-1,0 0 1,0 1 0,0-1-1,-1 1 1,1-1-1,0 1 1,-1 0 0,-5 0-1,5 0 0,-1 0-1,0 0 0,1 1 1,-1-1-1,0 1 0,1 1 1,-1-1-1,0 1 0,1 0 1,-1 0-1,0 1 1,1-1-1,0 1 0,-1 0 1,1 1-1,0-1 0,0 1 1,0 0-1,1 1 0,-9 6 1,11-7-104,0-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,3 6 0,-2-7-535,0 1-1,0 0 1,1 0 0,-1 0-1,1-1 1,0 1 0,-1-1 0,1 1-1,0-1 1,0 0 0,1 0 0,4 4-1,20 7-9537</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="516.11">810 959 14391,'0'0'9684,"0"14"-9572,0 12 112,-10 9 112,-1 3 32,0 5-191,1 1-161,-1-1-16,0-1 0,8-5-737,-1-5-3569,4-10-6803</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1059.55">1371 938 16680,'0'0'6050,"7"-8"-5943,-4 5-95,1-1-1,0 1 0,0 0 1,0 0-1,1 0 1,-1 0-1,0 1 0,1 0 1,5-3-1,-8 5-8,-1 0 0,1-1 0,-1 1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,1 2 0,-1 0 0,0-1-1,-1 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 3 1,2 2 18,-1 1 1,-1 0 0,1-1 0,-1 1 0,-1 0 0,1 0-1,-1-1 1,-1 1 0,1 0 0,-1-1 0,-3 8 0,-5 7 69,0 0 1,-17 24 0,-14 34 1145,40-80-1223,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 1,0 1-1,-1-1 0,1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,2 0 0,39-11-156,-34 8 188,83-27-1736,-28 9-3180,-51 17 3365,43-15-7688</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1619.08">2552 950 17848,'0'0'8196,"-7"-6"-7633,-21-17-336,28 23-225,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 1,0 1-1,1 0 0,15-10 44,-12 9-32,11-6-7,0 0 0,0 2 0,1-1 0,0 2 0,0 0 0,0 1 0,1 1 0,-1 0 0,1 1 0,17 2 0,-33-1-8,-1 1-1,1-1 1,0 1-1,0-1 0,-1 1 1,1-1-1,-1 1 1,1 0-1,0-1 1,-1 1-1,1 0 0,-1-1 1,0 1-1,1 0 1,-1 0-1,1-1 0,-1 1 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,0 0 1,-2 0-1,-15 36-33,-15-2 121,26-30-87,0 0-1,1 1 1,-1 0-1,1 0 1,0 0-1,1 1 0,-1-1 1,1 1-1,1 0 1,-1 1-1,1-1 0,0 0 1,1 1-1,0 0 1,-1 9-1,3-16-1,0 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,1-1 1,0 1 0,-1 0-1,1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1 0,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,32 11-74,-24-8 68,0-1 5,39 14-50,-48-16 54,0 1 1,-1-1-1,1 0 1,0 1 0,-1-1-1,1 0 1,0 1-1,-1-1 1,1 1-1,-1-1 1,1 1 0,0-1-1,-1 1 1,1-1-1,-1 1 1,0 0-1,1-1 1,-1 1-1,0 0 1,1-1 0,-1 1-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1-1 1,1 1 0,0 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,-1-1 1,1 1 0,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 0 1,0 1-1,1-1 1,-1 1-1,-1-1 1,-29 21 81,-2-2 0,0-1 0,-45 17 0,9-4-562,12-5-2443,1-5-5099</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2312.92">3420 850 15415,'0'0'9266,"-1"0"-9216,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 2 0,-3 19 201,1 1 1,0-1 0,2 0-1,0 1 1,3 23 0,-2-41-254,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1-1 0,1 1 1,-1 0-1,1-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 1,1 0-1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 0 0,7-1 1,-4 0-21,0-1 1,0 0 0,0 0 0,0 0 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 0-1,0 0 1,0 0 0,0-1 0,-1 1 0,0-1 0,0 0 0,6-10 0,5-8-71,-1 0 1,18-45 0,-33 75 123,0 1 1,0 0-1,1-1 1,0 1-1,0 0 1,2 8-1,0 15 138,-9 134 25,7-162-308,0 0 0,0 0 0,0 0 0,1 1-1,-1-1 1,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1-1 0,1 1 0,0 0 0,3 3 0,-2-4-603,-1 0 1,1 1-1,0-1 1,0 0-1,0-1 0,1 1 1,-1 0-1,0-1 1,6 2-1,32 5-11449</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2755.29">4436 840 18585,'0'0'5047,"-15"-1"-3547,-47-4-641,60 5-836,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,1 1-1,-1-1 0,0 1 1,0-1-1,1 1 0,-1 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 1-1,0-1 0,-1 0 1,1 1-1,0-1 0,0 1 1,0-1-1,0 1 0,1 0 1,-1 0-1,0-1 0,1 1 1,-1 0-1,1 0 0,-1-1 0,1 1 1,0 0-1,0 0 0,0 3 1,0 3-27,0 1 1,1 0-1,0-1 0,0 1 1,1 0-1,3 9 1,3 5 36,2 0 0,15 26 0,-17-37 6,-1 1-1,-1 1 0,0-1 1,0 1-1,-1 0 0,-1 0 1,0 0-1,-1 1 1,1 25-1,-3-39-69,-1-1-1,0 0 1,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 0 0,0 1-1,0-1 1,0 0 0,0 1 0,-1-1-1,1 0 1,0 1 0,0-1 0,-1 0 0,1 1-1,0-1 1,-1 0 0,1 0 0,0 0-1,-1 1 1,1-1 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 1 0,1-1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,0 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,-1 1-1,-19-23-5598,-1-29-2275,-1-1 3542,2-3 3319,9 1 3714,10 47-1315,1 1 0,0-1 0,0 0 0,3-14 0,-1 18-1084,-1 1-1,1-1 1,0 1 0,-1 0-1,2-1 1,-1 1-1,0 0 1,1 0 0,-1 0-1,1 1 1,0-1-1,0 0 1,0 1-1,0 0 1,0 0 0,6-3-1,64-28 1478,-59 28-1416,245-80-314,-228 76-4224</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3354.29">5394 918 11861,'0'0'13697,"3"-8"-12835,6-23-206,-9 31-643,0 0 0,0 1-1,-1-1 1,1 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,0 0 1,-1 0 0,1-1-1,0 1 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0-1-1,-1 2 39,-15 13-17,1 1-1,1 0 1,0 1 0,1 0 0,0 2-1,1-1 1,2 1 0,0 1-1,0 0 1,-11 37 0,17-46-35,1 0 0,0 1 1,1 0-1,0-1 0,1 1 0,0 0 1,1 0-1,0 0 0,1 0 1,0 0-1,4 16 0,-4-22-19,1-1-1,-1 0 1,1 1-1,1-1 1,-1 0-1,0 0 1,1 0-1,0 0 1,0-1-1,0 1 1,1-1 0,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,0-1 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1-1 0,1 1-1,-1-1 1,1-1-1,0 1 1,-1 0-1,1-1 1,0 0-1,5-1 1,-127-5 554,97 5-3342,8 0-3605,38 1-1193</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3760.19">6035 876 17608,'0'0'7265,"-13"0"-6217,-39 0-472,39 3-329,13 1-215,10 3-84,6-3 79,1-1-1,-1-1 1,0 0 0,1-1-1,-1 0 1,18-3-1,-20 1-9,0 0 0,0 1 0,0 1 0,0 0 0,0 1 0,0 0-1,0 1 1,0 1 0,14 5 0,-25-7-13,-1 0 0,1 0-1,0 0 1,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 1 0,0-1-1,0 0 1,0 1 0,-1-1 0,1 1-1,-1-1 1,0 0 0,0 1-1,0-1 1,0 1 0,-1-1 0,1 1-1,-2 3 1,-1 7 31,0 0 1,-1 1-1,-1-1 0,0-1 1,-9 17-1,6-13-179,-4 5-398,1 1 0,1 0-1,-12 41 1,18-52-3761</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3896.51">6036 1179 14679,'0'0'10837,"117"-88"-10885,-32 52-1649,11-7-5154</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7716.4">154 717 9941,'0'0'8660,"2"-6"-8322,-2 4-302,1 1-1,-1-1 1,1 0 0,0 0-1,-1 1 1,1-1-1,0 0 1,0 1-1,0-1 1,0 0 0,1 1-1,-1 0 1,0-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1 0-1,2-1 1,44-12 1065,-42 12-1049,416-62 1918,-205 36-1816,-13 2-31,282 0-1,-61 10-187,2 0 88,721 30 6,340 0 39,-1434-14-51,0 3-26,61 10-1,36 2 189,437-27 2457,-524 11-2337,-42 2-140,-1-2 0,35-4 1,-12 6 361,-39 0-522,0 0 1,-1-1-1,1 0 0,0 1 0,-1-2 0,1 1 0,-1 0 0,1-1 1,0 0-1,7-2 0,-12 2 153,-2-2-151,-1-1 0,0 1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1 0 1,-9-4-1,-5-3 6,-15-11 29,23 15-4,1 0 0,-1-1-1,1 0 1,-14-12 0,22 17 181,5 16-645,4-3 435,0-1 0,1 0 0,0-1 0,1 0 0,17 13 0,13 12-157,-40-34 150,-1 0-1,1 0 1,0 0 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,-1-1 0,1 1-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1-1 0,0 1-1,1 0 1,-1-1-1,0 1 1,0 0 0,0-1-1,1 1 1,-2 0 0,-35 24-7,35-24 4,-46 26-43,-13 7-159,22-10-5287,28-17-69</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8307.64">6035 29 13014,'0'0'10682,"-9"-4"-9871,-35-16 464,48 21-1264,1 0 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,6-2 0,8 1 45,111-3 24,-130 4-84,1 0 0,0 1-1,-1-1 1,1 0 0,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1 0 0,-1-1-1,0 1 1,1-1 0,-1 1-1,0 0 1,0-1 0,1 1-1,-1 0 1,0-1 0,0 1-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 1-1,-1 27-157,1-22 141,-2 12-618,0 1 1,-2-1 0,0 0-1,-1 0 1,-1-1 0,-1 1-1,0-1 1,-19 32 0,22-43 300,-3 6-4400</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8510.42">6063 159 16408,'0'0'7523,"106"-55"-7523,-60 47 0,1 0-32,-1 4-1121,-4-2-2624,-6 2-3763</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">152 1002 14150,'0'0'9925,"-12"-30"-7532,11 29-2365,-1 1-1,1 0 0,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 0,-1-1 1,1 1-1,-1-1 1,1 1-1,0-1 0,-1 1 1,1 0-1,0 0 1,-1-1-1,1 1 0,0 0 1,0 0-1,0 0 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 1,0 1-1,1-1 0,-2 2 1,-28 53-179,26-48 216,-2 6-64,0 1 0,1 0 0,-4 17 1,8-26-14,0 0 0,0 0 1,0 0-1,1 0 1,0 2-1,0-2 0,0 0 1,1 0-1,0 0 1,3 12-1,-3-16 6,0-1-1,0 1 1,1-1 0,-1 1 0,0-1-1,1 1 1,-1-1 0,0 0-1,1 0 1,0 1 0,-1-1-1,1 0 1,0-1 0,0 1-1,-1 0 1,1 0 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,1 0 0,-1 0-1,0 0 1,3-1 0,0 1 9,0-1 1,1 0-1,-1 0 1,0 0-1,-1 0 0,1-1 1,0 0-1,0 0 1,5-3-1,-3-1 9,0 1-1,0-1 0,0-1 1,-1 1-1,0-1 1,0 0-1,-1 0 1,0-2-1,0 2 1,-1-1-1,0 0 0,0-1 1,-1 1-1,0-1 1,0 1-1,-1-1 1,0 0-1,-1 0 1,1 0-1,-1 0 0,-1 0 1,0-1-1,-3-14 1,2 20-5,-1 0 1,1 0 0,-1-1-1,0 1 1,0 0 0,0 1-1,0-1 1,0 0-1,-1 0 1,0 1 0,0 0-1,0-1 1,0 1 0,-1 0-1,1 1 1,-1-1-1,1 1 1,-1-1 0,0 1-1,0 0 1,0 1 0,0-1-1,-1 1 1,1-1-1,0 1 1,-1 0 0,-5 0-1,5 0 0,-1 0-1,0 0 0,1 1 1,-1-1-1,0 1 0,1 1 1,-1-1-1,0 1 0,1 0 1,-2 0-1,1 1 1,1-1-1,0 1 0,-1 0 1,1 1-1,0-1 0,0 1 1,0 0-1,1 1 0,-9 6 1,11-7-104,0-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 0,0 0 1,1 0-1,-1 0 0,1 0 0,-1 0 0,3 6 0,-2-7-535,0 1-1,0 1 1,1-1 0,-1 0-1,1-1 1,0 1 0,-1-1 0,1 1-1,0-1 1,0 0 0,1 0 0,4 4-1,20 7-9537</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="516.11">815 967 14391,'0'0'9684,"0"14"-9572,0 12 112,-10 10 112,-1 2 32,0 5-191,1 2-161,-1-2-16,0-1 0,8-4-737,-1-6-3569,4-10-6803</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1059.55">1380 946 16680,'0'0'6050,"7"-8"-5943,-4 5-95,1-1-1,0 1 0,0 0 1,0 0-1,1-1 1,-1 1-1,0 1 0,1 0 1,5-3-1,-8 5-8,-1 0 0,1-1 0,-1 1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,2 1 0,-2-1 0,0 1 0,1-1 0,1 2 0,-1 0 0,0-1-1,-1 1 0,1-1 0,-1 1 0,1 1 0,-1-1 0,0-1 0,0 1 1,0 0-1,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,-1 3 1,2 2 18,-1 1 1,-1 0 0,1-1 0,-1 1 0,-1 0 0,1 0-1,-1-1 1,-1 1 0,1 0 0,-1-1 0,-3 9 0,-5 6 69,-1 0 1,-16 24 0,-14 35 1145,40-81-1223,1 1 0,-1-1 0,1 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,0-1 1,0 1-1,-1-1 0,1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,2 0 0,39-11-156,-34 8 188,84-27-1736,-29 9-3180,-50 17 3365,42-16-7688</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1619.08">2569 958 17848,'0'0'8196,"-7"-6"-7633,-21-17-336,28 23-225,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,1-1 0,-1 1 0,0-1 0,0 1 0,0-2 0,0 2 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 1,0 1-1,1 0 0,15-10 44,-12 9-32,11-6-7,0 0 0,0 2 0,1-1 0,0 2 0,0 0 0,0 1 0,2 1 0,-2 0 0,1 1 0,17 2 0,-33-1-8,-1 1-1,1-1 1,0 1-1,0-1 0,-1 1 1,1-1-1,-1 1 1,1 0-1,0-1 1,-1 1-1,1 0 0,-1-1 1,0 1-1,1 0 1,-1 0-1,1-1 0,-1 1 1,0 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,-1-1-1,1 1 1,0 0-1,0 0 1,-1 0-1,1-1 0,-1 1 1,1 0-1,0 0 1,-2 0-1,-15 37-33,-15-3 121,26-30-87,0 0-1,1 1 1,-1 0-1,0 0 1,1 0-1,1 1 0,-1-1 1,1 1-1,1 0 1,-1 1-1,1 0 0,0-1 1,1 1-1,0 0 1,-1 9-1,3-16-1,0 0-1,1 0 1,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 0-1,1-1 1,0 1 0,-1 0-1,1 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,-1-1 1,1 1 0,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,33 11-74,-25-8 68,0-1 5,39 14-50,-48-16 54,0 1 1,-1-1-1,1 0 1,0 1 0,-1-1-1,1 0 1,0 1-1,-1-1 1,1 1-1,-1-1 1,1 1 0,0-1-1,-1 1 1,1-1-1,-1 1 1,0 0-1,1-1 1,-1 1-1,0 0 1,1-1 0,-1 1-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,-1-1 1,1 1 0,0 0-1,0 0 1,-1-1-1,1 1 1,0 0-1,-1-1 1,1 1 0,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 2-1,1-2 1,-1 1 0,1-1-1,-1 0 1,0 1-1,1-1 1,-1 1-1,-1-1 1,-29 21 81,-2-2 0,-1-1 0,-44 17 0,8-3-562,13-6-2443,1-5-5099</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2312.92">3442 857 15415,'0'0'9266,"-1"0"-9216,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 2 0,-3 19 201,1 1 1,0 0 0,2-1-1,0 1 1,3 23 0,-2-41-254,1 0 0,-1 0 0,1-1 0,-1 2 0,1-1 0,0-1 0,1 1 1,-1-1-1,0 1 0,1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1-1 0,1 1 1,-1 0-1,2-1 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 1,1 0-1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 0 0,7-1 1,-4 0-21,0-1 1,0 0 0,0 0 0,0 0 0,0-1 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,-1-1 0,0 0 0,6-11 0,5-7-71,-1 0 1,18-45 0,-33 75 123,0 1 1,0 0-1,1-1 1,0 1-1,0 0 1,2 8-1,0 15 138,-9 136 25,7-164-308,0 0 0,0 0 0,0 0 0,1 1-1,-1-1 1,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1-1 0,1 1 0,0 0 0,3 3 0,-2-4-603,-1 0 1,1 1-1,0-1 1,0 0-1,0-1 0,1 1 1,-1 0-1,0-1 1,6 2-1,33 5-11449</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2755.29">4465 847 18585,'0'0'5047,"-15"-1"-3547,-47-4-641,60 5-836,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,1 1-1,-1-1 0,0 1 1,0-1-1,1 1 0,-1 0 1,-1 0-1,2 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1 1-1,0-1 0,-1 0 1,1 1-1,0-1 0,0 1 1,0-1-1,0 1 0,1 0 1,-1 0-1,0-1 0,1 1 1,-1 0-1,1 0 0,-1-1 0,1 1 1,0 0-1,0 0 0,0 3 1,0 3-27,0 1 1,1 0-1,0 0 0,0 0 1,1 0-1,3 9 1,3 5 36,3 0 0,14 27 0,-17-38 6,-1 1-1,-1 1 0,0-1 1,0 1-1,-1 0 0,-1 0 1,0 0-1,-1 2 1,1 24-1,-3-39-69,-1-1-1,0 0 1,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 0 0,0 1-1,0-1 1,0 0 0,0 1 0,-1-1-1,1 0 1,0 1 0,0-1 0,-1 0 0,1 1-1,0-1 1,-1 0 0,1 0 0,0 0-1,-1 1 1,1-1 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 1 0,1-1 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,0 0 0,-1 0-1,1 0 1,-1-1 0,1 1 0,0 0-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,0 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,-1 1-1,-19-23-5598,-1-30-2275,-1 0 3542,1-3 3319,10 0 3714,10 48-1315,1 1 0,0-1 0,0 0 0,3-14 0,-1 18-1084,-1 1-1,1-1 1,0 0 0,-1 1-1,2-1 1,-1 1-1,0 0 1,1 0 0,-1 0-1,1 1 1,1-1-1,-1 0 1,0 1-1,0 0 1,0 0 0,6-3-1,64-28 1478,-59 28-1416,247-81-314,-230 77-4224</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3354.29">5429 926 11861,'0'0'13697,"3"-9"-12835,7-22-206,-10 31-643,0 0 0,0 1-1,-1-1 1,1 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0-1,0 0 1,-1 0 0,1-1-1,0 1 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0-1,0 0 1,0-1 0,0 1-1,0 0 1,0-1-1,-1 2 39,-16 13-17,2 1-1,1 1 1,0 0 0,1 0 0,0 2-1,1-1 1,2 1 0,0 1-1,0 1 1,-11 36 0,17-46-35,0 0 0,1 1 1,1 0-1,0-1 0,1 2 0,0-1 1,1 0-1,0 0 0,1 0 1,0 0-1,4 16 0,-4-22-19,1-1-1,-1 0 1,2 1-1,0-1 1,-1 0-1,0 0 1,1 1-1,0-1 1,0-1-1,0 1 1,1-1 0,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,0-1 1,0 0-1,1 0 1,-1 0-1,1 0 1,-1-1 0,1 1-1,-1-1 1,1-1-1,0 1 1,-1 0-1,1-1 1,0 0-1,5-1 1,-128-5 554,98 5-3342,8 0-3605,38 1-1193</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3760.19">6075 883 17608,'0'0'7265,"-13"0"-6217,-40 0-472,40 3-329,13 1-215,10 3-84,6-3 79,1-1-1,0-1 1,-1 0 0,1-1-1,-1 0 1,18-3-1,-20 1-9,0 0 0,0 1 0,0 1 0,1 0 0,-1 1 0,0 0-1,0 1 1,0 2 0,14 4 0,-25-7-13,-1 0 0,1 0-1,0 0 1,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,0 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 1 0,0-1-1,0 0 1,0 1 0,-1-1 0,1 1-1,-1-1 1,0 0 0,0 1-1,0-1 1,0 1 0,-1-1 0,1 1-1,-2 3 1,-1 7 31,0 1 1,-1 0-1,-1-1 0,0-1 1,-9 17-1,6-13-179,-4 5-398,1 2 0,1-1-1,-12 41 1,18-52-3761</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3896.51">6076 1189 14679,'0'0'10837,"117"-89"-10885,-31 53-1649,11-8-5154</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7716.4">155 723 9941,'0'0'8660,"2"-6"-8322,-2 4-302,1 1-1,-1-1 1,1 0 0,0 0-1,-1 1 1,1-1-1,0 0 1,0 1-1,0-1 1,0 0 0,1 1-1,-1 0 1,0-1-1,1 1 1,-1 0 0,1-1-1,-1 1 1,1 0-1,2-1 1,44-13 1065,-41 13-1049,417-62 1918,-205 36-1816,-14 1-31,284 1-1,-61 10-187,2 0 88,725 30 6,343 0 39,-1443-14-51,-1 3-26,62 10-1,36 2 189,440-27 2457,-528 11-2337,-42 2-140,-1-2 0,36-4 1,-13 6 361,-39 0-522,0 0 1,-1-1-1,1 0 0,0 1 0,-1-2 0,1 1 0,-1 0 0,1-1 1,0 0-1,7-2 0,-12 2 153,-2-2-151,-1-1 0,0 1 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 1 0,-1-1 0,0 1 0,1 0 1,-9-4-1,-5-3 6,-15-11 29,23 15-4,1 0 0,-2-1-1,2 0 1,-14-13 0,22 18 181,5 17-645,4-4 435,0-1 0,2 0 0,-1-1 0,1 0 0,17 13 0,13 12-157,-40-34 150,-1 1-1,1-1 1,0 0 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,-1-1 0,1 1-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1-1 0,0 1-1,1 0 1,-1-1-1,0 1 1,0 0 0,0-1-1,1 1 1,-2 0 0,-35 24-7,35-24 4,-47 26-43,-12 7-159,22-9-5287,28-18-69</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8307.64">6075 29 13014,'0'0'10682,"-9"-4"-9871,-36-16 464,49 21-1264,1 0 0,-1-1 0,1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,6-2 0,8 1 45,112-3 24,-131 4-84,1 0 0,0 1-1,-1-1 1,1 0 0,-1 1-1,1-1 1,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,1 0 0,-1-1-1,0 1 1,1-1 0,-1 1-1,0 0 1,0-1 0,1 1-1,-1 0 1,0-1 0,0 1-1,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 1-1,-1 27-157,1-22 141,-2 13-618,0 0 1,-2-1 0,0 0-1,-1 0 1,-1-1 0,-2 2-1,1-2 1,-19 32 0,22-43 300,-3 6-4400</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8510.42">6103 160 16408,'0'0'7523,"107"-55"-7523,-61 47 0,1 0-32,-1 4-1121,-3-2-2624,-7 2-3763</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -17788,12 +18382,12 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 160 12710,'0'0'5757,"9"0"-5704,402-26 2744,-126 3-2784,322 14 168,-55 2-178,69-7 136,-395 6 1637,-248 0-396,-69-22-1363,58 18 141,-50-11 0,144 37-198,70 27 0,-129-41 15,0 1 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,2 3 0,-3-3 12,0-1 0,0 1 0,0 0 0,1-1-1,-1 1 1,-1-1 0,1 1 0,0 0 0,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1-1,0-1 1,-1 2 0,-3 3-123,0 1-1,-1-1 0,1-1 1,-1 1-1,-1-1 1,1 0-1,-10 5 0,-83 53-7909,78-46 1571</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="737.23">2340 423 10981,'0'0'10314,"-2"-6"-9450,2 4-806,-1 0-1,0 0 0,0-1 1,1 1-1,0 0 0,-1-1 0,1 1 1,0 0-1,0-1 0,0 1 0,0 0 1,1-1-1,0-3 0,0 4-29,1-1-1,-1 1 1,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 1 0,0 0-1,4-2 1,2-1 48,0 0-1,-1 1 1,2-1-1,-1 2 1,0-1 0,1 1-1,-1 0 1,1 1-1,-1 0 1,1 1 0,16 0-1,-24 1-71,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0-1 0,0 3 0,0 27 73,0-24-34,0-1-25,-1 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,-7 8 0,6-6 1,0-1-1,0 1 1,0 0 0,-4 14-1,7-20-19,1 1 1,0-1-1,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,2 2 0,48 12 16,-13-4-28,-38-10 15,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 1-1,-1-1 1,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,-1-1-1,1 0 1,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-28 13 204,26-13-173,-41 18 41,-33 13-299,26-19-3610,14-10-4585</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3106.41">2960 174 9508,'0'0'7353,"18"-2"-6993,446-10 2804,-297 14-2827,1361 49 68,-1250-30-441,92 10 56,-247-22 88,170-8 0,-242-6 859,0-2-1,50-14 1,-18 4-124,-85 16-1867,-12 1-5152,9 1 2798,-6-1-9721</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3489.78">6402 93 11157,'0'0'10709,"1"-7"-9927,1-20-243,-1 20 309,-1 31-531,0 320 1679,0-341-2342,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,1 0-1,0-1 1,0 1 0,0 0 0,0 0-1,0-1 1,1 1 0,2 3 0</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4337.93">2995 80 6723,'0'0'6742,"-4"-7"-5795,-11-19 61,10 47 4457,4 13-4537,1-8-767,4 133 954,-1-131-2946,11 47 1,-3-29-3560</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5409.71">3243 561 14551,'0'0'6285,"-2"-4"-5967,-6-8-241,1 14 6,-6 25 152,7-11-78,0-2-82,0 0 1,1 1 0,1 0-1,1 0 1,0 0-1,1 1 1,0-1-1,1 1 1,1-1-1,0 1 1,5 25-1,-3-33-63,-1-1 0,2 1-1,-1 0 1,1-1 0,0 0-1,1 0 1,0 0 0,0 0-1,0 0 1,1-1 0,0 1-1,0-1 1,0-1 0,1 1-1,0-1 1,0 0 0,1 0-1,-1-1 1,1 1 0,0-1-1,0-1 1,1 0-1,-1 0 1,11 3 0,16 1 9,0-2 0,0-1 0,0-2 0,0-1 0,1-1 0,42-7 0,157-37-178,-9 2-9,-67 27 112,193 6 1,-292 14 57,-1 4-1,0 1 1,0 4-1,64 23 1,-30-9 21,-88-27-14,13 3-9,-1 2-1,1 0 1,25 13-1,-39-17-4,-1-1 0,0 0 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,0 1 1,2 2 0,-3-3 1,1 0 1,-1 0-1,0-1 0,0 1 1,0 0-1,-1-1 0,1 1 0,0 0 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,0 0 1,0 1-1,0-1 0,-1 0 1,-1 1-1,-10 7 23,1 0-1,-2 0 1,1-1 0,-1-1-1,-1 0 1,1-1 0,-1-1-1,0 0 1,-1-1 0,1-1-1,-18 2 1,32-5-18,1-1 0,-1 1 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1-1,0-1 1,1 0 0,-1 1 0,0-1 0,1 1 0,0-2 0,13-31-206,-6 25 132,1 0-1,0 1 0,0 0 1,1 0-1,-1 1 0,1 0 1,1 1-1,-1 0 0,1 1 0,0 0 1,12-3-1,17-3-13,70-9 1,290-4-162,-67 7 301,-267 9-22,-1-2-1,0-4 0,64-21 0,-116 30-20,0-1 0,0 0 0,0-1 0,0 0 0,-1-1 0,0-1-1,-1 0 1,0 0 0,0-1 0,0-1 0,9-10 0,-13 10-13,1-1 1,-2 0-1,1 0 1,-1 0-1,-1 0 1,0-1-1,-1 0 1,0 0-1,-1 0 1,0-1-1,-1 1 1,1-18-1,-2 21-119,0 0-1,-1-1 1,0 1-1,0 0 1,-1-1-1,-4-15 1,4 22-83,0 0 0,0 0 0,0 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 1,0 0-1,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1 0 1,-1-1-1,0 1 0,0 0 0,1 0 0,-1 1 0,0-1 1,0 1-1,-4-1 0,-33-2-7908</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 161 12710,'0'0'5757,"9"0"-5704,405-26 2744,-127 3-2784,323 14 168,-54 2-178,69-7 136,-397 6 1637,-251 0-396,-68-23-1363,58 19 141,-51-11 0,145 37-198,71 27 0,-130-41 15,0 1 0,0-1 0,0 1 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,3 3 0,-4-3 12,0-1 0,0 1 0,0 0 0,1-1-1,-1 1 1,-1-1 0,1 1 0,0 0 0,0-1 0,-2 1-1,2-1 1,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1-1,0-1 1,-1 2 0,-3 3-123,0 1-1,-1-1 0,1-1 1,-1 1-1,-1-1 1,1 0-1,-10 5 0,-84 54-7909,79-47 1571</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="737.23">2355 426 10981,'0'0'10314,"-2"-6"-9450,2 4-806,-1 0-1,0 0 0,0-1 1,1 1-1,0 0 0,-1-1 0,1 1 1,0 0-1,0-1 0,0 1 0,0 0 1,1-1-1,0-3 0,0 4-29,1-1-1,-1 1 1,1 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0 1-1,1-1 1,-1 1 0,0 0-1,4-2 1,2-1 48,0 0-1,-1 1 1,3-1-1,-2 2 1,0-1 0,1 1-1,-1 0 1,1 1-1,-1 0 1,1 1 0,16 0-1,-24 1-71,-1-1 0,1 1 0,0-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0-1 0,0 3 0,0 27 73,0-24-34,0-1-25,-1 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,-7 9 0,6-7 1,0-1-1,0 1 1,0 0 0,-4 14-1,7-20-19,1 1 1,0-1-1,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,1-1 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,2 2 0,48 12 16,-13-4-28,-38-10 15,0 1 0,1-1 0,-1 0 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 1-1,-1-1 1,0 0 0,0 1 0,0-1 0,0 0 0,0 2 0,0-2 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,-1-1-1,1 0 1,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-28 13 204,26-13-173,-41 18 41,-34 13-299,27-19-3610,14-10-4585</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3106.41">2979 175 9508,'0'0'7353,"18"-2"-6993,449-10 2804,-299 14-2827,1370 50 68,-1258-31-441,92 10 56,-248-22 88,171-8 0,-244-6 859,1-2-1,49-14 1,-17 4-124,-86 16-1867,-12 1-5152,9 1 2798,-6-1-9721</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3489.78">6443 94 11157,'0'0'10709,"1"-7"-9927,1-21-243,-1 21 309,-1 32-531,0 321 1679,0-343-2342,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,1 1-1,0-2 1,0 1 0,0 0 0,0 0-1,0-1 1,1 1 0,3 3 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="4337.92">3014 81 6723,'0'0'6742,"-4"-7"-5795,-11-20 61,10 49 4457,4 12-4537,1-8-767,4 134 954,-1-131-2946,11 46 1,-3-29-3560</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5409.71">3264 565 14551,'0'0'6285,"-2"-4"-5967,-6-8-241,1 14 6,-6 26 152,7-12-78,0-2-82,0 0 1,1 1 0,1 0-1,1 0 1,0 0-1,1 2 1,0-2-1,1 1 1,1-1-1,0 1 1,5 25-1,-3-33-63,-1-1 0,2 2-1,-1-1 1,1-1 0,0 0-1,1 0 1,0 0 0,0 0-1,0 0 1,1-1 0,0 1-1,0-1 1,0-1 0,1 1-1,0-1 1,0 0 0,1 0-1,-1-1 1,1 1 0,0-1-1,0-1 1,1 0-1,-1 0 1,11 3 0,17 2 9,-1-3 0,0-1 0,0-2 0,1-1 0,0-1 0,42-7 0,159-38-178,-10 3-9,-67 27 112,195 6 1,-295 14 57,-1 4-1,1 1 1,-1 4-1,65 23 1,-31-8 21,-88-28-14,14 3-9,-2 2-1,1 0 1,25 13-1,-39-17-4,-1-1 0,0 0 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,0 1 1,2 2 0,-3-3 1,1 0 1,-1 0-1,0-1 0,0 1 1,0 0-1,-1-1 0,1 1 0,0 0 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,0 0 1,0 1-1,0-1 0,-1 0 1,-1 1-1,-10 7 23,1 1-1,-2-1 1,1-1 0,-1-1-1,-1 0 1,0-1 0,0-1-1,0 0 1,-1-1 0,1-1-1,-18 2 1,32-5-18,1-1 0,-1 1 0,0-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1-1,0-1 1,1 0 0,-1 1 0,0-1 0,1 1 0,0-2 0,13-31-206,-6 24 132,1 1-1,0 1 0,0 0 1,1 0-1,-1 1 0,1 0 1,1 1-1,-1 0 0,2 1 0,-1 0 1,12-3-1,17-3-13,71-9 1,291-4-162,-67 6 301,-268 10-22,-2-2-1,1-4 0,64-21 0,-117 30-20,0-1 0,0 0 0,0-1 0,0 0 0,-1-1 0,0-1-1,-1 0 1,0-1 0,0 0 0,0-1 0,10-10 0,-14 10-13,1-1 1,-2 0-1,1 0 1,-1 0-1,-1 0 1,0-1-1,-1-1 1,0 1-1,-1 0 1,0-1-1,-1 1 1,1-18-1,-2 21-119,0 0-1,-1-1 1,0 1-1,0-1 1,-1 0-1,-4-15 1,4 22-83,0 0 0,0 0 0,0 1 0,-1-1 1,0 1-1,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 1,0 0-1,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1 0 1,-1-1-1,0 1 0,0 0 0,1 0 0,-1 1 0,0-1 1,0 1-1,-4-1 0,-34-2-7908</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -17869,7 +18463,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:02:36.928"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-24T12:53:59.687"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -17877,15 +18471,21 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">218 50 3282,'0'2'22389,"0"16"-22552,-17 182 405,1-54-41,10-73 12,6-73-239,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,-8-8-4329,-2-8-4249</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="334.14">96 171 15319,'0'0'6707,"3"-12"-6195,-3 12-511,1-5 42,0 0 1,1 0-1,-1 0 0,1 0 1,0 0-1,1 0 0,-1 1 1,1-1-1,0 1 0,0-1 1,0 1-1,0 0 0,1 0 0,0 1 1,0-1-1,0 1 0,0 0 1,0 0-1,6-3 0,17-8 199,1 1 0,54-17 0,-69 27-287,0-1-1,0 2 0,0 0 1,0 0-1,0 1 0,0 1 1,1 0-1,-1 1 1,16 3-1,-28-4-75,1 1 0,-1 0-1,0-1 1,1 1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,0 0 1,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0-1,1 1 1,-1-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,0-1-1,0 1 1,0 1 0,0 2-564,0 0 1,0 1-1,-1-1 0,1 0 0,-1 0 1,-1 0-1,-1 7 0,-15 20-6604</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="629.47">22 585 13190,'0'0'9476,"-22"6"-8867,33-6-177,10 0-128,22 0 288,7-4-272,6-11-256,8 3 32,-11-4-96,-10 4-608,-11 2-2193,-8 2-1937,-6 0-3794</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1337.58">575 303 6627,'0'0'14252,"0"0"-14231,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1-1 0,-1 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,1 0-1,-1-1 1,0 1 0,0 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0-1,3 12 319,-1 0 0,-1 1 0,0-1 0,0 1 0,-1-1 0,-3 16 0,2 11 194,-10 20 219,11-58-426,0-13 15,1 1-331,0 1 1,0-1-1,1 1 1,1-1-1,0 1 1,6-14-1,-8 19-16,1 1 0,0 0 1,0 0-1,0 0 0,0 0 0,1 0 0,-1 0 0,1 1 1,0-1-1,1 1 0,-1 0 0,0 0 0,1 0 0,0 0 1,-1 1-1,1 0 0,7-4 0,-8 6-3,-1-1 0,1 1 0,0-1 0,-1 1 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,3 2 0,4 6 10,1 1 1,-2 0-1,11 16 0,-14-19 1,1 0 0,-1 0 0,1-1 0,0 0 1,12 10-1,-17-16 9,0-1 1,0 1 0,0-1-1,-1 0 1,1 1 0,0-1-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,-1 1-1,1-1 1,0 0 0,0 0-1,-1 1 1,1-1 0,-1 0-1,1 0 1,0 0 0,-1 1-1,1-3 1,21-43 230,-18 34-243,4-5-111,-1 0-1,-1-1 1,-1 0-1,-1 0 1,0 0-1,2-29 1</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1616.5">1047 215 15431,'0'0'9119,"-4"74"-7772,-15-6-639,13-50-1080,0 0-1,1 1 0,2 0 1,-3 32-1,17-53-8170,2-10 284</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1911.52">1067 270 10213,'0'0'13408,"-1"-5"-12986,0 4-425,1 1 0,-1-1 0,1 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,1 0 0,3 0-15,1 0 0,0 0 0,0 1 0,-1 0 0,1 0 0,8 3 1,-4-2 24,0 1 0,-1 1 1,1 0-1,-1 1 0,0-1 1,0 2-1,0-1 0,0 1 1,14 14-1,-19-16-4,0 0-1,0 1 1,-1 0 0,1 0 0,-1 0-1,0 0 1,-1 0 0,1 0 0,-1 1-1,0 0 1,0-1 0,-1 1 0,1 0-1,-1 0 1,-1 0 0,1-1-1,-1 1 1,-1 10 0,1-14 36,-1 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1-1,0 0 1,-1 0 0,1 1 0,-1-1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,-1 1 0,1-1 0,-4 2 0,-54 22 825,48-21-797,-18 7 15,-46 20-788</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2220.61">1373 303 17336,'0'0'7230,"-7"-10"-5248,5 40-1972,-1 0 0,-1 0 0,-15 51 0,7-30-1290,10-31-2221,2-7-3595</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2701.33">1600 296 13542,'0'0'7689,"-1"15"-6955,-2 14-369,-1 0 0,-1 0 0,-2 0 0,-1-1 0,-1 0 0,-13 28 1,22-56-355,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-1 0 0,1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0-1-1,0 1 1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,-2-15 179,4-22-235,5 8-11,3 2-1,0-1 1,1 1-1,2 1 1,1 0 0,20-29-1,-8 25-27,-14 29-35,-2 19 37,-5 5 163,-1 1 0,-1 0 0,-1-1-1,-2 41 1,-1-33-224,2-1 1,5 35-1,-5-55-3446</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2906.14">1593 470 8052,'0'0'13878,"60"-28"-13798,-17 16-16,-1 0-64,-6 2-176,-8 1-320,-14 3-1089,-14 4-896,-10 2-256</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">326 55 5507,'0'0'15217,"0"1"-15025,-1 0 0,1 0 0,0-1 1,0 1-1,0 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1-1 0,-1 1 1,1 0-1,-1-1 0,1 1 0,-1-1 0,1 0 0,-2 2 0,-50-13-118,1 1-47,39 9-36,0 1 0,0 1 0,0 0 0,0 0 0,0 1 0,-17 6 0,26-8 2,0 1 1,0 1-1,0-1 0,0 0 0,0 1 0,0-1 0,0 1 1,0 0-1,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 0,1 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0 1 0,0-1 1,1 0-1,-1 0 0,1 5 0,0-6-1,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1-1 1,1 1-1,-1-1 0,1 1 1,0-1-1,0 1 0,0-1 0,-1 0 1,1 0-1,0 0 0,0 0 1,4 1-1,58 20 22,-46-16 13,0-1-50,-1 2 0,1 0 0,-1 0 1,-1 2-1,0 0 0,0 1 0,-1 0 0,24 21 1,-38-30 6,0 0 0,1 0 1,-1 1-1,0-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0 1 1,0-1-1,-1 1 1,1-1-1,0 1 0,-1-1 1,1 1-1,-1-1 1,0 1-1,0 0 1,1-1-1,-1 1 0,0 0 1,0-1-1,0 1 1,-1 0-1,1-1 1,0 1-1,-1 1 0,-1 0 11,1-1-1,-1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1 0 1,0-1-1,-1 1 0,1-1 0,-1 0 1,1 0-1,-4 2 0,-12 2 56,0 0 0,0-1 0,-27 3 0,30-6 36,0 0 1,0 0-1,0-2 1,1 0 0,-1 0-1,-15-5 1,22 4-50,1 0 1,0 0 0,0-1-1,0 0 1,1 0 0,-1 0 0,1-1-1,-1 0 1,1-1 0,1 1-1,-1-1 1,0 0 0,-8-11 0,14 15-104,-1 0 1,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0-1,-1 0 1,0 1 0,1-1 0,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 1-1,1-1 1,0 0 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,0 0 0,0-1-1,-1 1 1,1 0 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,3 0-1,51-9-5558,-46 8 4192,33-4-5157</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="497.97">655 98 8100,'0'0'6907,"0"-7"-6072,4-31 5853,-4 47-6466,-4 69 448,-2 1 1,-25 111-1,18-134-1081,28-56-4241,8-9-561,5-14-3559</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1145.91">999 123 10389,'0'0'12590,"0"0"-12579,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0 0,0-1-1,-1 1 1,1 0-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,-1 1-1,1-1 1,-1 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,0 0-1,0 0 1,-1 1-1,1-1 1,0 0 0,-1 0-1,1 1 1,0-1-1,0 0 1,0 1 0,-1-1-1,1 1 1,-7 9 99,0 1 0,1 1 0,1-1 0,0 1 0,0 0 0,-4 19 0,0-3 8,-48 128 503,56-153-580,1-3 33,0-25 782,0 5-837,1-1 1,1 1 0,1 0 0,0 0-1,1 0 1,2 1 0,9-26-1,-12 39-26,0-1-1,0 0 0,1 1 0,0 0 0,0 0 1,0 0-1,1 0 0,0 1 0,0-1 0,0 1 1,1 1-1,-1-1 0,1 1 0,0 0 0,1 0 1,-1 1-1,1-1 0,-1 2 0,1-1 0,0 1 1,0 0-1,0 0 0,13-1 0,-17 2 4,1 1-1,-1-1 0,0 1 1,1 0-1,-1 0 0,1 0 1,-1 1-1,0-1 1,1 1-1,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,0 1-1,0-1 0,5 5 1,-6-3-5,0 0-1,0 0 1,0 0 0,-1 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 1 0,0-1-1,0 1 1,-1-1 0,0 6 0,0-4 9,-1 0 1,0 0 0,0 0-1,0 0 1,0-1 0,-1 1-1,0-1 1,0 1 0,0-1-1,0 0 1,-1 0 0,0-1-1,0 1 1,0-1 0,0 0-1,0 0 1,-8 4 0,3-1-17,0 0 0,-1-1 0,0-1 1,0 0-1,0 0 0,-1 0 0,-17 2 1,56 0-152,51 18 0,-46-14 202,-3-2-406,51 9 1,-5-11-8630,-50-6 2657</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1602.73">1491 162 8388,'0'0'14105,"1"-5"-13318,2-12-638,-2 30-78,-7 43 189,-3-27-75,0 0-1,-2-1 1,-2 0 0,-29 50-1,51-149 1060,3 32-1277,24-47 0,-29 72 20,0 0 1,1 0 0,1 1-1,0 0 1,1 1 0,17-18-1,-26 29 3,1-1 0,-1 1 0,1-1 0,0 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 1 0,3-1 0,-2 2 5,0-1 1,0 0 0,0 1 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,0 1 0,1-1 0,-1 1-1,2 3 1,1 2 7,0 0 0,0 1 0,-1 0 0,0 0 0,-1 0 0,0 1 0,0-1-1,2 20 1,-4-12-107,1-4-68,-1 1 0,0-1 0,-1 1 0,-1 0 0,0-1 0,-1 0 0,-3 16 0,4-28-253,0 1 1,1-1-1,-1 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,-1 1-1,-6 1-5927</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1851.2">1484 290 14999,'0'0'8993,"-4"-1"-8584,2-1-154,7-1-53,24-6 64,61-10-102,-33 6-158,9-1-854,9-3-6841,-43 8-56</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2076.21">1976 120 17544,'0'0'7219,"58"-24"-7139,-17 15-64,0 2 16,0-2-32,0-1 0,-13 6 16,-3-1-16,-13 3-480,-8 2-608,-24 7-10133</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2372.38">2070 131 14247,'0'0'7851,"0"12"-7758,5 228 740,-6-237-810,1 0 0,0 0 1,-1 0-1,1-1 0,-1 1 1,0 0-1,0-1 0,0 1 0,0 0 1,-1-1-1,1 0 0,0 1 0,-1-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0-1 0,0 1 0,0 0 1,0 0-1,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 0 0,0 0 1,1 0-1,-1-1 0,0 1 0,-3 0 1,-10 2 67,-1-1 0,1-1 1,0 0-1,-17-2 0,30 0-86,-1 1-33,0 0 1,0-1-1,1 1 0,-1-1 1,0 0-1,0 0 1,0-1-1,1 1 1,-1-1-1,1 0 0,-1 1 1,1-2-1,0 1 1,-1 0-1,1-1 1,0 1-1,1-1 0,-1 0 1,0 0-1,1 0 1,-3-5-1,-13-35-2756,13-3-3291,5 9-4527</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3553.95">2743 318 10341,'0'0'9727,"8"-12"-8503,25-41-138,-32 52-1001,0-1-1,0 0 0,1 0 0,-2 0 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,-1 0 1,0-3-1,0 3-63,-1 0 0,1 1 0,0-1-1,-1 1 1,1 0 0,-1-1 0,0 1 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 1 0,-4-1 0,-1 0-39,0 0 0,-1 0 0,1 1 1,-1 1-1,1-1 0,0 1 0,0 0 0,-1 1 1,-9 3-1,12-3-3,0 1 1,1 0-1,-1 1 0,1-1 1,0 1-1,0-1 0,0 1 1,1 1-1,-1-1 1,1 0-1,0 1 0,0 0 1,1-1-1,-1 1 0,1 0 1,0 0-1,0 1 1,1-1-1,-1 0 0,1 1 1,1-1-1,-1 1 0,1-1 1,0 1-1,0 7 1,1-12-11,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0-1 0,2 1 0,39-6-77,-30 0 154,0-1 0,-1 0 0,0-1 0,0 0 0,0 0 0,-1-2 0,-1 1 0,15-19 0,-32 109 138,8-81-88,25-21 742,-18 11-823,0 0 0,-1 0 0,0 0 1,-1-1-1,0 1 0,-1-1 0,0 0 1,-1-1-1,0 1 0,-1-1 0,0 1 1,-1-1-1,0 0 0,0 1 1,-2-1-1,1 0 0,-4-17 0,2 25-18,1 0 0,0 1-1,-1-1 1,1 0 0,-1 1-1,0-1 1,0 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1 1-1,0-1 1,0 0 0,0 1-1,-1 0 1,1-1 0,0 1-1,-1 1 1,0-1 0,1 0-1,-1 1 1,0 0 0,0 0-1,0 0 1,-7-1 0,0 1-23,-1-1 1,1 1-1,0 1 0,-1 0 1,1 1-1,-1 0 0,1 0 1,-16 5-1,4 3-1,1 1-1,-1 1 1,2 1-1,0 1 1,0 1 0,1 0-1,1 2 1,0 0-1,2 1 1,0 1-1,0 1 1,2 0-1,-23 37 1,33-46 21,0 0-1,0 0 1,1 1 0,0 0 0,1-1-1,0 1 1,1 0 0,0 1-1,0-1 1,1 0 0,1 1 0,0-1-1,2 13 1,-2-21 6,1 0 0,-1 0-1,1 1 1,0-1 0,0 0 0,0 0 0,0 0-1,1 0 1,-1-1 0,1 1 0,-1 0 0,1-1-1,0 1 1,0-1 0,0 1 0,1-1-1,2 2 1,0 0 0,0-1-1,0 0 0,0 0 0,1 0 1,-1-1-1,1 0 0,0 0 0,8 2 1,10-1 0,-1 0 1,1-2 0,37-2 0,-56 1 1,4-1 37,0-1 0,0 0-1,0 0 1,0-1 0,0 0 0,-1 0 0,1-1 0,-1-1 0,0 1 0,0-1 0,-1 0 0,1-1 0,-1 0 0,7-8 0,-6 7-171,-1-1-1,-1 1 1,0-2 0,0 1-1,0-1 1,-1 1-1,4-12 1,-6 14-407,-1 0-1,0 0 1,-1 0 0,1 0-1,-1 0 1,0-13 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5049.77">203 781 8900,'0'0'13844,"0"-9"-12860,1-9-839,0 2 1195,-8 37-773,-5 18-529,2 0 0,2 1-1,2 1 1,-2 58 0,8-46 30,0-30-2742,8-28-5882</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="5570.94">523 829 10117,'0'0'11800,"13"-11"-11072,43-33-184,-51 41-461,0 1-1,0-1 0,1 1 1,-1 0-1,0 1 1,1-1-1,0 1 0,-1 0 1,1 0-1,-1 1 1,1-1-1,0 1 0,-1 1 1,1-1-1,0 1 1,9 2-1,-14-2-85,1 1 0,-1-1-1,0 1 1,0-1 0,1 1 0,-1-1 0,0 1 0,0-1-1,-1 1 1,1 0 0,0 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,0 1 0,-1 3 0,-7 47 39,1-37-2,-1 0 0,0 0-1,-2 0 1,1-1 0,-2 0 0,-19 19 0,-18 27 36,47-59-66,0 0 0,0-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 0,-1 1 0,1-1 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,0 0 1,0 1-1,0-1 0,1 1 0,0-1 16,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,1 0 1,-1-1-1,0 1 0,0 0 0,1 0 0,60-19 417,-51 15-408,-7 4-22,-1-1 0,0 0 0,0 0-1,0 0 1,0 0 0,0-1 0,0 1 0,0-1 0,0 0-1,-1 1 1,1-1 0,4-5 0,-29 2-3156,10 3-4614,1 0-4256</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6104.68">987 812 11093,'0'0'11317,"1"-9"-10362,2-28-298,-3 35-615,1 1-1,-1 0 1,0-1 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1-1 0,1 1 0,0 0 0,0 0-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 1-1,1-1 1,-1 1 0,2-1 0,34-2-58,-30 3 59,-6 1-48,0 0 0,0 0 1,0-1-1,-1 1 0,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,0 1 1,0-1-1,1 0 0,-1 0 1,0 0-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,-1 1 0,-1 35 25,2-36-18,-1 4-2,0 1 1,-1 0 0,0 0-1,-1-1 1,1 1 0,-1-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,-7 6 0,5-5-123,0 0-1,0 1 1,1 0 0,-7 13 0,10-19 28,1 0 1,-1 1-1,1-1 1,0 0-1,0 0 1,-1 1 0,1-1-1,0 0 1,0 0-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 1 1,0-1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,0-1-1,1 2 1,0-1 78,-1 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 0,-1-1 1,0 1-1,1 3 0,-1-4 39,0 1 0,0-1 0,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 1,1-1-1,-1 1 0,1-1 0,0 0 0,-3 1 0,-52 2 388,45-3-642,10-6-4666,1-4-643</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6719.51">1406 819 9925,'0'0'12611,"0"13"-10157,0 43-2347,1-54-108,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 0 0,2 0 0,-2 1-11,0-1 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0-1,0 0 1,0 0 0,0-1 0,0 1-1,-1-1 1,1 0 0,0 1 0,0-1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0-1 0,1 1-1,-1 0 1,0-1 0,0 1 0,0-1 0,1-1-1,-1-4 14,1 1-1,-1-1 0,-1 1 1,1-1-1,-2-9 0,1 5 62,0 10-54,-5 37-178,-76 216 290,77-243-231,1 1-886,2-3-4875</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7293.32">1971 839 9204,'0'0'10538,"-4"-5"-9785,2 3-696,-1-1 0,1 1 1,-1 0-1,0 0 1,1 1-1,-1-1 0,0 0 1,0 1-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,-1 1 0,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,-1 0 1,1 1-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 1 1,0 0-1,-4 3 0,5-4-41,0 1-1,0-1 1,0 1 0,1 0-1,-1-1 1,0 1 0,1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 1 1,0-1-1,1 0 1,-1 0 0,0 1-1,1-1 1,0 0 0,0 1-1,-1-1 1,1 1-1,1-1 1,-1 0 0,0 1-1,1-1 1,-1 0-1,1 1 1,-1-1 0,1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,1 0-1,-1 0 1,1 0 0,1 1-1,8 8 16,0-1-1,0-1 1,1 0 0,1 0-1,16 8 1,23 17 25,-51-33-60,0 0 1,1 0-1,-1 1 1,0-1 0,0 0-1,0 0 1,0 1 0,0-1-1,0 1 1,0-1-1,0 1 1,0-1 0,-1 1-1,1 0 1,-1-1 0,1 1-1,-1 0 1,1-1-1,-1 1 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,-1-1 0,1 3-1,-2-1 7,1-1 1,-1 1-1,1-1 0,-1 1 0,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1-1 0,-5 3 0,-10 4 61,1-1 0,-1-1-1,-29 7 1,45-13-61,-12 3-235,-1 0-1,1-1 0,-21 2 0,34-5 88,-1 1-1,1-1 1,0 1-1,-1 0 1,1-1-1,-1 1 1,1-1-1,0 1 0,0-1 1,-1 1-1,1-1 1,0 1-1,0-1 1,0 1-1,-1-1 1,1 1-1,0-1 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,1-1 1,-1 1-1,0-1 1,0 1-1,0-1 1,1 1-1,-1-1 1,1 0-1,7-22-3451,8-5-1451,7-4-311</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7514.12">1951 836 10053,'0'0'11319,"11"-14"-10150,-4 12-1106,-1 0 0,1 1 1,0 0-1,0 0 0,1 0 0,-1 1 1,0 0-1,0 0 0,10 2 0,7 0 108,65-2 350,-50 0-9449</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8083">2682 825 9748,'0'0'8183,"-16"-10"-7244,13 9-879,-1 0 1,0 1-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 1,0 1-1,1 0 0,-1-1 1,0 1-1,1 1 1,-1-1-1,0 0 1,1 1-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 0,-4 5 1,-5 3 213,1 0-1,0 1 1,-17 23 0,22-25-228,0 0-1,0 1 1,1-1-1,0 1 1,1 0-1,0 0 1,1 0-1,0 1 1,1-1 0,0 1-1,0 0 1,1-1-1,1 19 1,0-26-36,1 0 1,-1 0-1,1-1 1,0 1-1,0 0 1,0-1-1,0 1 1,0-1-1,1 0 1,-1 1-1,1-1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0-1 1,0 1-1,1-1 1,-1 0-1,1 0 1,-1 1-1,1-2 1,0 1-1,-1 0 1,6 0-1,0 1-24,0 0-1,0-1 0,0 0 0,0-1 1,0 1-1,0-2 0,1 1 1,-1-1-1,9-2 0,-16 3 22,1-1 1,-1 1-1,0-1 0,1 1 0,-1-1 0,0 0 1,0 1-1,0-1 0,0 0 0,0 0 0,1 0 1,-1 0-1,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 1,-1 1-1,0 0 0,1-1 0,-1 1 0,0 0 1,0-1-1,0 1 0,0-1 0,0 1 0,0 0 1,0-1-1,-1-1 0,1 1 9,-1 0 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,-4 0 0,-7 0 17,0 1 1,0 0-1,0 1 0,0 0 1,0 1-1,-19 5 0,27-6-174,0 0-1,-1 1 0,1-1 1,0 1-1,0 0 0,0 0 0,0 1 1,0-1-1,0 1 0,0 0 1,1 0-1,0 0 0,-1 0 0,1 1 1,1-1-1,-1 1 0,0 0 1,1 0-1,0 0 0,-3 6 1,4 1-3685,1-3-2567</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -17905,7 +18505,7 @@
           <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
         </inkml:channelProperties>
       </inkml:inkSource>
-      <inkml:timestamp xml:id="ts0" timeString="2025-05-18T15:02:45.016"/>
+      <inkml:timestamp xml:id="ts0" timeString="2025-05-24T12:54:17.408"/>
     </inkml:context>
     <inkml:brush xml:id="br0">
       <inkml:brushProperty name="width" value="0.035" units="cm"/>
@@ -17913,12 +18513,7 @@
       <inkml:brushProperty name="color" value="#004F8B"/>
     </inkml:brush>
   </inkml:definitions>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0">107 103 4786,'0'-3'16502,"0"-1"-13003,-1 12-3493,-1-1 0,0 0 1,0 0-1,0 0 0,-1 0 0,-7 13 0,-4 12 37,-47 117 133,57-143-156,-2 14 75,6-19 51,9-11-9494,4 0-51</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="979.13">584 95 2353,'0'0'14866,"-3"-40"-10809,4 38-3986,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 1,0 0-1,4-2 0,36-14 176,-36 15-239,0 0 1,0 0-1,0 1 1,0 0-1,12-1 1,-17 4-17,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0-1,0 1 1,-1 1 0,1 0 3,0 1 10,-1 1 0,0 0 0,0 0 0,0 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,-1 0 0,1 0 0,-7 6 0,-1 1 8,-1-1 1,0 0-1,-1-1 0,-14 9 1,26-18-14,0-1-1,0 0 1,0 1 0,0-1 0,0 1-1,1 0 1,-1-1 0,0 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0 0,1 0-1,-1 0 1,1 2 0,0-3 5,1 1 0,-1 0 0,1-1 1,-1 1-1,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 0 0,0 1 0,-1-1 1,1 0-1,0 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 1,1 0-1,59 0 316,-49 0-254,17-2 1476,-15 0-3426,-7 2-2545,0 0-3388</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1738.4">1031 114 11445,'0'0'7876,"1"-34"-4461,7 30-3414,-1 0 1,0 1-1,1-1 0,-1 1 1,1 1-1,0 0 1,0 0-1,0 0 1,0 1-1,0 0 1,1 0-1,9 2 0,-23 26-169,2-21 188,-2 1-1,1-1 1,-1 0-1,0 0 0,0 0 1,0-1-1,-1 0 0,-12 9 1,11-10-24,1 1-1,0 0 1,0 1-1,0-1 1,1 1 0,0 0-1,0 0 1,1 1-1,-5 7 1,11-12-86,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 1,0 1-1,0 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,4 1 0,18 10-291,-23-12 374,0 1 1,0-1-1,0 1 1,-1 0-1,1-1 1,0 1-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,-1-1-1,1 1 1,-1 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,1-1-1,-1 1 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 2-1,-2-2 17,1 1 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 0,0 0 0,-3 0 0,-61 11 862,61-11-1108,-30-2 1289,24-6-2403,14-9-3685,6 6-274</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2656.47">1279 106 7267,'0'0'8964,"10"-26"-3249,-9 26-5695,-1-1 0,0 1 0,1 0 0,-1-1 0,0 1 0,1 0 1,-1 0-1,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1 0 1,0 0-1,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 1,0 0-1,1 1 0,-1-1 0,0 0 0,0 1 0,1-1 0,1 23 97,-2-21-114,0 66 280,1-67-279,-1-1-1,1 1 1,0-1 0,-1 0-1,1 1 1,0-1-1,-1 0 1,1 1 0,0-1-1,0 0 1,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1-1-1,1 1 1,0 0 0,-1 0-1,1-1 1,1 0 0,23-8-33,-21 7 10,-1 0-1,1 0 1,-1-1-1,1 1 1,-1-1 0,0 0-1,0 0 1,0 0-1,-1-1 1,1 1-1,-1 0 1,0-1-1,1 0 1,-2 0-1,1 1 1,2-7 0,-4 9 35,-1 36-347,-5-12 489,-1 0 0,0-1 0,-21 39 0,28-55 560,1-3-2629</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3084.09">1688 95 10261,'0'0'7790,"-5"0"-7515,3 0-224,-1 0 1,1 0-1,-1 1 1,1-1-1,0 0 0,0 1 1,-1 0-1,1-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,1 1 0,-1 0 1,0-1-1,1 1 1,0 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,1 0-1,-1 1 0,1-1 1,-1 0-1,1 0 1,0 1-1,0-1 1,0 3-1,0-2-37,1 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1-1 0,-1 1-1,1 0 1,0-1 0,0 1 0,0-1 0,0 1-1,0-1 1,5 4 0,-4-3 0,1 1 0,-1-1 0,1 1 0,-1 0 0,0 0 0,-1 1 0,3 4 0,-5-8 25,0 1-1,0-1 1,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0-1,0-1 1,0 1 0,0-1 0,0 1 0,0-1 0,-1 1 0,1-1-1,0 0 1,0 1 0,0-1 0,-3 0 0,-23 5-1301,10-7-5692</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3341.47">1695 104 10773,'0'0'10183,"6"-3"-9759,26-9-307,0 1 0,53-9 0,-50 13-5772,-59 14-3026</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">529 109 7059,'0'0'4866,"2"-7"-4492,-1 5-211,0-4 189,1 1 0,0 0 0,0 0 1,1-1-1,-1 1 0,7-8 0,-9 13-276,1-1 0,-1 1 0,0 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,-15-7 416,-19 2-904,34 5 496,-68-8-120,48 4 19,1 1 0,0 1 0,-1 1 0,0 1 0,-36 5 0,42-2 18,1 1 1,0 0 0,-1 1-1,2 1 1,-1 0 0,1 1 0,0 0-1,0 1 1,1 0 0,0 1-1,0 0 1,1 1 0,-17 20 0,18-12-21,0 1 1,2 1 0,0-1 0,1 1 0,-6 33 0,-4 13 36,8-40-16,1 0 0,1 0 0,2 0-1,1 0 1,0 1 0,2 32 0,3-53-1,-1 1 0,1 0 0,1-1-1,-1 1 1,1-1 0,0 0 0,0 0 0,1 0 0,0 0-1,0-1 1,0 1 0,1-1 0,-1 0 0,1 0 0,0-1-1,12 8 1,-5-3 3,1-1 0,0 0-1,1-1 1,0-1 0,0 0-1,24 7 1,-9-8 30,0-2 0,1 0 0,-1-2 1,38-3-1,-35 1-34,-16 1 3,-1-1 0,0-1 0,1 0-1,-1-1 1,0-1 0,-1 0 0,1-1 0,-1 0 0,0-2 0,0 1 0,-1-2 0,1 1-1,-2-2 1,1 0 0,-1-1 0,-1 0 0,1 0 0,-2-1 0,0-1 0,0 0-1,-1 0 1,0-1 0,-1 0 0,11-26 0,-9 14-1,-2 0 1,0 0-1,-2-1 0,-1 0 0,3-36 1,-3-136 48,-5 145-28,0 50-32,0 0 0,0-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,1 1 0,-1 1 0,1-1 0,-3 3 0,-33 34-3692,18-20-1989</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -18354,7 +18949,7 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="9" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -18364,7 +18959,7 @@
     </row>
     <row r="4" spans="2:7" ht="14.25" customHeight="1">
       <c r="B4" s="11" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -18599,7 +19194,7 @@
         <v>192</v>
       </c>
       <c r="C53" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="54" spans="2:3">
@@ -18656,7 +19251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEDA74AC-C52D-4467-9D08-FCE1AD0029BD}">
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -18671,25 +19266,25 @@
   <sheetData>
     <row r="2" spans="2:9">
       <c r="B2" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D2" s="2">
         <f ca="1">TODAY()</f>
-        <v>45795</v>
+        <v>45801</v>
       </c>
     </row>
     <row r="3" spans="2:9">
       <c r="B3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="D3" s="10">
         <f ca="1">NOW()</f>
-        <v>45795.91765127315</v>
+        <v>45801.783003935183</v>
       </c>
     </row>
     <row r="4" spans="2:9">
       <c r="B4" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D4">
         <f ca="1">YEAR(D3)</f>
@@ -18701,7 +19296,7 @@
     </row>
     <row r="5" spans="2:9">
       <c r="B5" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D5">
         <f ca="1">MONTH(D3)</f>
@@ -18718,60 +19313,60 @@
     </row>
     <row r="6" spans="2:9">
       <c r="B6" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D6">
         <f ca="1">DAY(D3)</f>
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E6" t="str">
         <f ca="1">TEXT(D3,"ddd")</f>
-        <v>Sun</v>
+        <v>Sat</v>
       </c>
       <c r="F6" t="str">
         <f ca="1">TEXT(D3,"dddd")</f>
-        <v>Sunday</v>
+        <v>Saturday</v>
       </c>
     </row>
     <row r="7" spans="2:9">
       <c r="B7" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="D7">
         <f ca="1">HOUR(D3)</f>
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D8">
         <f ca="1">MINUTE(D3)</f>
-        <v>1</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="D9">
         <f ca="1">SECOND(D3)</f>
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="2:9">
       <c r="B10" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="D10">
         <f ca="1">WEEKDAY(D3,1)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:9">
       <c r="B11" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D11">
         <f ca="1">WEEKNUM(D3)</f>
@@ -18787,7 +19382,7 @@
         <v>46022</v>
       </c>
       <c r="F12" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G12">
         <v>12</v>
@@ -18833,10 +19428,10 @@
     </row>
     <row r="17" spans="2:5">
       <c r="B17" t="s">
+        <v>893</v>
+      </c>
+      <c r="D17" t="s">
         <v>894</v>
-      </c>
-      <c r="D17" t="s">
-        <v>895</v>
       </c>
       <c r="E17">
         <f>YEARFRAC(E14,F14,3)</f>
@@ -18845,7 +19440,7 @@
     </row>
     <row r="18" spans="2:5">
       <c r="B18" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E18" s="2">
         <f>EDATE(E14,3)</f>
@@ -18854,7 +19449,7 @@
     </row>
     <row r="19" spans="2:5">
       <c r="B19" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E19" s="2">
         <f>EOMONTH(E14,3)</f>
@@ -18870,10 +19465,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B71C03-7B12-4842-AAB8-D655859B4B5C}">
-  <dimension ref="B2:G14"/>
+  <dimension ref="B2:G49"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B13"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -18884,23 +19479,21 @@
     <col min="4" max="4" width="9.46484375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.19921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C2" t="s">
+        <v>853</v>
+      </c>
+      <c r="D2" t="s">
         <v>854</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>855</v>
-      </c>
-      <c r="E2" t="s">
-        <v>856</v>
-      </c>
-      <c r="G2" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="3" spans="2:7">
@@ -18915,8 +19508,13 @@
         <f>PROPER(MID(B3,FIND(".",B3)+1,FIND("@",B3)-FIND(".",B3)-1))</f>
         <v>Ahmad</v>
       </c>
-      <c r="G3" t="s">
-        <v>846</v>
+      <c r="F3" t="str">
+        <f>PROPER(MID(B3,FIND("@",B3)+1,FIND(".com",B3)-FIND("@",B3)-1))</f>
+        <v>Acciojob</v>
+      </c>
+      <c r="G3">
+        <f>FIND(".com",B3)</f>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:7">
@@ -18931,8 +19529,13 @@
         <f t="shared" ref="D4:D13" si="1">PROPER(MID(B4,FIND(".",B4)+1,FIND("@",B4)-FIND(".",B4)-1))</f>
         <v>Vaidwan</v>
       </c>
-      <c r="G4" t="s">
-        <v>847</v>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F13" si="2">PROPER(MID(B4,FIND("@",B4)+1,FIND(".com",B4)-FIND("@",B4)-1))</f>
+        <v>Tcs</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G13" si="3">FIND(".com",B4)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:7">
@@ -18947,8 +19550,13 @@
         <f t="shared" si="1"/>
         <v>M</v>
       </c>
-      <c r="G5" t="s">
-        <v>849</v>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>Nestle</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -18963,8 +19571,13 @@
         <f t="shared" si="1"/>
         <v>Anuj</v>
       </c>
-      <c r="G6" t="s">
-        <v>848</v>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>Google</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="3"/>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="2:7">
@@ -18979,6 +19592,14 @@
         <f t="shared" si="1"/>
         <v>Rahman</v>
       </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>Aramco</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="7" t="s">
@@ -18992,6 +19613,14 @@
         <f t="shared" si="1"/>
         <v>Verma</v>
       </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>Tcs</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="7" t="s">
@@ -19005,10 +19634,18 @@
         <f t="shared" si="1"/>
         <v>Vishnoi</v>
       </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>Genpact</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -19018,6 +19655,14 @@
         <f t="shared" si="1"/>
         <v>Ak</v>
       </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>Pg</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="7" t="s">
@@ -19031,6 +19676,14 @@
         <f t="shared" si="1"/>
         <v>Soabhagya</v>
       </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>Ahead</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="7" t="s">
@@ -19044,10 +19697,18 @@
         <f t="shared" si="1"/>
         <v>Kumar</v>
       </c>
+      <c r="F12" t="str">
+        <f t="shared" si="2"/>
+        <v>Ecl</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="2:7">
       <c r="B13" s="7" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -19057,11 +19718,102 @@
         <f t="shared" si="1"/>
         <v>Afsar</v>
       </c>
+      <c r="F13" t="str">
+        <f t="shared" si="2"/>
+        <v>Gmail</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="2:7">
       <c r="B14" s="7"/>
     </row>
+    <row r="35" spans="3:7" s="12" customFormat="1"/>
+    <row r="37" spans="3:7">
+      <c r="C37" s="12"/>
+      <c r="D37" s="13" t="str">
+        <f>IF(1=1,"",1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="3:7">
+      <c r="C38" t="b">
+        <f>ISBLANK(C37)</f>
+        <v>1</v>
+      </c>
+      <c r="D38" t="b">
+        <f>ISBLANK(D37)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7">
+      <c r="C39">
+        <f>COUNTA(C37)</f>
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <f>COUNTA(D37)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7">
+      <c r="C40">
+        <f>COUNTBLANK(C37)</f>
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <f>COUNTBLANK(D37)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" ht="14.25" customHeight="1">
+      <c r="C42" s="15" t="s">
+        <v>896</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
+    </row>
+    <row r="43" spans="3:7">
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+    </row>
+    <row r="45" spans="3:7">
+      <c r="C45" t="s">
+        <v>897</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7">
+      <c r="C47" s="14" t="s">
+        <v>899</v>
+      </c>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" t="s">
+        <v>900</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C42:G43"/>
+    <mergeCell ref="C47:G47"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{42BB3EAB-2A7F-43CC-9AEE-124D32724445}"/>
     <hyperlink ref="B4" r:id="rId2" xr:uid="{B7A155DF-B4FB-4D1C-AB84-F1095316D381}"/>
@@ -48244,31 +48996,31 @@
     </row>
     <row r="2" spans="2:14">
       <c r="B2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C2" t="s">
+        <v>857</v>
+      </c>
+      <c r="D2" t="s">
         <v>858</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>858</v>
+      </c>
+      <c r="F2" t="s">
         <v>859</v>
       </c>
-      <c r="E2" t="s">
-        <v>859</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>860</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>861</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>860</v>
+      </c>
+      <c r="J2" t="s">
         <v>862</v>
-      </c>
-      <c r="I2" t="s">
-        <v>861</v>
-      </c>
-      <c r="J2" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="3" spans="2:14">
@@ -48284,16 +49036,16 @@
     </row>
     <row r="4" spans="2:14">
       <c r="B4" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D4" t="s">
+        <v>857</v>
+      </c>
+      <c r="E4" t="s">
         <v>858</v>
       </c>
-      <c r="E4" t="s">
-        <v>859</v>
-      </c>
       <c r="F4" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="L4" t="str">
         <f>LEFT(B2,3)</f>
@@ -48324,16 +49076,16 @@
     </row>
     <row r="6" spans="2:14">
       <c r="B6" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="D6" t="s">
+        <v>861</v>
+      </c>
+      <c r="E6" t="s">
+        <v>860</v>
+      </c>
+      <c r="F6" t="s">
         <v>862</v>
-      </c>
-      <c r="E6" t="s">
-        <v>861</v>
-      </c>
-      <c r="F6" t="s">
-        <v>863</v>
       </c>
       <c r="L6" t="str">
         <f>LEFT(B2,100)</f>
@@ -48350,15 +49102,15 @@
     </row>
     <row r="8" spans="2:14">
       <c r="B8" t="s">
+        <v>874</v>
+      </c>
+      <c r="D8" t="s">
         <v>875</v>
-      </c>
-      <c r="D8" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="10" spans="2:14">
       <c r="B10" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="L10" t="str">
         <f>LEFT(B10,10)</f>
@@ -48402,7 +49154,7 @@
     </row>
     <row r="17" spans="2:13">
       <c r="B17" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C17">
         <f>LEN(B2)</f>
@@ -48419,12 +49171,12 @@
     </row>
     <row r="18" spans="2:13">
       <c r="B18" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="7" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="D20">
         <f>LEN(B20)</f>
@@ -48433,7 +49185,7 @@
     </row>
     <row r="24" spans="2:13">
       <c r="B24" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="E24" t="str">
         <f>LEFT(B24,5)</f>
@@ -48453,7 +49205,7 @@
     </row>
     <row r="25" spans="2:13">
       <c r="B25" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="E25" t="str">
         <f>LEFT(B25,3)</f>
@@ -48473,7 +49225,7 @@
     </row>
     <row r="26" spans="2:13">
       <c r="B26" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="F26">
         <v>7</v>
@@ -48489,7 +49241,7 @@
     </row>
     <row r="27" spans="2:13">
       <c r="B27" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="F27">
         <v>5</v>
@@ -48505,7 +49257,7 @@
     </row>
     <row r="28" spans="2:13">
       <c r="B28" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -48521,20 +49273,20 @@
     </row>
     <row r="31" spans="2:13">
       <c r="B31" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="K31" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="32" spans="2:13">
       <c r="B32" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E34" t="str">
         <f>SUBSTITUTE(B34,"a","A")</f>
@@ -48640,7 +49392,7 @@
     </row>
     <row r="45" spans="2:11">
       <c r="B45" s="7" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="2"/>
@@ -48679,7 +49431,7 @@
     </row>
     <row r="48" spans="2:11">
       <c r="B48" s="7" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="2"/>
@@ -48692,7 +49444,7 @@
     </row>
     <row r="54" spans="2:5">
       <c r="B54" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E54" t="str">
         <f>REPLACE(B54,2,5,"*")</f>

</xml_diff>